<commit_message>
finished most of overhead costs
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c2c6e3652e668e7/Work/Projects/dogen/Finances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{62DE8BDC-26E7-4C6E-8182-96466A9BEAC6}"/>
+  <xr:revisionPtr revIDLastSave="583" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1F3DE9B9-B60F-4707-AE9A-C18EBCFD3DE4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overhead" sheetId="2" r:id="rId1"/>
-    <sheet name="Comprehensive" sheetId="3" r:id="rId2"/>
-    <sheet name="Scaling" sheetId="4" r:id="rId3"/>
-    <sheet name="employee_expenses" sheetId="10" r:id="rId4"/>
-    <sheet name="Insurances" sheetId="5" r:id="rId5"/>
-    <sheet name="Liabilities" sheetId="6" r:id="rId6"/>
-    <sheet name="Gaming" sheetId="7" r:id="rId7"/>
-    <sheet name="Dance_Studio" sheetId="8" r:id="rId8"/>
-    <sheet name="Kitchen" sheetId="9" r:id="rId9"/>
-    <sheet name="paperwork" sheetId="12" r:id="rId10"/>
+    <sheet name="Operating_Costs" sheetId="4" r:id="rId2"/>
+    <sheet name="Comprehensive" sheetId="3" r:id="rId3"/>
+    <sheet name="Projection" sheetId="14" r:id="rId4"/>
+    <sheet name="employee_expenses" sheetId="10" r:id="rId5"/>
+    <sheet name="Gaming" sheetId="7" r:id="rId6"/>
+    <sheet name="Dance_Studio" sheetId="8" r:id="rId7"/>
+    <sheet name="Kitchen" sheetId="9" r:id="rId8"/>
+    <sheet name="Liabilities" sheetId="12" r:id="rId9"/>
+    <sheet name="Eating Area" sheetId="13" r:id="rId10"/>
     <sheet name="decor" sheetId="11" r:id="rId11"/>
     <sheet name="Initial" sheetId="1" r:id="rId12"/>
   </sheets>
@@ -34,7 +34,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
   <si>
     <t>Overhead</t>
   </si>
@@ -257,19 +259,91 @@
     <t>kitchen shelves</t>
   </si>
   <si>
-    <t>paint</t>
-  </si>
-  <si>
     <t>decorations</t>
   </si>
   <si>
-    <t>liabaility waiver for the kitchen</t>
-  </si>
-  <si>
     <t>stainless steel cookware</t>
   </si>
   <si>
     <t>knives</t>
+  </si>
+  <si>
+    <t>allergy form</t>
+  </si>
+  <si>
+    <t>liabaility waiver for the kitchen use</t>
+  </si>
+  <si>
+    <t>sq feet per 1 gal. can</t>
+  </si>
+  <si>
+    <t>paint per 1 gal</t>
+  </si>
+  <si>
+    <t>sq feet (3 walls and half of fourth)</t>
+  </si>
+  <si>
+    <t>One normal wall sq feet</t>
+  </si>
+  <si>
+    <t>paint cans per wall</t>
+  </si>
+  <si>
+    <t>Number of walls</t>
+  </si>
+  <si>
+    <t>Length (ft)</t>
+  </si>
+  <si>
+    <t>height (ft)</t>
+  </si>
+  <si>
+    <t>Paint cans needed</t>
+  </si>
+  <si>
+    <t>gaming</t>
+  </si>
+  <si>
+    <t>dancing</t>
+  </si>
+  <si>
+    <t>cooking</t>
+  </si>
+  <si>
+    <t>liability forms</t>
+  </si>
+  <si>
+    <t>Likely scenario</t>
+  </si>
+  <si>
+    <t>cleaning supplies</t>
+  </si>
+  <si>
+    <t>Total Equipment Costs</t>
+  </si>
+  <si>
+    <t>décor</t>
+  </si>
+  <si>
+    <t>chairs</t>
+  </si>
+  <si>
+    <t>8 seater tables</t>
+  </si>
+  <si>
+    <t>4 seater tables</t>
+  </si>
+  <si>
+    <t>2 seater tables</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>People per</t>
+  </si>
+  <si>
+    <t>eating area</t>
   </si>
 </sst>
 </file>
@@ -643,29 +717,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAC8DE-41B9-46A0-BE44-EAAB92E58FB4}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="7">
+        <f>Gaming!D11</f>
+        <v>16930</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="7">
+        <f>Dance_Studio!D5</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="7">
+        <f>Kitchen!G17</f>
+        <v>12865</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="7">
+        <f>Liabilities!B7</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="7">
+        <f>decor!K7</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="7">
+        <f>'Eating Area'!E10</f>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="7">
+        <f>SUM(B3:B8)</f>
+        <v>38295</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36F18DE-64EC-418D-B15A-DB7866B424E3}">
-  <dimension ref="A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725D3AE5-3953-4739-93F6-EFB9BCC1B4E0}">
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>73</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3">
+        <f>SUM(C4:C6)</f>
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <f>D3*B3</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>400</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E6" si="0">D4*B4</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUM(E3:E6)</f>
+        <v>2550</v>
       </c>
     </row>
   </sheetData>
@@ -675,25 +915,121 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A6F31-02C3-4DB3-8520-6CC51B52F01A}">
-  <dimension ref="A2:A3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <f>D2*G2</f>
+        <v>3500</v>
+      </c>
+      <c r="D2">
+        <f>I2*H2</f>
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>350</v>
+      </c>
+      <c r="F2">
+        <f>D2/E2</f>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="G2">
+        <v>3.5</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <f>C2/E2</f>
+        <v>10</v>
+      </c>
+      <c r="K2" s="1">
+        <f>B2*J2</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>72</v>
+      <c r="K3" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K4" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="1">
+        <f>SUM(K2:K4)</f>
+        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -706,16 +1042,16 @@
   <dimension ref="A2:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -723,7 +1059,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -734,7 +1070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -745,7 +1081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -754,7 +1090,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -763,7 +1099,7 @@
         <v>8400</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -772,7 +1108,7 @@
         <v>107100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -780,7 +1116,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -791,7 +1127,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -799,7 +1135,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -807,7 +1143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -815,7 +1151,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -824,7 +1160,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -833,12 +1169,12 @@
         <v>175500</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -846,7 +1182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -854,12 +1190,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -867,12 +1203,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -880,7 +1216,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -888,7 +1224,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
@@ -897,7 +1233,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -905,7 +1241,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
@@ -913,7 +1249,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -922,7 +1258,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -931,7 +1267,7 @@
         <v>15750</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -940,7 +1276,7 @@
         <v>63000</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -949,7 +1285,7 @@
         <v>803250</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
@@ -958,7 +1294,7 @@
         <v>200812.5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -967,7 +1303,7 @@
         <v>602437.5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
@@ -982,70 +1318,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6542B2-EFD7-436F-B204-92A7E08F055C}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2">
-        <v>1769.23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>134.69999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>108.42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>25.35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>53.42</v>
       </c>
     </row>
   </sheetData>
@@ -1053,170 +1382,232 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A196D7-1B02-45CD-9C95-BE4237B2582D}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E8F79C-848E-45C7-B440-BCF016365DF9}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AE74F5-6EBD-4CE2-9D78-29A3C9723FF5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7">
+        <f>B2*C2</f>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D8" si="0">B3*C3</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1">
+        <v>110</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <f>C3</f>
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7">
+        <f>SUM(D2:D8)</f>
+        <v>16930</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E8F79C-848E-45C7-B440-BCF016365DF9}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6007EBCF-A6A9-4054-90A6-E709ADB7E2B5}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1500</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7">
-        <f>B2*C2</f>
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>900</v>
       </c>
       <c r="D3" s="7">
-        <f t="shared" ref="D3:D8" si="0">B3*C3</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <f>C3*B3</f>
+        <v>13500</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1">
-        <v>110</v>
+        <v>3</v>
       </c>
       <c r="C4">
+        <v>900</v>
+      </c>
+      <c r="D4" s="7">
+        <f>C4*B4</f>
+        <v>2700</v>
+      </c>
+      <c r="G4" s="6">
         <v>3</v>
       </c>
-      <c r="D4" s="7">
-        <f t="shared" si="0"/>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="1">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <f>C3</f>
-        <v>4</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="1">
-        <v>500</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="1">
-        <v>100</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="1">
-        <v>200</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="7">
-        <f>SUM(D2:D8)</f>
-        <v>19930</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1225,76 +1616,262 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6007EBCF-A6A9-4054-90A6-E709ADB7E2B5}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560605D-AE6F-456E-B5FE-7223BF3283FD}">
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
       <c r="G1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>5*5</f>
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>400</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7">
+        <f>(PRODUCT(B2:D2) +E2)*F2</f>
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="1">
+        <v>300</v>
+      </c>
+      <c r="C3">
+        <f>$F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="7">
+        <f>B3*C3</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="1">
-        <v>15</v>
-      </c>
-      <c r="C3">
+      <c r="C4">
+        <f>$F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:G14" si="0">B4*C4</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <f>$F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <f>$F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1">
+        <v>200</v>
+      </c>
+      <c r="C7">
+        <f>$F$2</f>
+        <v>3</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1">
+        <v>300</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1">
         <v>900</v>
       </c>
-      <c r="D3" s="7">
-        <f>C3*B3</f>
-        <v>13500</v>
-      </c>
-      <c r="G3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="C9">
+        <f>$F$2</f>
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>900</v>
-      </c>
-      <c r="D4" s="7">
-        <f>C4*B4</f>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
         <v>2700</v>
       </c>
-      <c r="G4" s="6">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1">
+        <v>250</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>53</v>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="1">
+        <v>80</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="7">
+        <f>SUM(G2:G14)</f>
+        <v>12865</v>
       </c>
     </row>
   </sheetData>
@@ -1303,262 +1880,46 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560605D-AE6F-456E-B5FE-7223BF3283FD}">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36F18DE-64EC-418D-B15A-DB7866B424E3}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1">
-        <v>35</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <f>5*5</f>
-        <v>25</v>
-      </c>
-      <c r="E2">
-        <v>400</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" s="7">
-        <f>(PRODUCT(B2:D2) +E2)*F2</f>
-        <v>3825</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1">
-        <v>300</v>
-      </c>
-      <c r="C3">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G3" s="7">
-        <f>B3*C3</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="1">
         <v>50</v>
       </c>
-      <c r="C4">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:G14" si="0">B4*C4</f>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="7">
+        <f>B2+B3</f>
         <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="1">
-        <v>500</v>
-      </c>
-      <c r="C5">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="1">
-        <v>100</v>
-      </c>
-      <c r="C6">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G6" s="7">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="1">
-        <v>200</v>
-      </c>
-      <c r="C7">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G7" s="7">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="1">
-        <v>300</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="1">
-        <v>900</v>
-      </c>
-      <c r="C9">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G9" s="7">
-        <f t="shared" si="0"/>
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="1">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="1">
-        <v>250</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="0"/>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="1">
-        <v>80</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="G14" s="7">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="7">
-        <f>SUM(G2:G14)</f>
-        <v>12865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added rent. Almost forgot it
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1569" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{FC8FE27B-59ED-4B36-AEA2-A8F82C53411A}"/>
+  <xr:revisionPtr revIDLastSave="1588" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8386D0D-0FE2-4ECA-9B90-00B30D3FFD23}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="237">
   <si>
     <t>Overhead</t>
   </si>
@@ -749,6 +749,12 @@
   </si>
   <si>
     <t>Diminishing returns</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>monthly rent estimate</t>
   </si>
 </sst>
 </file>
@@ -759,9 +765,9 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
-    <numFmt numFmtId="173" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -838,14 +844,14 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1166,9 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1187,7 +1191,7 @@
       </c>
       <c r="B4">
         <f>Net_And_Analysis!H5</f>
-        <v>182</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1248,7 +1252,7 @@
       <c r="B13" t="s">
         <v>208</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>209</v>
       </c>
     </row>
@@ -1264,7 +1268,7 @@
       <c r="A15" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>60592</v>
       </c>
     </row>
@@ -1272,7 +1276,7 @@
       <c r="A16" t="s">
         <v>213</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <v>58106</v>
       </c>
     </row>
@@ -1280,7 +1284,7 @@
       <c r="A17" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="15">
         <v>55391</v>
       </c>
     </row>
@@ -1288,7 +1292,7 @@
       <c r="A18" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="15">
         <f>SUM(B15:B17)</f>
         <v>174089</v>
       </c>
@@ -1297,7 +1301,7 @@
       <c r="A19" t="s">
         <v>215</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="15">
         <v>25000</v>
       </c>
     </row>
@@ -1310,7 +1314,7 @@
       <c r="A21" t="s">
         <v>216</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="16">
         <f>B18+B19</f>
         <v>199089</v>
       </c>
@@ -1319,7 +1323,7 @@
       <c r="A22" t="s">
         <v>217</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="15">
         <v>200000</v>
       </c>
     </row>
@@ -1327,16 +1331,16 @@
       <c r="A24" t="s">
         <v>219</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="18">
         <f>B4/B22</f>
-        <v>9.1E-4</v>
+        <v>1.2149999999999999E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>220</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="17">
         <f>B9/B22</f>
         <v>2E-3</v>
       </c>
@@ -2213,8 +2217,7 @@
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2287,8 +2290,8 @@
         <v>137</v>
       </c>
       <c r="B12" s="7">
-        <f>Operating_Costs!F12</f>
-        <v>189166.66666666666</v>
+        <f>Operating_Costs!F13</f>
+        <v>252166.66666666666</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2349,27 +2352,27 @@
       </c>
       <c r="B15" s="7">
         <f>$B$11+($B$12*B14)</f>
-        <v>133528.33333333331</v>
+        <v>165028.33333333331</v>
       </c>
       <c r="C15" s="7">
         <f t="shared" ref="C15:G15" si="1">$B$11+($B$12*C14)</f>
-        <v>117764.44444444444</v>
+        <v>144014.44444444444</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="1"/>
-        <v>102000.55555555555</v>
+        <v>123000.55555555555</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="1"/>
-        <v>86236.666666666657</v>
+        <v>101986.66666666666</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>70472.777777777781</v>
+        <v>80972.777777777781</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="1"/>
-        <v>54708.888888888891</v>
+        <v>59958.888888888891</v>
       </c>
       <c r="H15" s="7"/>
     </row>
@@ -2439,7 +2442,7 @@
   <dimension ref="A4:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2491,7 +2494,7 @@
       </c>
       <c r="H5" s="10">
         <f>Gross!I30</f>
-        <v>182</v>
+        <v>243</v>
       </c>
       <c r="I5">
         <f>Gross!J30</f>
@@ -2540,7 +2543,7 @@
       </c>
       <c r="H6" s="11">
         <f>Gross!I45</f>
-        <v>189280.00000000003</v>
+        <v>252720.00000000006</v>
       </c>
       <c r="I6" s="7">
         <f>Gross!J45</f>
@@ -2564,8 +2567,8 @@
         <v>182</v>
       </c>
       <c r="B8" s="7">
-        <f>Operating_Costs!F12</f>
-        <v>189166.66666666666</v>
+        <f>Operating_Costs!F13</f>
+        <v>252166.66666666666</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2574,47 +2577,47 @@
       </c>
       <c r="B10" s="7">
         <f>B6-$B$8</f>
-        <v>-183966.66666666666</v>
+        <v>-246966.66666666666</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:L10" si="0">C6-$B$8</f>
-        <v>-178766.66666666666</v>
+        <v>-241766.66666666666</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>-168366.66666666666</v>
+        <v>-231366.66666666666</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>-147566.66666666666</v>
+        <v>-210566.66666666666</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
-        <v>-105966.66666666664</v>
+        <v>-168966.66666666663</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>-22766.666666666628</v>
+        <v>-85766.666666666628</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>113.33333333337214</v>
+        <v>553.33333333340124</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="0"/>
-        <v>143633.3333333334</v>
+        <v>80633.333333333401</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="0"/>
-        <v>226833.33333333346</v>
+        <v>163833.33333333346</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="0"/>
-        <v>330833.33333333349</v>
+        <v>267833.33333333349</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="0"/>
-        <v>434833.33333333349</v>
+        <v>371833.33333333349</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2628,7 +2631,7 @@
       </c>
       <c r="B12">
         <f>H5</f>
-        <v>182</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2637,7 +2640,7 @@
       </c>
       <c r="B13">
         <f>Gross!I37</f>
-        <v>29.120000000000008</v>
+        <v>38.88000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2761,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7959888-B526-4FAC-9FC1-7A03020906F6}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2949,7 +2952,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
+      <c r="A20" s="19">
         <v>0.8</v>
       </c>
       <c r="B20">
@@ -2974,7 +2977,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="19"/>
       <c r="B21">
         <v>0.2</v>
       </c>
@@ -2997,7 +3000,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="19"/>
       <c r="B22">
         <v>0.8</v>
       </c>
@@ -3020,7 +3023,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="19"/>
       <c r="B23">
         <v>0.8</v>
       </c>
@@ -3057,7 +3060,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
+      <c r="A25" s="19">
         <v>0.2</v>
       </c>
       <c r="B25" s="8">
@@ -3078,7 +3081,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="8">
         <v>0.2</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>160</v>
       </c>
       <c r="I30">
-        <v>182</v>
+        <v>243</v>
       </c>
       <c r="J30">
         <v>320</v>
@@ -3188,7 +3191,7 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" ref="I31" si="3">$E20*$F20*$B31*I$30</f>
-        <v>465.92000000000007</v>
+        <v>622.08000000000015</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" ref="J31:M34" si="4">$E20*$F20*$B31*J$30</f>
@@ -3240,7 +3243,7 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" ref="I32" si="6">$E21*$F21*$B32*I$30</f>
-        <v>174.72000000000006</v>
+        <v>233.28000000000009</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="4"/>
@@ -3292,7 +3295,7 @@
       </c>
       <c r="I33" s="1">
         <f t="shared" ref="I33" si="7">$E22*$F22*$B33*I$30</f>
-        <v>1863.6800000000003</v>
+        <v>2488.3200000000006</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="4"/>
@@ -3344,7 +3347,7 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" ref="I34" si="8">$E23*$F23*$B34*I$30</f>
-        <v>931.84000000000015</v>
+        <v>1244.1600000000003</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="4"/>
@@ -3393,7 +3396,7 @@
       </c>
       <c r="I35" s="7">
         <f t="shared" si="9"/>
-        <v>3436.1600000000008</v>
+        <v>4587.8400000000011</v>
       </c>
       <c r="J35" s="7">
         <f>SUM(J31:J34)</f>
@@ -3442,7 +3445,7 @@
       </c>
       <c r="I36" s="3">
         <f t="shared" si="10"/>
-        <v>203.84000000000006</v>
+        <v>272.16000000000008</v>
       </c>
       <c r="J36" s="3">
         <f>J$30*($G$24)</f>
@@ -3491,7 +3494,7 @@
       </c>
       <c r="I37">
         <f t="shared" si="11"/>
-        <v>29.120000000000008</v>
+        <v>38.88000000000001</v>
       </c>
       <c r="J37">
         <f>J36/7</f>
@@ -3540,7 +3543,7 @@
       </c>
       <c r="I41" s="7">
         <f t="shared" si="12"/>
-        <v>171808.00000000003</v>
+        <v>229392.00000000006</v>
       </c>
       <c r="J41" s="7">
         <f t="shared" si="12"/>
@@ -3592,7 +3595,7 @@
       </c>
       <c r="I42" s="7">
         <f t="shared" si="13"/>
-        <v>1456</v>
+        <v>1944</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="13"/>
@@ -3641,7 +3644,7 @@
       </c>
       <c r="I43" s="7">
         <f t="shared" si="14"/>
-        <v>17472</v>
+        <v>23328</v>
       </c>
       <c r="J43" s="7">
         <f>J42*12</f>
@@ -3690,7 +3693,7 @@
       </c>
       <c r="I45" s="7">
         <f t="shared" si="15"/>
-        <v>189280.00000000003</v>
+        <v>252720.00000000006</v>
       </c>
       <c r="J45" s="7">
         <f t="shared" si="15"/>
@@ -3720,10 +3723,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
-  <dimension ref="A3:F14"/>
+  <dimension ref="A3:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3736,7 +3739,7 @@
     <col min="6" max="6" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>107</v>
       </c>
@@ -3753,7 +3756,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -3777,7 +3780,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -3801,7 +3804,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -3826,7 +3829,7 @@
         <v>2333.3333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -3851,7 +3854,7 @@
         <v>4666.666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -3876,7 +3879,7 @@
         <v>1166.6666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -3949,32 +3952,62 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="1">
+        <f>C12/7</f>
+        <v>714.28571428571433</v>
+      </c>
+      <c r="C12" s="1">
+        <f>F12/12</f>
+        <v>5000</v>
+      </c>
+      <c r="D12" s="1">
+        <f>C12*2</f>
+        <v>10000</v>
+      </c>
+      <c r="E12" s="1">
+        <f>D12*2</f>
+        <v>20000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>60000</v>
+      </c>
+      <c r="H12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="1">
-        <f>SUM(B4:B11)</f>
-        <v>531.90476190476193</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" ref="C12:E12" si="0">SUM(C4:C11)</f>
-        <v>3723.3333333333339</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="B13" s="1">
+        <f>SUM(B4:B12)</f>
+        <v>1246.1904761904761</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:F13" si="0">SUM(C4:C12)</f>
+        <v>8723.3333333333339</v>
+      </c>
+      <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>10177.435897435897</v>
-      </c>
-      <c r="E12" s="1">
+        <v>20177.435897435898</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>20354.871794871793</v>
-      </c>
-      <c r="F12" s="1">
-        <f>SUM(F4:F9)</f>
-        <v>189166.66666666666</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40354.871794871797</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>252166.66666666666</v>
+      </c>
+      <c r="H13" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
created powerpoint presentation slides. Now they just need some words
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1588" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8386D0D-0FE2-4ECA-9B90-00B30D3FFD23}"/>
+  <xr:revisionPtr revIDLastSave="1591" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB4EFF9F-0804-4F39-A9B0-9CED114612D1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="236">
   <si>
     <t>Overhead</t>
   </si>
@@ -697,9 +697,6 @@
     <t>True Total</t>
   </si>
   <si>
-    <t>Target demographic size in New Haven Country</t>
-  </si>
-  <si>
     <t>2017 data</t>
   </si>
   <si>
@@ -742,9 +739,6 @@
     <t>Month 4 -12</t>
   </si>
   <si>
-    <t>Attempt to reach target of 182 community members</t>
-  </si>
-  <si>
     <t>sub-sub-communities</t>
   </si>
   <si>
@@ -755,6 +749,9 @@
   </si>
   <si>
     <t>monthly rent estimate</t>
+  </si>
+  <si>
+    <t>Attempt to reach target of break-even community members</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1218,7 +1217,7 @@
         <v>350</v>
       </c>
       <c r="C8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1231,7 +1230,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B10">
         <v>450</v>
@@ -1239,7 +1238,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B11">
         <v>500</v>
@@ -1261,7 +1260,7 @@
         <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1321,7 +1320,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B22" s="15">
         <v>200000</v>
@@ -1329,7 +1328,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B24" s="18">
         <f>B4/B22</f>
@@ -1338,7 +1337,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B25" s="17">
         <f>B9/B22</f>
@@ -2210,7 +2209,7 @@
   <dimension ref="A3:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2378,26 +2377,26 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2405,7 +2404,7 @@
         <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2413,23 +2412,23 @@
         <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B25" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2939,7 +2938,7 @@
         <v>166</v>
       </c>
       <c r="D19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E19" t="s">
         <v>171</v>
@@ -3916,11 +3915,11 @@
         <v>20</v>
       </c>
       <c r="D10" s="1">
-        <f>C10*2</f>
+        <f t="shared" ref="D10:E12" si="0">C10*2</f>
         <v>40</v>
       </c>
       <c r="E10" s="1">
-        <f>D10*2</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="F10" s="1">
@@ -3941,11 +3940,11 @@
         <v>38.46153846153846</v>
       </c>
       <c r="D11" s="1">
-        <f>C11*2</f>
+        <f t="shared" si="0"/>
         <v>76.92307692307692</v>
       </c>
       <c r="E11" s="1">
-        <f>D11*2</f>
+        <f t="shared" si="0"/>
         <v>153.84615384615384</v>
       </c>
       <c r="F11" s="1">
@@ -3954,7 +3953,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B12" s="1">
         <f>C12/7</f>
@@ -3965,18 +3964,18 @@
         <v>5000</v>
       </c>
       <c r="D12" s="1">
-        <f>C12*2</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="E12" s="1">
-        <f>D12*2</f>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="F12" s="1">
         <v>60000</v>
       </c>
       <c r="H12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -3988,19 +3987,19 @@
         <v>1246.1904761904761</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:F13" si="0">SUM(C4:C12)</f>
+        <f t="shared" ref="C13:F13" si="1">SUM(C4:C12)</f>
         <v>8723.3333333333339</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20177.435897435898</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40354.871794871797</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252166.66666666666</v>
       </c>
       <c r="H13" s="6">

</xml_diff>

<commit_message>
found the real innovation
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1591" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB4EFF9F-0804-4F39-A9B0-9CED114612D1}"/>
+  <xr:revisionPtr revIDLastSave="1599" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{87713364-0840-449F-9515-BF9CDECD7660}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="235">
   <si>
     <t>Overhead</t>
   </si>
@@ -343,12 +343,6 @@
     <t>eating area</t>
   </si>
   <si>
-    <t>Cooking Instructor</t>
-  </si>
-  <si>
-    <t>Cooking Assistant</t>
-  </si>
-  <si>
     <t>Greeter/security</t>
   </si>
   <si>
@@ -752,6 +746,9 @@
   </si>
   <si>
     <t>Attempt to reach target of break-even community members</t>
+  </si>
+  <si>
+    <t>Business Management/Maintenance</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1181,12 +1178,12 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B4">
         <f>Net_And_Analysis!H5</f>
@@ -1195,7 +1192,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B6">
         <v>200</v>
@@ -1203,7 +1200,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B7">
         <v>300</v>
@@ -1211,18 +1208,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B8">
         <v>350</v>
       </c>
       <c r="C8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B9">
         <v>400</v>
@@ -1230,7 +1227,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B10">
         <v>450</v>
@@ -1238,7 +1235,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B11">
         <v>500</v>
@@ -1246,26 +1243,26 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="B13" t="s">
-        <v>208</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B15" s="15">
         <v>60592</v>
@@ -1273,7 +1270,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B16" s="15">
         <v>58106</v>
@@ -1281,7 +1278,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B17" s="15">
         <v>55391</v>
@@ -1298,7 +1295,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B19" s="15">
         <v>25000</v>
@@ -1306,12 +1303,12 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B21" s="16">
         <f>B18+B19</f>
@@ -1320,7 +1317,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B22" s="15">
         <v>200000</v>
@@ -1328,7 +1325,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B24" s="18">
         <f>B4/B22</f>
@@ -1337,7 +1334,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B25" s="17">
         <f>B9/B22</f>
@@ -1688,7 +1685,7 @@
         <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
         <v>66</v>
@@ -2286,7 +2283,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" s="7">
         <f>Operating_Costs!F13</f>
@@ -2295,7 +2292,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -2318,7 +2315,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14">
         <f>B13/12</f>
@@ -2347,7 +2344,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" s="7">
         <f>$B$11+($B$12*B14)</f>
@@ -2377,58 +2374,58 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2457,10 +2454,10 @@
   <sheetData>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H4" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2514,7 +2511,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" s="7">
         <f>Gross!C45</f>
@@ -2563,7 +2560,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B8" s="7">
         <f>Operating_Costs!F13</f>
@@ -2572,7 +2569,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B10" s="7">
         <f>B6-$B$8</f>
@@ -2621,12 +2618,12 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B12">
         <f>H5</f>
@@ -2635,7 +2632,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B13">
         <f>Gross!I37</f>
@@ -2644,24 +2641,24 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B16">
         <f>K5</f>
         <v>500</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B17">
         <f>B16*0.2</f>
@@ -2674,7 +2671,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B18">
         <f>B16-(0.2*710)</f>
@@ -2683,7 +2680,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B20">
         <f>Gross!L37</f>
@@ -2692,7 +2689,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B21" s="9">
         <v>0.5</v>
@@ -2700,19 +2697,19 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B22">
         <f>B20*(1+B21)</f>
         <v>120.00000000000003</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B24">
         <f>Gross!B7</f>
@@ -2721,7 +2718,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2729,7 +2726,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B26">
         <f>B24*B25</f>
@@ -2738,7 +2735,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B28">
         <f>B26-B22</f>
@@ -2747,7 +2744,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B29">
         <f>C17-B28</f>
@@ -2763,7 +2760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7959888-B526-4FAC-9FC1-7A03020906F6}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
@@ -2782,36 +2779,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3">
         <f>10</f>
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F3" s="9">
         <v>0.2</v>
@@ -2820,13 +2817,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F4" s="9">
         <v>0.8</v>
@@ -2834,7 +2831,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -2851,22 +2848,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" s="9">
         <v>0.2</v>
@@ -2877,7 +2874,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" s="1">
         <v>40</v>
@@ -2891,7 +2888,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B15" s="1">
         <v>20</v>
@@ -2929,25 +2926,25 @@
     <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" t="s">
         <v>170</v>
       </c>
-      <c r="B19" t="s">
-        <v>172</v>
-      </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2958,7 +2955,7 @@
         <v>0.2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D20" s="8">
         <v>0.8</v>
@@ -2981,7 +2978,7 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D21" s="8">
         <v>0.2</v>
@@ -3004,7 +3001,7 @@
         <v>0.8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D22" s="8">
         <v>0.8</v>
@@ -3027,7 +3024,7 @@
         <v>0.8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D23" s="8">
         <v>0.2</v>
@@ -3066,10 +3063,10 @@
         <v>0.8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E25" s="3">
         <f>$A$25*$B25</f>
@@ -3085,10 +3082,10 @@
         <v>0.2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E26" s="3">
         <f>$A$25*$B26</f>
@@ -3112,16 +3109,16 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -3159,7 +3156,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
@@ -3211,7 +3208,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B32" s="1">
         <v>10</v>
@@ -3263,7 +3260,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B33" s="1">
         <v>20</v>
@@ -3315,7 +3312,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B34" s="1">
         <v>20</v>
@@ -3367,7 +3364,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C35" s="7">
         <f>SUM(C31:C34)</f>
@@ -3416,7 +3413,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C36" s="3">
         <f>C$30*($G$24)</f>
@@ -3465,7 +3462,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C37">
         <f>C36/7</f>
@@ -3514,7 +3511,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C41" s="7">
         <f t="shared" ref="C41:M41" si="12">C35*50</f>
@@ -3563,7 +3560,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B42" s="1">
         <v>40</v>
@@ -3615,7 +3612,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C43" s="7">
         <f>C42*12</f>
@@ -3664,7 +3661,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C45" s="7">
         <f t="shared" ref="C45:M45" si="15">C43+C41</f>
@@ -3740,24 +3737,24 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1">
         <f>C4/7</f>
@@ -3769,11 +3766,11 @@
       </c>
       <c r="D4" s="1">
         <f>employees!B9</f>
-        <v>2884.6153846153848</v>
+        <v>1826.9230769230769</v>
       </c>
       <c r="E4" s="1">
         <f>D4*2</f>
-        <v>5769.2307692307695</v>
+        <v>3653.8461538461538</v>
       </c>
       <c r="F4" s="1">
         <v>4000</v>
@@ -3781,23 +3778,23 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1">
         <f>C5/7</f>
-        <v>412.08791208791212</v>
+        <v>260.98901098901098</v>
       </c>
       <c r="C5" s="1">
         <f>employees!B9</f>
-        <v>2884.6153846153848</v>
+        <v>1826.9230769230769</v>
       </c>
       <c r="D5" s="1">
         <f>employees!B10</f>
-        <v>5769.2307692307695</v>
+        <v>3653.8461538461538</v>
       </c>
       <c r="E5" s="1">
         <f>D5*2</f>
-        <v>11538.461538461539</v>
+        <v>7307.6923076923076</v>
       </c>
       <c r="F5" s="1">
         <v>150000</v>
@@ -3805,7 +3802,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" s="1">
         <f>200/30</f>
@@ -3830,7 +3827,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="1">
         <f>400/30</f>
@@ -3855,7 +3852,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" s="1">
         <f>100/30</f>
@@ -3880,7 +3877,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" s="1">
         <f>C9/7</f>
@@ -3905,7 +3902,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="1">
         <f>C10/7</f>
@@ -3929,7 +3926,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" s="1">
         <f>C11/7</f>
@@ -3953,7 +3950,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B12" s="1">
         <f>C12/7</f>
@@ -3975,7 +3972,7 @@
         <v>60000</v>
       </c>
       <c r="H12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -3984,19 +3981,19 @@
       </c>
       <c r="B13" s="1">
         <f>SUM(B4:B12)</f>
-        <v>1246.1904761904761</v>
+        <v>1095.0915750915751</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:F13" si="1">SUM(C4:C12)</f>
-        <v>8723.3333333333339</v>
+        <v>7665.6410256410254</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>20177.435897435898</v>
+        <v>17004.358974358976</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>40354.871794871797</v>
+        <v>34008.717948717953</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
@@ -4008,7 +4005,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -4020,9 +4017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72B0531-F9EA-4BB7-8657-7C884FA8D7D5}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4039,21 +4034,21 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>116</v>
-      </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -4077,7 +4072,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -4101,7 +4096,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -4125,7 +4120,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="4">
         <v>0.15</v>
@@ -4149,7 +4144,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="4">
         <v>0.1</v>
@@ -4173,7 +4168,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" s="4">
         <v>0.05</v>
@@ -4206,7 +4201,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -4226,7 +4221,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" s="1">
         <v>7.5</v>
@@ -4250,7 +4245,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -4258,7 +4253,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -4266,7 +4261,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" s="7">
         <f>B12*B15</f>
@@ -4275,7 +4270,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17" s="7">
         <f>B14*B16</f>
@@ -4284,7 +4279,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B18" s="9">
         <v>0.2</v>
@@ -4292,7 +4287,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B19" s="7">
         <f>B17*(B18+1)</f>
@@ -4307,7 +4302,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B22" s="7"/>
     </row>
@@ -4321,12 +4316,12 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4335,25 +4330,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="1">
-        <v>60000</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>234</v>
       </c>
       <c r="B3" s="1">
-        <v>45000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="1">
         <v>45000</v>
@@ -4365,25 +4352,25 @@
       </c>
       <c r="B6" s="1">
         <f>SUM(B2:B4)</f>
-        <v>150000</v>
+        <v>95000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="1">
         <f>B6/52</f>
-        <v>2884.6153846153848</v>
+        <v>1826.9230769230769</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B10" s="1">
         <f>B6/26</f>
-        <v>5769.2307692307695</v>
+        <v>3653.8461538461538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on powerpoint presentation. Updating finances: I might need part-time workers to man the front desk.
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1599" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{87713364-0840-449F-9515-BF9CDECD7660}"/>
+  <xr:revisionPtr revIDLastSave="1806" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C86C5F9-210D-433E-85CA-06C25F0C1889}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="246">
   <si>
     <t>Overhead</t>
   </si>
@@ -154,9 +154,6 @@
     <t>per PC, accessories, and software</t>
   </si>
   <si>
-    <t>four chairs, hard dining chairs, emphasis on cleanability</t>
-  </si>
-  <si>
     <t>long table, fits three PCs, 3x8 ft^2 design</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Costs Estimate</t>
   </si>
   <si>
-    <t>Custom Wooden Panel cover decorations per table</t>
-  </si>
-  <si>
     <t>Cleaning Supplies</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>Best case dance floor (synthetic)</t>
   </si>
   <si>
-    <t>no mirror for now because it would a pose a risk if converted to a nightclub</t>
-  </si>
-  <si>
     <t>Wifi</t>
   </si>
   <si>
@@ -217,15 +208,6 @@
     <t>sink installation and plumbing</t>
   </si>
   <si>
-    <t>hot plates</t>
-  </si>
-  <si>
-    <t>mini oven</t>
-  </si>
-  <si>
-    <t>airflow modifications</t>
-  </si>
-  <si>
     <t>premium refrigerator</t>
   </si>
   <si>
@@ -298,9 +280,6 @@
     <t>Paint cans needed</t>
   </si>
   <si>
-    <t>gaming</t>
-  </si>
-  <si>
     <t>dancing</t>
   </si>
   <si>
@@ -664,24 +643,9 @@
     <t>Target demographic</t>
   </si>
   <si>
-    <t>18-34 year-olds</t>
-  </si>
-  <si>
-    <t>https://data.census.gov/cedsci/table?g=1600000USundefined_0500000US09009&amp;tid=ACSST5Y2017.S0101&amp;q=S0101</t>
-  </si>
-  <si>
     <t>Target demographic size in New Haven County</t>
   </si>
   <si>
-    <t>20-24 year olds</t>
-  </si>
-  <si>
-    <t>29-34 year olds</t>
-  </si>
-  <si>
-    <t>25-29 year olds</t>
-  </si>
-  <si>
     <t>not including 18-19 year=olds due to lack of data</t>
   </si>
   <si>
@@ -691,9 +655,6 @@
     <t>True Total</t>
   </si>
   <si>
-    <t>2017 data</t>
-  </si>
-  <si>
     <t>Percent of people needed to break even</t>
   </si>
   <si>
@@ -736,9 +697,6 @@
     <t>sub-sub-communities</t>
   </si>
   <si>
-    <t>Diminishing returns</t>
-  </si>
-  <si>
     <t>rent</t>
   </si>
   <si>
@@ -749,21 +707,95 @@
   </si>
   <si>
     <t>Business Management/Maintenance</t>
+  </si>
+  <si>
+    <t>gas range</t>
+  </si>
+  <si>
+    <t>range hoods</t>
+  </si>
+  <si>
+    <t>hood installations</t>
+  </si>
+  <si>
+    <t>White board and markers</t>
+  </si>
+  <si>
+    <t>Comfy office chairs</t>
+  </si>
+  <si>
+    <t>counter installation</t>
+  </si>
+  <si>
+    <t>Operating Costs</t>
+  </si>
+  <si>
+    <t>mirror</t>
+  </si>
+  <si>
+    <t>Total for worst case scenario</t>
+  </si>
+  <si>
+    <t>Unforeseen Costs</t>
+  </si>
+  <si>
+    <t>PC area</t>
+  </si>
+  <si>
+    <t>https://data.census.gov/cedsci/table?q=S0101&amp;g=1600000USundefined_0500000US09009_0400000US09&amp;tid=ACSST1Y2018.S0101</t>
+  </si>
+  <si>
+    <t>40-44</t>
+  </si>
+  <si>
+    <t>35-39</t>
+  </si>
+  <si>
+    <t>29-34</t>
+  </si>
+  <si>
+    <t>25-29</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>45-49</t>
+  </si>
+  <si>
+    <t>50-54</t>
+  </si>
+  <si>
+    <t>55-59</t>
+  </si>
+  <si>
+    <t>60-64</t>
+  </si>
+  <si>
+    <t>65-69</t>
+  </si>
+  <si>
+    <t>70-74</t>
+  </si>
+  <si>
+    <t>Part-time greeter/security</t>
+  </si>
+  <si>
+    <t>18-80 year-olds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -786,8 +818,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -806,13 +844,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -823,7 +882,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -841,11 +900,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1164,186 +1224,249 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
-  <dimension ref="A3:C25"/>
+  <dimension ref="A3:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B4">
         <f>Net_And_Analysis!H5</f>
-        <v>243</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <f>Net_And_Analysis!H5</f>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B7">
-        <v>300</v>
+        <f>Net_And_Analysis!I5</f>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B8">
-        <v>350</v>
-      </c>
-      <c r="C8" t="s">
-        <v>230</v>
+        <f>Net_And_Analysis!J5</f>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B9">
+        <f>Net_And_Analysis!K5</f>
         <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="B10">
-        <v>450</v>
+        <f>Net_And_Analysis!L5</f>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B11">
-        <v>500</v>
+        <f>Net_And_Analysis!M5</f>
+        <v>580</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C14" t="s">
-        <v>215</v>
+        <v>199</v>
+      </c>
+      <c r="C14">
+        <v>2018</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>209</v>
-      </c>
-      <c r="B15" s="15">
-        <v>60592</v>
+        <v>237</v>
+      </c>
+      <c r="B15">
+        <v>58809</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>211</v>
-      </c>
-      <c r="B16" s="15">
-        <v>58106</v>
+        <v>236</v>
+      </c>
+      <c r="B16">
+        <v>56453</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>210</v>
-      </c>
-      <c r="B17" s="15">
-        <v>55391</v>
+        <v>235</v>
+      </c>
+      <c r="B17">
+        <v>58645</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="15">
-        <f>SUM(B15:B17)</f>
-        <v>174089</v>
+        <v>234</v>
+      </c>
+      <c r="B18">
+        <v>49754</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>213</v>
-      </c>
-      <c r="B19" s="15">
-        <v>25000</v>
+        <v>233</v>
+      </c>
+      <c r="B19">
+        <v>50741</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>238</v>
+      </c>
+      <c r="B20">
+        <v>54969</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>214</v>
-      </c>
-      <c r="B21" s="16">
-        <f>B18+B19</f>
-        <v>199089</v>
+        <v>239</v>
+      </c>
+      <c r="B21">
+        <v>59755</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>208</v>
-      </c>
-      <c r="B22" s="15">
-        <v>200000</v>
+        <v>240</v>
+      </c>
+      <c r="B22">
+        <v>59073</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>241</v>
+      </c>
+      <c r="B23">
+        <v>60768</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>216</v>
-      </c>
-      <c r="B24" s="18">
-        <f>B4/B22</f>
-        <v>1.2149999999999999E-3</v>
+        <v>242</v>
+      </c>
+      <c r="B24">
+        <v>45951</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>217</v>
-      </c>
-      <c r="B25" s="17">
-        <f>B9/B22</f>
-        <v>2E-3</v>
+        <v>243</v>
+      </c>
+      <c r="B25">
+        <v>37199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="15">
+        <f>SUM(B15:B25)</f>
+        <v>592117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="15">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="16">
+        <f>B28+B29</f>
+        <v>617117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="15"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="17">
+        <f>$B$4/$B$31</f>
+        <v>3.4677378843882116E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" s="17">
+        <f>$B$11/$B$28</f>
+        <v>9.7953613897253404E-4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1" xr:uid="{CBC7024E-77B0-4A57-9A0D-0571A1646C6F}"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{9F460612-A357-4BC2-96AB-6169A788747C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1354,43 +1477,43 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1">
         <v>35</v>
@@ -1415,197 +1538,208 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>226</v>
       </c>
       <c r="B3" s="1">
+        <v>700</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="G3" s="7">
+        <f>B3*C3</f>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1">
         <v>300</v>
       </c>
-      <c r="C3">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7">
+        <f>B4*C4</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G15" si="0">B5*C5</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="1">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="1">
+        <v>600</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8000</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="1">
+        <v>350</v>
+      </c>
+      <c r="C9">
+        <f>C7</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1">
+        <v>900</v>
+      </c>
+      <c r="C10">
         <f>$F$2</f>
         <v>3</v>
       </c>
-      <c r="G3" s="7">
-        <f>B3*C3</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="1">
-        <v>50</v>
-      </c>
-      <c r="C4">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4:G14" si="0">B4*C4</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="1">
-        <v>500</v>
-      </c>
-      <c r="C5">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="1">
         <v>100</v>
       </c>
-      <c r="C6">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G6" s="7">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="1">
-        <v>200</v>
-      </c>
-      <c r="C7">
-        <f>$F$2</f>
-        <v>3</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="1">
-        <v>300</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="1">
-        <v>900</v>
-      </c>
-      <c r="C9">
-        <f>$F$2</f>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1">
+        <v>250</v>
+      </c>
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="G9" s="7">
-        <f t="shared" si="0"/>
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="1">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="1">
-        <v>250</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="G14" s="7">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="1">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1">
         <v>80</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G17" s="7">
-        <f>SUM(G2:G14)</f>
-        <v>12865</v>
+        <f>SUM(G2:G15)</f>
+        <v>27115</v>
       </c>
     </row>
   </sheetData>
@@ -1628,12 +1762,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
@@ -1641,7 +1775,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
@@ -1649,7 +1783,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7">
         <f>B2+B3</f>
@@ -1679,24 +1813,24 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <f>D3</f>
@@ -1719,7 +1853,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1741,7 +1875,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1763,7 +1897,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1785,7 +1919,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1">
         <f>SUM(F3:F6)</f>
@@ -1821,39 +1955,39 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" t="s">
-        <v>83</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -1893,7 +2027,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1">
         <v>400</v>
@@ -1901,7 +2035,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="K4" s="1">
         <v>200</v>
@@ -1909,7 +2043,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1">
         <f>SUM(K2:K4)</f>
@@ -2203,10 +2337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAC8DE-41B9-46A0-BE44-EAAB92E58FB4}">
-  <dimension ref="A3:H25"/>
+  <dimension ref="A3:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2220,34 +2354,34 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>231</v>
       </c>
       <c r="B3" s="7">
-        <f>Gaming!D11</f>
-        <v>16930</v>
+        <f>Gaming!D12</f>
+        <v>19680</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7">
-        <f>Dance_Studio!D5</f>
-        <v>5000</v>
+        <f>Dance_Studio!D8</f>
+        <v>16500</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B5" s="7">
         <f>Kitchen!G17</f>
-        <v>12865</v>
+        <v>27115</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B6" s="7">
         <f>Liabilities!B7</f>
@@ -2256,7 +2390,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B7" s="7">
         <f>decor!K7</f>
@@ -2265,167 +2399,205 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B8" s="7">
         <f>'Eating Area'!F10</f>
         <v>3200</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="7">
+        <f>SUM(B3:B8)</f>
+        <v>67445</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="7">
-        <f>SUM(B3:B8)</f>
-        <v>38945</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="7">
-        <f>Operating_Costs!F13</f>
-        <v>252166.66666666666</v>
+        <v>230</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
+        <v>128</v>
+      </c>
+      <c r="B13" s="7">
+        <f>Operating_Costs!F13</f>
+        <v>222166.66666666666</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B14">
-        <f>B13/12</f>
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <f>B14/12</f>
         <v>0.5</v>
       </c>
-      <c r="C14">
-        <f t="shared" ref="C14:G14" si="0">C13/12</f>
+      <c r="C15">
+        <f t="shared" ref="C15:G15" si="0">C14/12</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B15" s="7">
-        <f>$B$11+($B$12*B14)</f>
-        <v>165028.33333333331</v>
-      </c>
-      <c r="C15" s="7">
-        <f t="shared" ref="C15:G15" si="1">$B$11+($B$12*C14)</f>
-        <v>144014.44444444444</v>
-      </c>
-      <c r="D15" s="7">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B16" s="7">
+        <f>$B$13*B$15</f>
+        <v>111083.33333333333</v>
+      </c>
+      <c r="C16" s="7">
+        <f>$B$13*C$15</f>
+        <v>92569.444444444438</v>
+      </c>
+      <c r="D16" s="7">
+        <f>$B$13*D$15</f>
+        <v>74055.555555555547</v>
+      </c>
+      <c r="E16" s="7">
+        <f>$B$13*E$15</f>
+        <v>55541.666666666664</v>
+      </c>
+      <c r="F16" s="7">
+        <f>$B$13*F$15</f>
+        <v>37027.777777777774</v>
+      </c>
+      <c r="G16" s="7">
+        <f>$B$13*G$15</f>
+        <v>18513.888888888887</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B17" s="7">
+        <f>$B$10+($B$13*B$15)+$B$11</f>
+        <v>188528.33333333331</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" ref="C17:G17" si="1">$B$10+($B$13*C$15)+$B$11</f>
+        <v>170014.44444444444</v>
+      </c>
+      <c r="D17" s="7">
         <f t="shared" si="1"/>
-        <v>123000.55555555555</v>
-      </c>
-      <c r="E15" s="7">
+        <v>151500.55555555556</v>
+      </c>
+      <c r="E17" s="7">
         <f t="shared" si="1"/>
-        <v>101986.66666666666</v>
-      </c>
-      <c r="F15" s="7">
+        <v>132986.66666666666</v>
+      </c>
+      <c r="F17" s="7">
         <f t="shared" si="1"/>
-        <v>80972.777777777781</v>
-      </c>
-      <c r="G15" s="7">
+        <v>114472.77777777778</v>
+      </c>
+      <c r="G17" s="7">
         <f t="shared" si="1"/>
-        <v>59958.888888888891</v>
-      </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>225</v>
-      </c>
-      <c r="B19" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>95958.888888888891</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>223</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B25" t="s">
-        <v>233</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2435,10 +2607,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A112772E-1427-43D2-80C2-98741A931E56}">
-  <dimension ref="A4:L29"/>
+  <dimension ref="A4:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2448,19 +2620,20 @@
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H4" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="K4" s="12" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2490,28 +2663,32 @@
       </c>
       <c r="H5" s="10">
         <f>Gross!I30</f>
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="I5">
         <f>Gross!J30</f>
-        <v>320</v>
+        <v>250</v>
       </c>
       <c r="J5">
         <f>Gross!K30</f>
+        <v>300</v>
+      </c>
+      <c r="K5" s="19">
+        <f>Gross!L30</f>
         <v>400</v>
-      </c>
-      <c r="K5" s="12">
-        <f>Gross!L30</f>
-        <v>500</v>
       </c>
       <c r="L5">
         <f>Gross!M30</f>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+      <c r="M5" s="12">
+        <f>Gross!N30</f>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B6" s="7">
         <f>Gross!C45</f>
@@ -2539,177 +2716,185 @@
       </c>
       <c r="H6" s="11">
         <f>Gross!I45</f>
-        <v>252720.00000000006</v>
+        <v>222560.00000000006</v>
       </c>
       <c r="I6" s="7">
         <f>Gross!J45</f>
-        <v>332800.00000000006</v>
+        <v>260000.00000000006</v>
       </c>
       <c r="J6" s="7">
         <f>Gross!K45</f>
+        <v>312000.00000000006</v>
+      </c>
+      <c r="K6" s="20">
+        <f>Gross!L45</f>
         <v>416000.00000000012</v>
-      </c>
-      <c r="K6" s="13">
-        <f>Gross!L45</f>
-        <v>520000.00000000012</v>
       </c>
       <c r="L6" s="7">
         <f>Gross!M45</f>
-        <v>624000.00000000012</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>520000.00000000012</v>
+      </c>
+      <c r="M6" s="13">
+        <f>Gross!N45</f>
+        <v>603200.00000000012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B8" s="7">
         <f>Operating_Costs!F13</f>
-        <v>252166.66666666666</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>222166.66666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B10" s="7">
         <f>B6-$B$8</f>
-        <v>-246966.66666666666</v>
+        <v>-216966.66666666666</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:L10" si="0">C6-$B$8</f>
-        <v>-241766.66666666666</v>
+        <v>-211766.66666666666</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>-231366.66666666666</v>
+        <v>-201366.66666666666</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>-210566.66666666666</v>
+        <v>-180566.66666666666</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
-        <v>-168966.66666666663</v>
+        <v>-138966.66666666663</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>-85766.666666666628</v>
+        <v>-55766.666666666628</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>553.33333333340124</v>
+        <v>393.33333333340124</v>
       </c>
       <c r="I10" s="7">
         <f t="shared" si="0"/>
-        <v>80633.333333333401</v>
+        <v>37833.333333333401</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="0"/>
-        <v>163833.33333333346</v>
-      </c>
-      <c r="K10" s="13">
+        <v>89833.333333333401</v>
+      </c>
+      <c r="K10" s="20">
         <f t="shared" si="0"/>
-        <v>267833.33333333349</v>
+        <v>193833.33333333346</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="0"/>
-        <v>371833.33333333349</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>297833.33333333349</v>
+      </c>
+      <c r="M10" s="13">
+        <f t="shared" ref="M10" si="1">M6-$B$8</f>
+        <v>381033.33333333349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B12">
         <f>H5</f>
-        <v>243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B13">
         <f>Gross!I37</f>
-        <v>38.88000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>34.240000000000009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B16">
-        <f>K5</f>
-        <v>500</v>
+        <f>M5</f>
+        <v>580</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B17">
         <f>B16*0.2</f>
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C17">
         <f>B17/2</f>
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B18">
         <f>B16-(0.2*710)</f>
-        <v>358</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B20">
         <f>Gross!L37</f>
-        <v>80.000000000000014</v>
+        <v>64.000000000000014</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B21" s="9">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B22">
         <f>B20*(1+B21)</f>
-        <v>120.00000000000003</v>
+        <v>112.00000000000003</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B24">
         <f>Gross!B7</f>
@@ -2718,7 +2903,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2726,7 +2911,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B26">
         <f>B24*B25</f>
@@ -2735,16 +2920,16 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B28">
         <f>B26-B22</f>
-        <v>49.999999999999972</v>
+        <v>57.999999999999972</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B29">
         <f>C17-B28</f>
@@ -2758,10 +2943,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7959888-B526-4FAC-9FC1-7A03020906F6}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2775,40 +2960,41 @@
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B3">
         <f>10</f>
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F3" s="9">
         <v>0.2</v>
@@ -2817,13 +3003,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F4" s="9">
         <v>0.8</v>
@@ -2831,7 +3017,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -2839,7 +3025,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <f>SUM(B2:B5)</f>
@@ -2848,22 +3034,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C12" s="9">
         <v>0.2</v>
@@ -2874,7 +3060,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B13" s="1">
         <v>40</v>
@@ -2888,7 +3074,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
@@ -2902,7 +3088,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B15" s="1">
         <v>20</v>
@@ -2914,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D17" s="9">
         <v>0.2</v>
       </c>
@@ -2923,39 +3109,39 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E19" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
         <v>0.8</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D20" s="8">
         <v>0.8</v>
@@ -2972,13 +3158,13 @@
         <v>0.25600000000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
       <c r="B21">
         <v>0.2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D21" s="8">
         <v>0.2</v>
@@ -2995,13 +3181,13 @@
         <v>9.600000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
       <c r="B22">
         <v>0.8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D22" s="8">
         <v>0.8</v>
@@ -3018,13 +3204,13 @@
         <v>0.51200000000000012</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
       <c r="B23">
         <v>0.8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D23" s="8">
         <v>0.2</v>
@@ -3041,32 +3227,32 @@
         <v>0.25600000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D24" s="3"/>
       <c r="E24" s="3">
         <f>SUM(E20:E23)</f>
         <v>0.80000000000000016</v>
       </c>
       <c r="F24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G24">
         <f>SUM(G20:G23)</f>
         <v>1.1200000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="19">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="18">
         <v>0.2</v>
       </c>
       <c r="B25" s="8">
         <v>0.8</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" t="s">
         <v>165</v>
-      </c>
-      <c r="D25" t="s">
-        <v>172</v>
       </c>
       <c r="E25" s="3">
         <f>$A$25*$B25</f>
@@ -3076,16 +3262,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="19"/>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
       <c r="B26" s="8">
         <v>0.2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E26" s="3">
         <f>$A$25*$B26</f>
@@ -3095,30 +3281,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E27">
         <f>SUM(E25:E26)</f>
         <v>0.20000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E28">
         <f>E24+E27</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -3139,24 +3325,27 @@
         <v>160</v>
       </c>
       <c r="I30">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="J30">
-        <v>320</v>
+        <v>250</v>
       </c>
       <c r="K30">
+        <v>300</v>
+      </c>
+      <c r="L30">
         <v>400</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>500</v>
       </c>
-      <c r="M30">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
@@ -3187,28 +3376,32 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" ref="I31" si="3">$E20*$F20*$B31*I$30</f>
-        <v>622.08000000000015</v>
+        <v>547.84000000000015</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" ref="J31:M34" si="4">$E20*$F20*$B31*J$30</f>
-        <v>819.20000000000016</v>
+        <v>640.00000000000011</v>
       </c>
       <c r="K31" s="1">
         <f t="shared" si="4"/>
-        <v>1024.0000000000002</v>
+        <v>768.00000000000011</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="4"/>
-        <v>1280.0000000000002</v>
+        <v>1024.0000000000002</v>
       </c>
       <c r="M31" s="1">
         <f t="shared" si="4"/>
-        <v>1536.0000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1280.0000000000002</v>
+      </c>
+      <c r="N31" s="1">
+        <f>$E20*$F20*$B31*N$30</f>
+        <v>1484.8000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B32" s="1">
         <v>10</v>
@@ -3239,28 +3432,32 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" ref="I32" si="6">$E21*$F21*$B32*I$30</f>
-        <v>233.28000000000009</v>
+        <v>205.44000000000005</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="4"/>
-        <v>307.2000000000001</v>
+        <v>240.00000000000009</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="4"/>
-        <v>384.00000000000011</v>
+        <v>288.00000000000011</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="4"/>
-        <v>480.00000000000017</v>
+        <v>384.00000000000011</v>
       </c>
       <c r="M32" s="1">
         <f t="shared" si="4"/>
-        <v>576.00000000000023</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+        <v>480.00000000000017</v>
+      </c>
+      <c r="N32" s="1">
+        <f t="shared" ref="N32" si="7">$E21*$F21*$B32*N$30</f>
+        <v>556.80000000000018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B33" s="1">
         <v>20</v>
@@ -3290,29 +3487,33 @@
         <v>1638.4000000000003</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" ref="I33" si="7">$E22*$F22*$B33*I$30</f>
-        <v>2488.3200000000006</v>
+        <f t="shared" ref="I33" si="8">$E22*$F22*$B33*I$30</f>
+        <v>2191.3600000000006</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="4"/>
-        <v>3276.8000000000006</v>
+        <v>2560.0000000000005</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" si="4"/>
-        <v>4096.0000000000009</v>
+        <v>3072.0000000000005</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="4"/>
-        <v>5120.0000000000009</v>
+        <v>4096.0000000000009</v>
       </c>
       <c r="M33" s="1">
         <f t="shared" si="4"/>
-        <v>6144.0000000000009</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+        <v>5120.0000000000009</v>
+      </c>
+      <c r="N33" s="1">
+        <f t="shared" ref="N33" si="9">$E22*$F22*$B33*N$30</f>
+        <v>5939.2000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B34" s="1">
         <v>20</v>
@@ -3342,29 +3543,33 @@
         <v>819.20000000000016</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" ref="I34" si="8">$E23*$F23*$B34*I$30</f>
-        <v>1244.1600000000003</v>
+        <f t="shared" ref="I34" si="10">$E23*$F23*$B34*I$30</f>
+        <v>1095.6800000000003</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="4"/>
-        <v>1638.4000000000003</v>
+        <v>1280.0000000000002</v>
       </c>
       <c r="K34" s="1">
         <f t="shared" si="4"/>
-        <v>2048.0000000000005</v>
+        <v>1536.0000000000002</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="4"/>
-        <v>2560.0000000000005</v>
+        <v>2048.0000000000005</v>
       </c>
       <c r="M34" s="1">
         <f t="shared" si="4"/>
-        <v>3072.0000000000005</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+        <v>2560.0000000000005</v>
+      </c>
+      <c r="N34" s="1">
+        <f t="shared" ref="N34" si="11">$E23*$F23*$B34*N$30</f>
+        <v>2969.6000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C35" s="7">
         <f>SUM(C31:C34)</f>
@@ -3375,337 +3580,365 @@
         <v>188.80000000000004</v>
       </c>
       <c r="E35" s="7">
-        <f t="shared" ref="E35:I35" si="9">SUM(E31:E34)</f>
+        <f t="shared" ref="E35:I35" si="12">SUM(E31:E34)</f>
         <v>377.60000000000008</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>755.20000000000016</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1510.4000000000003</v>
       </c>
       <c r="H35" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>3020.8000000000006</v>
       </c>
       <c r="I35" s="7">
-        <f t="shared" si="9"/>
-        <v>4587.8400000000011</v>
+        <f t="shared" si="12"/>
+        <v>4040.3200000000011</v>
       </c>
       <c r="J35" s="7">
         <f>SUM(J31:J34)</f>
-        <v>6041.6000000000013</v>
+        <v>4720.0000000000009</v>
       </c>
       <c r="K35" s="7">
         <f>SUM(K31:K34)</f>
-        <v>7552.0000000000018</v>
+        <v>5664.0000000000009</v>
       </c>
       <c r="L35" s="7">
         <f>SUM(L31:L34)</f>
-        <v>9440.0000000000018</v>
+        <v>7552.0000000000018</v>
       </c>
       <c r="M35" s="7">
         <f>SUM(M31:M34)</f>
-        <v>11328.000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+        <v>9440.0000000000018</v>
+      </c>
+      <c r="N35" s="7">
+        <f>SUM(N31:N34)</f>
+        <v>10950.400000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C36" s="3">
         <f>C$30*($G$24)</f>
         <v>5.6000000000000014</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" ref="D36:I36" si="10">D$30*($G$24)</f>
+        <f t="shared" ref="D36:I36" si="13">D$30*($G$24)</f>
         <v>11.200000000000003</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>22.400000000000006</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>44.800000000000011</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>89.600000000000023</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>179.20000000000005</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="10"/>
-        <v>272.16000000000008</v>
+        <f t="shared" si="13"/>
+        <v>239.68000000000006</v>
       </c>
       <c r="J36" s="3">
         <f>J$30*($G$24)</f>
-        <v>358.40000000000009</v>
+        <v>280.00000000000006</v>
       </c>
       <c r="K36" s="3">
         <f>K$30*($G$24)</f>
-        <v>448.00000000000011</v>
+        <v>336.00000000000011</v>
       </c>
       <c r="L36" s="3">
         <f>L$30*($G$24)</f>
-        <v>560.00000000000011</v>
+        <v>448.00000000000011</v>
       </c>
       <c r="M36" s="3">
         <f>M$30*($G$24)</f>
-        <v>672.00000000000023</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+        <v>560.00000000000011</v>
+      </c>
+      <c r="N36" s="3">
+        <f>N$30*($G$24)</f>
+        <v>649.60000000000014</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C37">
         <f>C36/7</f>
         <v>0.80000000000000016</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:I37" si="11">D36/7</f>
+        <f t="shared" ref="D37:I37" si="14">D36/7</f>
         <v>1.6000000000000003</v>
       </c>
       <c r="E37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>3.2000000000000006</v>
       </c>
       <c r="F37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>6.4000000000000012</v>
       </c>
       <c r="G37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>12.800000000000002</v>
       </c>
       <c r="H37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>25.600000000000005</v>
       </c>
       <c r="I37">
-        <f t="shared" si="11"/>
-        <v>38.88000000000001</v>
+        <f t="shared" si="14"/>
+        <v>34.240000000000009</v>
       </c>
       <c r="J37">
         <f>J36/7</f>
-        <v>51.20000000000001</v>
+        <v>40.000000000000007</v>
       </c>
       <c r="K37">
         <f>K36/7</f>
-        <v>64.000000000000014</v>
+        <v>48.000000000000014</v>
       </c>
       <c r="L37">
         <f>L36/7</f>
-        <v>80.000000000000014</v>
+        <v>64.000000000000014</v>
       </c>
       <c r="M37">
         <f>M36/7</f>
-        <v>96.000000000000028</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+        <v>80.000000000000014</v>
+      </c>
+      <c r="N37">
+        <f>N36/7</f>
+        <v>92.800000000000026</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" ref="C41:M41" si="12">C35*50</f>
+        <f t="shared" ref="C41:M41" si="15">C35*50</f>
         <v>4720.0000000000009</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>9440.0000000000018</v>
       </c>
       <c r="E41" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>18880.000000000004</v>
       </c>
       <c r="F41" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>37760.000000000007</v>
       </c>
       <c r="G41" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>75520.000000000015</v>
       </c>
       <c r="H41" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>151040.00000000003</v>
       </c>
       <c r="I41" s="7">
-        <f t="shared" si="12"/>
-        <v>229392.00000000006</v>
+        <f t="shared" si="15"/>
+        <v>202016.00000000006</v>
       </c>
       <c r="J41" s="7">
-        <f t="shared" si="12"/>
-        <v>302080.00000000006</v>
+        <f t="shared" si="15"/>
+        <v>236000.00000000006</v>
       </c>
       <c r="K41" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
+        <v>283200.00000000006</v>
+      </c>
+      <c r="L41" s="7">
+        <f t="shared" si="15"/>
         <v>377600.00000000012</v>
       </c>
-      <c r="L41" s="7">
-        <f t="shared" si="12"/>
+      <c r="M41" s="7">
+        <f t="shared" si="15"/>
         <v>472000.00000000012</v>
       </c>
-      <c r="M41" s="7">
-        <f t="shared" si="12"/>
-        <v>566400.00000000012</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N41" s="7">
+        <f t="shared" ref="N41" si="16">N35*50</f>
+        <v>547520.00000000012</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B42" s="1">
         <v>40</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" ref="C42:M42" si="13">C$30*$B42*$A$25</f>
+        <f t="shared" ref="C42:N42" si="17">C$30*$B42*$A$25</f>
         <v>40</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>80</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>160</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>320</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>640</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1280</v>
       </c>
       <c r="I42" s="7">
-        <f t="shared" si="13"/>
-        <v>1944</v>
+        <f t="shared" si="17"/>
+        <v>1712</v>
       </c>
       <c r="J42" s="7">
-        <f t="shared" si="13"/>
-        <v>2560</v>
+        <f t="shared" si="17"/>
+        <v>2000</v>
       </c>
       <c r="K42" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
+        <v>2400</v>
+      </c>
+      <c r="L42" s="7">
+        <f t="shared" si="17"/>
         <v>3200</v>
       </c>
-      <c r="L42" s="7">
-        <f t="shared" si="13"/>
+      <c r="M42" s="7">
+        <f t="shared" si="17"/>
         <v>4000</v>
       </c>
-      <c r="M42" s="7">
-        <f t="shared" si="13"/>
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N42" s="7">
+        <f t="shared" si="17"/>
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C43" s="7">
         <f>C42*12</f>
         <v>480</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" ref="D43:I43" si="14">D42*12</f>
+        <f t="shared" ref="D43:I43" si="18">D42*12</f>
         <v>960</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1920</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3840</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>7680</v>
       </c>
       <c r="H43" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>15360</v>
       </c>
       <c r="I43" s="7">
-        <f t="shared" si="14"/>
-        <v>23328</v>
+        <f t="shared" si="18"/>
+        <v>20544</v>
       </c>
       <c r="J43" s="7">
         <f>J42*12</f>
-        <v>30720</v>
+        <v>24000</v>
       </c>
       <c r="K43" s="7">
         <f>K42*12</f>
-        <v>38400</v>
+        <v>28800</v>
       </c>
       <c r="L43" s="7">
         <f>L42*12</f>
-        <v>48000</v>
+        <v>38400</v>
       </c>
       <c r="M43" s="7">
         <f>M42*12</f>
-        <v>57600</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+        <v>48000</v>
+      </c>
+      <c r="N43" s="7">
+        <f>N42*12</f>
+        <v>55680</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" ref="C45:M45" si="15">C43+C41</f>
+        <f t="shared" ref="C45:M45" si="19">C43+C41</f>
         <v>5200.0000000000009</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>10400.000000000002</v>
       </c>
       <c r="E45" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>20800.000000000004</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>41600.000000000007</v>
       </c>
       <c r="G45" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>83200.000000000015</v>
       </c>
       <c r="H45" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>166400.00000000003</v>
       </c>
       <c r="I45" s="7">
-        <f t="shared" si="15"/>
-        <v>252720.00000000006</v>
+        <f t="shared" si="19"/>
+        <v>222560.00000000006</v>
       </c>
       <c r="J45" s="7">
-        <f t="shared" si="15"/>
-        <v>332800.00000000006</v>
+        <f t="shared" si="19"/>
+        <v>260000.00000000006</v>
       </c>
       <c r="K45" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
+        <v>312000.00000000006</v>
+      </c>
+      <c r="L45" s="7">
+        <f t="shared" si="19"/>
         <v>416000.00000000012</v>
       </c>
-      <c r="L45" s="7">
-        <f t="shared" si="15"/>
+      <c r="M45" s="7">
+        <f t="shared" si="19"/>
         <v>520000.00000000012</v>
       </c>
-      <c r="M45" s="7">
-        <f t="shared" si="15"/>
-        <v>624000.00000000012</v>
+      <c r="N45" s="7">
+        <f t="shared" ref="N45" si="20">N43+N41</f>
+        <v>603200.00000000012</v>
       </c>
     </row>
   </sheetData>
@@ -3722,7 +3955,7 @@
   <dimension ref="A3:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3737,24 +3970,24 @@
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1">
         <f>C4/7</f>
@@ -3766,11 +3999,11 @@
       </c>
       <c r="D4" s="1">
         <f>employees!B9</f>
-        <v>1826.9230769230769</v>
+        <v>2307.6923076923076</v>
       </c>
       <c r="E4" s="1">
         <f>D4*2</f>
-        <v>3653.8461538461538</v>
+        <v>4615.3846153846152</v>
       </c>
       <c r="F4" s="1">
         <v>4000</v>
@@ -3778,31 +4011,32 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1">
         <f>C5/7</f>
-        <v>260.98901098901098</v>
+        <v>329.67032967032964</v>
       </c>
       <c r="C5" s="1">
         <f>employees!B9</f>
-        <v>1826.9230769230769</v>
+        <v>2307.6923076923076</v>
       </c>
       <c r="D5" s="1">
         <f>employees!B10</f>
-        <v>3653.8461538461538</v>
+        <v>4615.3846153846152</v>
       </c>
       <c r="E5" s="1">
         <f>D5*2</f>
-        <v>7307.6923076923076</v>
+        <v>9230.7692307692305</v>
       </c>
       <c r="F5" s="1">
-        <v>150000</v>
+        <f>employees!B6</f>
+        <v>120000</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1">
         <f>200/30</f>
@@ -3827,7 +4061,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B7" s="1">
         <f>400/30</f>
@@ -3852,7 +4086,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1">
         <f>100/30</f>
@@ -3877,7 +4111,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1">
         <f>C9/7</f>
@@ -3902,7 +4136,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B10" s="1">
         <f>C10/7</f>
@@ -3926,7 +4160,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1">
         <f>C11/7</f>
@@ -3950,54 +4184,54 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B12" s="1">
         <f>C12/7</f>
-        <v>714.28571428571433</v>
+        <v>164.83516483516482</v>
       </c>
       <c r="C12" s="1">
-        <f>F12/12</f>
-        <v>5000</v>
+        <f>F12/52</f>
+        <v>1153.8461538461538</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>2307.6923076923076</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>4615.3846153846152</v>
       </c>
       <c r="F12" s="1">
         <v>60000</v>
       </c>
       <c r="H12" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1">
         <f>SUM(B4:B12)</f>
-        <v>1095.0915750915751</v>
+        <v>614.32234432234429</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:F13" si="1">SUM(C4:C12)</f>
-        <v>7665.6410256410254</v>
+        <v>4300.2564102564102</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>17004.358974358976</v>
+        <v>10754.358974358973</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>34008.717948717953</v>
+        <v>21508.717948717946</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>252166.66666666666</v>
+        <v>222166.66666666666</v>
       </c>
       <c r="H13" s="6">
         <v>5000</v>
@@ -4005,7 +4239,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4017,7 +4251,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72B0531-F9EA-4BB7-8657-7C884FA8D7D5}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4034,21 +4270,21 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -4072,7 +4308,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -4096,7 +4332,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -4120,7 +4356,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4">
         <v>0.15</v>
@@ -4144,7 +4380,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B6" s="4">
         <v>0.1</v>
@@ -4168,7 +4404,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B7" s="4">
         <v>0.05</v>
@@ -4192,7 +4428,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="9">
         <f>SUM(B3:B7)</f>
@@ -4201,7 +4437,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -4221,7 +4457,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1">
         <v>7.5</v>
@@ -4245,7 +4481,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -4253,7 +4489,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -4261,7 +4497,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B16" s="7">
         <f>B12*B15</f>
@@ -4270,7 +4506,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B17" s="7">
         <f>B14*B16</f>
@@ -4279,7 +4515,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B18" s="9">
         <v>0.2</v>
@@ -4287,7 +4523,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B19" s="7">
         <f>B17*(B18+1)</f>
@@ -4302,7 +4538,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B22" s="7"/>
     </row>
@@ -4313,10 +4549,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4327,12 +4563,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B3" s="1">
         <v>50000</v>
@@ -4340,37 +4576,54 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1">
         <v>45000</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" s="1">
+        <v>25000</v>
+      </c>
+    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1">
-        <f>SUM(B2:B4)</f>
-        <v>95000</v>
+        <f>SUM(B2:B5)</f>
+        <v>120000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B9" s="1">
         <f>B6/52</f>
-        <v>1826.9230769230769</v>
+        <v>2307.6923076923076</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1">
         <f>B6/26</f>
-        <v>3653.8461538461538</v>
+        <v>4615.3846153846152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="1">
+        <f>B10*2</f>
+        <v>9230.7692307692305</v>
       </c>
     </row>
   </sheetData>
@@ -4380,10 +4633,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E8F79C-848E-45C7-B440-BCF016365DF9}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4396,13 +4649,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4410,44 +4663,45 @@
         <v>35</v>
       </c>
       <c r="B2" s="1">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2" s="7">
         <f>B2*C2</f>
-        <v>15000</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" ref="D3:D8" si="0">B3*C3</f>
-        <v>400</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>225</v>
       </c>
       <c r="B4" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <f>C3</f>
+        <v>12</v>
       </c>
       <c r="D4" s="7">
-        <f t="shared" si="0"/>
-        <v>330</v>
+        <f>B4*C4</f>
+        <v>1200</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4455,69 +4709,68 @@
         <v>42</v>
       </c>
       <c r="B5" s="1">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C5">
-        <f>C3</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>224</v>
       </c>
       <c r="B8" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="7">
         <f>SUM(D2:D8)</f>
-        <v>16930</v>
+        <v>19680</v>
       </c>
     </row>
   </sheetData>
@@ -4527,10 +4780,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6007EBCF-A6A9-4054-90A6-E709ADB7E2B5}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4543,23 +4796,23 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1">
         <v>15</v>
@@ -4572,12 +4825,12 @@
         <v>13500</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -4595,7 +4848,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1">
         <v>5000</v>
@@ -4603,7 +4856,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>228</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="7">
+        <f>D3+D6</f>
+        <v>16500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created the powerpoint presentation
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1806" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C86C5F9-210D-433E-85CA-06C25F0C1889}"/>
+  <xr:revisionPtr revIDLastSave="1824" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{571B69B0-BB1B-4B0D-8528-62A11DB95011}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="249">
   <si>
     <t>Overhead</t>
   </si>
@@ -601,9 +601,6 @@
     <t>Waves of people</t>
   </si>
   <si>
-    <t>Breakeven Point</t>
-  </si>
-  <si>
     <t>Estimated possible visits per day</t>
   </si>
   <si>
@@ -782,6 +779,18 @@
   </si>
   <si>
     <t>18-80 year-olds</t>
+  </si>
+  <si>
+    <t>Break-even Point</t>
+  </si>
+  <si>
+    <t>Estimate Number of People</t>
+  </si>
+  <si>
+    <t>Website Setup</t>
+  </si>
+  <si>
+    <t>Total Overhead Costs</t>
   </si>
 </sst>
 </file>
@@ -793,7 +802,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -882,7 +891,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -893,19 +902,21 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1226,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,12 +1249,12 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4">
         <f>Net_And_Analysis!H5</f>
@@ -1252,7 +1263,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <f>Net_And_Analysis!H5</f>
@@ -1261,7 +1272,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7">
         <f>Net_And_Analysis!I5</f>
@@ -1270,7 +1281,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B8">
         <f>Net_And_Analysis!J5</f>
@@ -1279,7 +1290,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B9">
         <f>Net_And_Analysis!K5</f>
@@ -1288,7 +1299,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10">
         <f>Net_And_Analysis!L5</f>
@@ -1297,7 +1308,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11">
         <f>Net_And_Analysis!M5</f>
@@ -1306,18 +1317,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>245</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>232</v>
+        <v>244</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14">
         <v>2018</v>
@@ -1325,7 +1336,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B15">
         <v>58809</v>
@@ -1333,7 +1344,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B16">
         <v>56453</v>
@@ -1341,7 +1352,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B17">
         <v>58645</v>
@@ -1349,7 +1360,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B18">
         <v>49754</v>
@@ -1357,7 +1368,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B19">
         <v>50741</v>
@@ -1365,7 +1376,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B20">
         <v>54969</v>
@@ -1373,7 +1384,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B21">
         <v>59755</v>
@@ -1381,7 +1392,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B22">
         <v>59073</v>
@@ -1389,7 +1400,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B23">
         <v>60768</v>
@@ -1397,7 +1408,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B24">
         <v>45951</v>
@@ -1405,7 +1416,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B25">
         <v>37199</v>
@@ -1415,50 +1426,55 @@
       <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="11">
         <f>SUM(B15:B25)</f>
         <v>592117</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>201</v>
-      </c>
-      <c r="B29" s="15">
+        <v>200</v>
+      </c>
+      <c r="B29" s="11">
         <v>25000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>202</v>
-      </c>
-      <c r="B31" s="16">
+        <v>201</v>
+      </c>
+      <c r="B31" s="12">
         <f>B28+B29</f>
         <v>617117</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="15"/>
+      <c r="A32" t="s">
+        <v>246</v>
+      </c>
+      <c r="B32" s="11">
+        <v>620000</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>203</v>
-      </c>
-      <c r="B34" s="17">
+        <v>202</v>
+      </c>
+      <c r="B34" s="13">
         <f>$B$4/$B$31</f>
         <v>3.4677378843882116E-4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>204</v>
-      </c>
-      <c r="B35" s="17">
+        <v>203</v>
+      </c>
+      <c r="B35" s="13">
         <f>$B$11/$B$28</f>
         <v>9.7953613897253404E-4</v>
       </c>
@@ -1538,7 +1554,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B3" s="1">
         <v>700</v>
@@ -1598,7 +1614,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B7" s="1">
         <v>600</v>
@@ -1613,7 +1629,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" s="1">
         <v>8000</v>
@@ -1628,7 +1644,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B9" s="1">
         <v>350</v>
@@ -2337,10 +2353,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAC8DE-41B9-46A0-BE44-EAAB92E58FB4}">
-  <dimension ref="A3:H26"/>
+  <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2352,16 +2368,16 @@
     <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B3" s="7">
         <f>Gaming!D12</f>
         <v>19680</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -2370,7 +2386,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -2379,7 +2395,7 @@
         <v>27115</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -2388,7 +2404,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -2397,7 +2413,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -2406,7 +2422,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -2415,189 +2431,206 @@
         <v>67445</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>230</v>
-      </c>
-      <c r="B11" s="1">
+        <v>247</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="7">
+        <f>SUM(B10:B12)</f>
+        <v>79445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B15" s="7">
         <f>Operating_Costs!F13</f>
         <v>222166.66666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>129</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>6</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>5</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>4</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <v>2</v>
       </c>
-      <c r="G14">
+      <c r="G16">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B15">
-        <f>B14/12</f>
+      <c r="B17">
+        <f>B16/12</f>
         <v>0.5</v>
       </c>
-      <c r="C15">
-        <f t="shared" ref="C15:G15" si="0">C14/12</f>
+      <c r="C17">
+        <f t="shared" ref="C17:G17" si="0">C16/12</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G15">
+      <c r="G17">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>227</v>
-      </c>
-      <c r="B16" s="7">
-        <f>$B$13*B$15</f>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="7">
+        <f>$B$15*B$17</f>
         <v>111083.33333333333</v>
       </c>
-      <c r="C16" s="7">
-        <f>$B$13*C$15</f>
+      <c r="C18" s="7">
+        <f>$B$15*C$17</f>
         <v>92569.444444444438</v>
       </c>
-      <c r="D16" s="7">
-        <f>$B$13*D$15</f>
+      <c r="D18" s="7">
+        <f>$B$15*D$17</f>
         <v>74055.555555555547</v>
       </c>
-      <c r="E16" s="7">
-        <f>$B$13*E$15</f>
+      <c r="E18" s="7">
+        <f>$B$15*E$17</f>
         <v>55541.666666666664</v>
       </c>
-      <c r="F16" s="7">
-        <f>$B$13*F$15</f>
+      <c r="F18" s="7">
+        <f>$B$15*F$17</f>
         <v>37027.777777777774</v>
       </c>
-      <c r="G16" s="7">
-        <f>$B$13*G$15</f>
+      <c r="G18" s="7">
+        <f>$B$15*G$17</f>
         <v>18513.888888888887</v>
       </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="7">
-        <f>$B$10+($B$13*B$15)+$B$11</f>
-        <v>188528.33333333331</v>
-      </c>
-      <c r="C17" s="7">
-        <f t="shared" ref="C17:G17" si="1">$B$10+($B$13*C$15)+$B$11</f>
-        <v>170014.44444444444</v>
-      </c>
-      <c r="D17" s="7">
+      <c r="B19" s="7">
+        <f>$B$10+($B$15*B$17)+$B$12+$B$11</f>
+        <v>190528.33333333331</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" ref="C19:G19" si="1">$B$10+($B$15*C$17)+$B$12+$B$11</f>
+        <v>172014.44444444444</v>
+      </c>
+      <c r="D19" s="7">
         <f t="shared" si="1"/>
-        <v>151500.55555555556</v>
-      </c>
-      <c r="E17" s="7">
+        <v>153500.55555555556</v>
+      </c>
+      <c r="E19" s="7">
         <f t="shared" si="1"/>
-        <v>132986.66666666666</v>
-      </c>
-      <c r="F17" s="7">
+        <v>134986.66666666666</v>
+      </c>
+      <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>114472.77777777778</v>
-      </c>
-      <c r="G17" s="7">
+        <v>116472.77777777778</v>
+      </c>
+      <c r="G19" s="7">
         <f t="shared" si="1"/>
-        <v>95958.888888888891</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B21" t="s">
-        <v>211</v>
-      </c>
+        <v>97958.888888888891</v>
+      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>210</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>215</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>219</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2610,7 +2643,7 @@
   <dimension ref="A4:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2618,18 +2651,18 @@
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H4" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="M4" s="12" t="s">
+      <c r="H4" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2661,27 +2694,27 @@
         <f>Gross!H30</f>
         <v>160</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="17">
         <f>Gross!I30</f>
         <v>214</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="18">
         <f>Gross!J30</f>
         <v>250</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="18">
         <f>Gross!K30</f>
         <v>300</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="14">
         <f>Gross!L30</f>
         <v>400</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="18">
         <f>Gross!M30</f>
         <v>500</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="19">
         <f>Gross!N30</f>
         <v>580</v>
       </c>
@@ -2714,27 +2747,27 @@
         <f>Gross!H45</f>
         <v>166400.00000000003</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="20">
         <f>Gross!I45</f>
         <v>222560.00000000006</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="21">
         <f>Gross!J45</f>
         <v>260000.00000000006</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="21">
         <f>Gross!K45</f>
         <v>312000.00000000006</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="15">
         <f>Gross!L45</f>
         <v>416000.00000000012</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="21">
         <f>Gross!M45</f>
         <v>520000.00000000012</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="22">
         <f>Gross!N45</f>
         <v>603200.00000000012</v>
       </c>
@@ -2776,27 +2809,27 @@
         <f t="shared" si="0"/>
         <v>-55766.666666666628</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="20">
         <f t="shared" si="0"/>
         <v>393.33333333340124</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="21">
         <f t="shared" si="0"/>
         <v>37833.333333333401</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="21">
         <f t="shared" si="0"/>
         <v>89833.333333333401</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="15">
         <f t="shared" si="0"/>
         <v>193833.33333333346</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="21">
         <f t="shared" si="0"/>
         <v>297833.33333333349</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="22">
         <f t="shared" ref="M10" si="1">M6-$B$8</f>
         <v>381033.33333333349</v>
       </c>
@@ -2838,7 +2871,7 @@
         <v>580</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -2856,7 +2889,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18">
         <f>B16-(0.2*710)</f>
@@ -2882,14 +2915,14 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22">
         <f>B20*(1+B21)</f>
         <v>112.00000000000003</v>
       </c>
       <c r="C22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -2920,7 +2953,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B28">
         <f>B26-B22</f>
@@ -2929,7 +2962,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B29">
         <f>C17-B28</f>
@@ -3121,7 +3154,7 @@
         <v>157</v>
       </c>
       <c r="D19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E19" t="s">
         <v>162</v>
@@ -3134,7 +3167,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
+      <c r="A20" s="16">
         <v>0.8</v>
       </c>
       <c r="B20">
@@ -3159,7 +3192,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
+      <c r="A21" s="16"/>
       <c r="B21">
         <v>0.2</v>
       </c>
@@ -3182,7 +3215,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
+      <c r="A22" s="16"/>
       <c r="B22">
         <v>0.8</v>
       </c>
@@ -3205,7 +3238,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
+      <c r="A23" s="16"/>
       <c r="B23">
         <v>0.8</v>
       </c>
@@ -3242,7 +3275,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
+      <c r="A25" s="16">
         <v>0.2</v>
       </c>
       <c r="B25" s="8">
@@ -3263,7 +3296,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="8">
         <v>0.2</v>
       </c>
@@ -4184,7 +4217,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B12" s="1">
         <f>C12/7</f>
@@ -4206,7 +4239,7 @@
         <v>60000</v>
       </c>
       <c r="H12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -4568,7 +4601,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B3" s="1">
         <v>50000</v>
@@ -4584,7 +4617,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="1">
         <v>25000</v>
@@ -4690,7 +4723,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -4751,7 +4784,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" s="1">
         <v>300</v>
@@ -4856,7 +4889,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D6" s="1">
         <v>3000</v>
@@ -4864,7 +4897,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D8" s="7">
         <f>D3+D6</f>

</xml_diff>

<commit_message>
looked into employee costs
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1824" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{571B69B0-BB1B-4B0D-8528-62A11DB95011}"/>
+  <xr:revisionPtr revIDLastSave="1828" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{13F8F6F8-F69B-41B3-805D-C363026AC50D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -908,15 +908,15 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -2355,7 +2355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAC8DE-41B9-46A0-BE44-EAAB92E58FB4}">
   <dimension ref="A3:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2522,27 +2522,27 @@
         <v>226</v>
       </c>
       <c r="B18" s="7">
-        <f>$B$15*B$17</f>
+        <f t="shared" ref="B18:G18" si="1">$B$15*B$17</f>
         <v>111083.33333333333</v>
       </c>
       <c r="C18" s="7">
-        <f>$B$15*C$17</f>
+        <f t="shared" si="1"/>
         <v>92569.444444444438</v>
       </c>
       <c r="D18" s="7">
-        <f>$B$15*D$17</f>
+        <f t="shared" si="1"/>
         <v>74055.555555555547</v>
       </c>
       <c r="E18" s="7">
-        <f>$B$15*E$17</f>
+        <f t="shared" si="1"/>
         <v>55541.666666666664</v>
       </c>
       <c r="F18" s="7">
-        <f>$B$15*F$17</f>
+        <f t="shared" si="1"/>
         <v>37027.777777777774</v>
       </c>
       <c r="G18" s="7">
-        <f>$B$15*G$17</f>
+        <f t="shared" si="1"/>
         <v>18513.888888888887</v>
       </c>
       <c r="H18" s="7"/>
@@ -2556,23 +2556,23 @@
         <v>190528.33333333331</v>
       </c>
       <c r="C19" s="7">
-        <f t="shared" ref="C19:G19" si="1">$B$10+($B$15*C$17)+$B$12+$B$11</f>
+        <f t="shared" ref="C19:G19" si="2">$B$10+($B$15*C$17)+$B$12+$B$11</f>
         <v>172014.44444444444</v>
       </c>
       <c r="D19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>153500.55555555556</v>
       </c>
       <c r="E19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134986.66666666666</v>
       </c>
       <c r="F19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116472.77777777778</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97958.888888888891</v>
       </c>
       <c r="H19" s="7"/>
@@ -2651,18 +2651,18 @@
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.109375" style="17" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="18" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2694,15 +2694,15 @@
         <f>Gross!H30</f>
         <v>160</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="16">
         <f>Gross!I30</f>
         <v>214</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="17">
         <f>Gross!J30</f>
         <v>250</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="17">
         <f>Gross!K30</f>
         <v>300</v>
       </c>
@@ -2710,11 +2710,11 @@
         <f>Gross!L30</f>
         <v>400</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="17">
         <f>Gross!M30</f>
         <v>500</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="18">
         <f>Gross!N30</f>
         <v>580</v>
       </c>
@@ -2747,15 +2747,15 @@
         <f>Gross!H45</f>
         <v>166400.00000000003</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="19">
         <f>Gross!I45</f>
         <v>222560.00000000006</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="20">
         <f>Gross!J45</f>
         <v>260000.00000000006</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="20">
         <f>Gross!K45</f>
         <v>312000.00000000006</v>
       </c>
@@ -2763,11 +2763,11 @@
         <f>Gross!L45</f>
         <v>416000.00000000012</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="20">
         <f>Gross!M45</f>
         <v>520000.00000000012</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="21">
         <f>Gross!N45</f>
         <v>603200.00000000012</v>
       </c>
@@ -2809,15 +2809,15 @@
         <f t="shared" si="0"/>
         <v>-55766.666666666628</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <f t="shared" si="0"/>
         <v>393.33333333340124</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <f t="shared" si="0"/>
         <v>37833.333333333401</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="20">
         <f t="shared" si="0"/>
         <v>89833.333333333401</v>
       </c>
@@ -2825,11 +2825,11 @@
         <f t="shared" si="0"/>
         <v>193833.33333333346</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="20">
         <f t="shared" si="0"/>
         <v>297833.33333333349</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="21">
         <f t="shared" ref="M10" si="1">M6-$B$8</f>
         <v>381033.33333333349</v>
       </c>
@@ -3167,7 +3167,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
+      <c r="A20" s="22">
         <v>0.8</v>
       </c>
       <c r="B20">
@@ -3192,7 +3192,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
+      <c r="A21" s="22"/>
       <c r="B21">
         <v>0.2</v>
       </c>
@@ -3215,7 +3215,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
+      <c r="A22" s="22"/>
       <c r="B22">
         <v>0.8</v>
       </c>
@@ -3238,7 +3238,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
+      <c r="A23" s="22"/>
       <c r="B23">
         <v>0.8</v>
       </c>
@@ -3275,7 +3275,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="16">
+      <c r="A25" s="22">
         <v>0.2</v>
       </c>
       <c r="B25" s="8">
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="8">
         <v>0.2</v>
       </c>
@@ -3985,10 +3985,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
-  <dimension ref="A3:H14"/>
+  <dimension ref="A3:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4001,7 +4001,7 @@
     <col min="6" max="6" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>98</v>
       </c>
@@ -4017,8 +4017,11 @@
       <c r="F3" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -4042,7 +4045,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -4067,7 +4070,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -4092,7 +4095,7 @@
         <v>2333.3333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -4117,7 +4120,7 @@
         <v>4666.666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>1166.6666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4167,7 +4170,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -4191,7 +4194,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4215,7 +4218,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -4242,7 +4245,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -4268,11 +4271,6 @@
       </c>
       <c r="H13" s="6">
         <v>5000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4584,8 +4582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
NDA, updated rent cost
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1828" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{13F8F6F8-F69B-41B3-805D-C363026AC50D}"/>
+  <xr:revisionPtr revIDLastSave="1902" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{C292F9C4-F4DD-4655-A607-82185010C9E2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="257">
   <si>
     <t>Overhead</t>
   </si>
@@ -199,18 +199,12 @@
     <t>Wifi</t>
   </si>
   <si>
-    <t>laminate countertops per square foot</t>
-  </si>
-  <si>
     <t>Electrical outlets</t>
   </si>
   <si>
     <t>sink installation and plumbing</t>
   </si>
   <si>
-    <t>premium refrigerator</t>
-  </si>
-  <si>
     <t>shared kitchen appliances</t>
   </si>
   <si>
@@ -791,6 +785,36 @@
   </si>
   <si>
     <t>Total Overhead Costs</t>
+  </si>
+  <si>
+    <t>granite countertops</t>
+  </si>
+  <si>
+    <t>Commercial Triple Door Fridge</t>
+  </si>
+  <si>
+    <t>knife sharpener</t>
+  </si>
+  <si>
+    <t>rent in downtown newhaven area</t>
+  </si>
+  <si>
+    <t>per year</t>
+  </si>
+  <si>
+    <t>per sq ft</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>per month</t>
+  </si>
+  <si>
+    <t>https://www.loopnet.com/Listing/57-Broadway-New-Haven-CT/18172597/</t>
+  </si>
+  <si>
+    <t>put it on broadway</t>
   </si>
 </sst>
 </file>
@@ -804,7 +828,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,8 +857,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -843,24 +881,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -868,30 +898,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -906,22 +923,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="6"/>
+    <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1237,7 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1249,48 +1264,48 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B4">
         <f>Net_And_Analysis!H5</f>
-        <v>214</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B6">
         <f>Net_And_Analysis!H5</f>
-        <v>214</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B7">
         <f>Net_And_Analysis!I5</f>
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B8">
         <f>Net_And_Analysis!J5</f>
-        <v>300</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B9">
         <f>Net_And_Analysis!K5</f>
@@ -1299,7 +1314,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B10">
         <f>Net_And_Analysis!L5</f>
@@ -1308,7 +1323,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B11">
         <f>Net_And_Analysis!M5</f>
@@ -1317,18 +1332,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C14">
         <v>2018</v>
@@ -1336,7 +1351,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B15">
         <v>58809</v>
@@ -1344,7 +1359,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B16">
         <v>56453</v>
@@ -1352,7 +1367,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B17">
         <v>58645</v>
@@ -1360,7 +1375,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B18">
         <v>49754</v>
@@ -1368,7 +1383,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B19">
         <v>50741</v>
@@ -1376,7 +1391,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B20">
         <v>54969</v>
@@ -1384,7 +1399,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B21">
         <v>59755</v>
@@ -1392,7 +1407,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B22">
         <v>59073</v>
@@ -1400,7 +1415,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B23">
         <v>60768</v>
@@ -1408,7 +1423,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B24">
         <v>45951</v>
@@ -1416,7 +1431,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B25">
         <v>37199</v>
@@ -1433,7 +1448,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B29" s="11">
         <v>25000</v>
@@ -1441,12 +1456,12 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B31" s="12">
         <f>B28+B29</f>
@@ -1455,7 +1470,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B32" s="11">
         <v>620000</v>
@@ -1463,16 +1478,16 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B34" s="13">
         <f>$B$4/$B$31</f>
-        <v>3.4677378843882116E-4</v>
+        <v>4.0510956593320228E-4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B35" s="13">
         <f>$B$11/$B$28</f>
@@ -1490,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560605D-AE6F-456E-B5FE-7223BF3283FD}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1512,27 +1527,27 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>247</v>
       </c>
       <c r="B2" s="1">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1549,12 +1564,12 @@
       </c>
       <c r="G2" s="7">
         <f>(PRODUCT(B2:D2) +E2)*F2</f>
-        <v>3825</v>
+        <v>4950</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B3" s="1">
         <v>700</v>
@@ -1569,7 +1584,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1">
         <v>300</v>
@@ -1584,7 +1599,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
@@ -1593,13 +1608,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G15" si="0">B5*C5</f>
+        <f t="shared" ref="G5:G16" si="0">B5*C5</f>
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1">
         <v>500</v>
@@ -1614,22 +1629,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B7" s="1">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>2400</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B8" s="1">
         <v>8000</v>
@@ -1644,10 +1659,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B9" s="1">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="C9">
         <f>C7</f>
@@ -1655,28 +1670,27 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>1400</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
       <c r="B10" s="1">
-        <v>900</v>
+        <v>3900</v>
       </c>
       <c r="C10">
-        <f>$F$2</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>2700</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1">
         <v>1000</v>
@@ -1691,7 +1705,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1706,7 +1720,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1">
         <v>100</v>
@@ -1721,7 +1735,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1">
         <v>250</v>
@@ -1736,7 +1750,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1">
         <v>80</v>
@@ -1749,13 +1763,28 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="1">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="7">
-        <f>SUM(G2:G15)</f>
-        <v>27115</v>
+      <c r="G18" s="7">
+        <f>SUM(G2:G16)</f>
+        <v>39740</v>
       </c>
     </row>
   </sheetData>
@@ -1778,12 +1807,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
@@ -1791,7 +1820,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
@@ -1829,16 +1858,16 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>43</v>
@@ -1846,7 +1875,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <f>D3</f>
@@ -1869,7 +1898,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1891,7 +1920,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1913,7 +1942,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1971,31 +2000,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>43</v>
@@ -2003,7 +2032,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -2043,7 +2072,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K3" s="1">
         <v>400</v>
@@ -2051,7 +2080,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K4" s="1">
         <v>200</v>
@@ -2356,7 +2385,7 @@
   <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2370,7 +2399,7 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B3" s="7">
         <f>Gaming!D12</f>
@@ -2379,7 +2408,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="7">
         <f>Dance_Studio!D8</f>
@@ -2388,16 +2417,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="7">
-        <f>Kitchen!G17</f>
-        <v>27115</v>
+        <f>Kitchen!G18</f>
+        <v>39740</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="7">
         <f>Liabilities!B7</f>
@@ -2406,7 +2435,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="7">
         <f>decor!K7</f>
@@ -2415,7 +2444,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B8" s="7">
         <f>'Eating Area'!F10</f>
@@ -2424,16 +2453,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" s="7">
         <f>SUM(B3:B8)</f>
-        <v>67445</v>
+        <v>80070</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B11" s="6">
         <v>2000</v>
@@ -2441,7 +2470,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B12" s="1">
         <v>10000</v>
@@ -2449,25 +2478,25 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B13" s="7">
         <f>SUM(B10:B12)</f>
-        <v>79445</v>
+        <v>92070</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" s="7">
         <f>Operating_Costs!F13</f>
-        <v>222166.66666666666</v>
+        <v>378166.66666666663</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -2490,7 +2519,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B17">
         <f>B16/12</f>
@@ -2519,118 +2548,118 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B18" s="7">
         <f t="shared" ref="B18:G18" si="1">$B$15*B$17</f>
-        <v>111083.33333333333</v>
+        <v>189083.33333333331</v>
       </c>
       <c r="C18" s="7">
         <f t="shared" si="1"/>
-        <v>92569.444444444438</v>
+        <v>157569.44444444444</v>
       </c>
       <c r="D18" s="7">
         <f t="shared" si="1"/>
-        <v>74055.555555555547</v>
+        <v>126055.55555555553</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="1"/>
-        <v>55541.666666666664</v>
+        <v>94541.666666666657</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>37027.777777777774</v>
+        <v>63027.777777777766</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="1"/>
-        <v>18513.888888888887</v>
+        <v>31513.888888888883</v>
       </c>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" s="7">
         <f>$B$10+($B$15*B$17)+$B$12+$B$11</f>
-        <v>190528.33333333331</v>
+        <v>281153.33333333331</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:G19" si="2">$B$10+($B$15*C$17)+$B$12+$B$11</f>
-        <v>172014.44444444444</v>
+        <v>249639.44444444444</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="2"/>
-        <v>153500.55555555556</v>
+        <v>218125.55555555553</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="2"/>
-        <v>134986.66666666666</v>
+        <v>186611.66666666666</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="2"/>
-        <v>116472.77777777778</v>
+        <v>155097.77777777775</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="2"/>
-        <v>97958.888888888891</v>
+        <v>123583.88888888888</v>
       </c>
       <c r="H19" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2643,27 +2672,27 @@
   <dimension ref="A4:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H4" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>178</v>
+      <c r="J4" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2694,34 +2723,34 @@
         <f>Gross!H30</f>
         <v>160</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5">
         <f>Gross!I30</f>
-        <v>214</v>
-      </c>
-      <c r="I5" s="17">
+        <v>250</v>
+      </c>
+      <c r="I5">
         <f>Gross!J30</f>
-        <v>250</v>
-      </c>
-      <c r="J5" s="17">
+        <v>300</v>
+      </c>
+      <c r="J5" s="16">
         <f>Gross!K30</f>
-        <v>300</v>
-      </c>
-      <c r="K5" s="14">
+        <v>365</v>
+      </c>
+      <c r="K5">
         <f>Gross!L30</f>
         <v>400</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5">
         <f>Gross!M30</f>
         <v>500</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="15">
         <f>Gross!N30</f>
         <v>580</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B6" s="7">
         <f>Gross!C45</f>
@@ -2747,136 +2776,136 @@
         <f>Gross!H45</f>
         <v>166400.00000000003</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6">
         <f>Gross!I45</f>
-        <v>222560.00000000006</v>
-      </c>
-      <c r="I6" s="20">
+        <v>260000.00000000006</v>
+      </c>
+      <c r="I6">
         <f>Gross!J45</f>
-        <v>260000.00000000006</v>
-      </c>
-      <c r="J6" s="20">
+        <v>312000.00000000006</v>
+      </c>
+      <c r="J6" s="16">
         <f>Gross!K45</f>
-        <v>312000.00000000006</v>
-      </c>
-      <c r="K6" s="15">
+        <v>379600.00000000006</v>
+      </c>
+      <c r="K6">
         <f>Gross!L45</f>
         <v>416000.00000000012</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6">
         <f>Gross!M45</f>
         <v>520000.00000000012</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="15">
         <f>Gross!N45</f>
         <v>603200.00000000012</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" s="7">
         <f>Operating_Costs!F13</f>
-        <v>222166.66666666666</v>
+        <v>378166.66666666663</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B10" s="7">
         <f>B6-$B$8</f>
-        <v>-216966.66666666666</v>
+        <v>-372966.66666666663</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:L10" si="0">C6-$B$8</f>
-        <v>-211766.66666666666</v>
+        <v>-367766.66666666663</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>-201366.66666666666</v>
+        <v>-357366.66666666663</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>-180566.66666666666</v>
+        <v>-336566.66666666663</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
-        <v>-138966.66666666663</v>
+        <v>-294966.66666666663</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>-55766.666666666628</v>
-      </c>
-      <c r="H10" s="19">
+        <v>-211766.6666666666</v>
+      </c>
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
-        <v>393.33333333340124</v>
-      </c>
-      <c r="I10" s="20">
+        <v>-118166.66666666657</v>
+      </c>
+      <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>37833.333333333401</v>
-      </c>
-      <c r="J10" s="20">
+        <v>-66166.66666666657</v>
+      </c>
+      <c r="J10" s="17">
         <f t="shared" si="0"/>
-        <v>89833.333333333401</v>
-      </c>
-      <c r="K10" s="15">
+        <v>1433.3333333334303</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="0"/>
-        <v>193833.33333333346</v>
-      </c>
-      <c r="L10" s="20">
+        <v>37833.333333333489</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>297833.33333333349</v>
-      </c>
-      <c r="M10" s="21">
+        <v>141833.33333333349</v>
+      </c>
+      <c r="M10" s="18">
         <f t="shared" ref="M10" si="1">M6-$B$8</f>
-        <v>381033.33333333349</v>
+        <v>225033.33333333349</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <f>H5</f>
-        <v>214</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B13">
         <f>Gross!I37</f>
-        <v>34.240000000000009</v>
+        <v>40.000000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B16">
         <f>M5</f>
         <v>580</v>
       </c>
       <c r="C16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B17">
         <f>B16*0.2</f>
@@ -2889,7 +2918,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B18">
         <f>B16-(0.2*710)</f>
@@ -2898,7 +2927,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B20">
         <f>Gross!L37</f>
@@ -2907,7 +2936,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B21" s="9">
         <v>0.75</v>
@@ -2915,19 +2944,19 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B22">
         <f>B20*(1+B21)</f>
         <v>112.00000000000003</v>
       </c>
       <c r="C22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B24">
         <f>Gross!B7</f>
@@ -2936,7 +2965,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2944,7 +2973,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B26">
         <f>B24*B25</f>
@@ -2953,7 +2982,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B28">
         <f>B26-B22</f>
@@ -2962,7 +2991,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B29">
         <f>C17-B28</f>
@@ -2978,8 +3007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7959888-B526-4FAC-9FC1-7A03020906F6}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2998,36 +3027,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <f>10</f>
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3" s="9">
         <v>0.2</v>
@@ -3036,13 +3065,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F4" s="9">
         <v>0.8</v>
@@ -3050,7 +3079,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -3067,22 +3096,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12" s="9">
         <v>0.2</v>
@@ -3093,7 +3122,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B13" s="1">
         <v>40</v>
@@ -3107,7 +3136,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
@@ -3121,7 +3150,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B15" s="1">
         <v>20</v>
@@ -3145,36 +3174,36 @@
     <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" t="s">
         <v>161</v>
       </c>
-      <c r="B19" t="s">
-        <v>163</v>
-      </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="A20" s="14">
         <v>0.8</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D20" s="8">
         <v>0.8</v>
@@ -3192,12 +3221,12 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
+      <c r="A21" s="14"/>
       <c r="B21">
         <v>0.2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D21" s="8">
         <v>0.2</v>
@@ -3215,12 +3244,12 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
+      <c r="A22" s="14"/>
       <c r="B22">
         <v>0.8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D22" s="8">
         <v>0.8</v>
@@ -3238,12 +3267,12 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
+      <c r="A23" s="14"/>
       <c r="B23">
         <v>0.8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D23" s="8">
         <v>0.2</v>
@@ -3275,17 +3304,17 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="22">
+      <c r="A25" s="14">
         <v>0.2</v>
       </c>
       <c r="B25" s="8">
         <v>0.8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E25" s="3">
         <f>$A$25*$B25</f>
@@ -3296,15 +3325,15 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="8">
         <v>0.2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E26" s="3">
         <f>$A$25*$B26</f>
@@ -3328,16 +3357,16 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -3358,13 +3387,13 @@
         <v>160</v>
       </c>
       <c r="I30">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="J30">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="K30">
-        <v>300</v>
+        <v>365</v>
       </c>
       <c r="L30">
         <v>400</v>
@@ -3378,7 +3407,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
@@ -3408,23 +3437,23 @@
         <v>409.60000000000008</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" ref="I31" si="3">$E20*$F20*$B31*I$30</f>
-        <v>547.84000000000015</v>
+        <f>$E20*$F20*$B31*I$30</f>
+        <v>640.00000000000011</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" ref="J31:M34" si="4">$E20*$F20*$B31*J$30</f>
-        <v>640.00000000000011</v>
+        <f>$E20*$F20*$B31*J$30</f>
+        <v>768.00000000000011</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="4"/>
-        <v>768.00000000000011</v>
+        <f>$E20*$F20*$B31*K$30</f>
+        <v>934.4000000000002</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="4"/>
+        <f>$E20*$F20*$B31*L$30</f>
         <v>1024.0000000000002</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="4"/>
+        <f>$E20*$F20*$B31*M$30</f>
         <v>1280.0000000000002</v>
       </c>
       <c r="N31" s="1">
@@ -3434,175 +3463,175 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B32" s="1">
         <v>10</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" ref="C32:H34" si="5">$E21*$F21*$B32*C$30</f>
+        <f t="shared" ref="C32:H34" si="3">$E21*$F21*$B32*C$30</f>
         <v>4.8000000000000016</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>9.6000000000000032</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>19.200000000000006</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>38.400000000000013</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>76.800000000000026</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>153.60000000000005</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" ref="I32" si="6">$E21*$F21*$B32*I$30</f>
-        <v>205.44000000000005</v>
+        <f>$E21*$F21*$B32*I$30</f>
+        <v>240.00000000000009</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="4"/>
-        <v>240.00000000000009</v>
+        <f>$E21*$F21*$B32*J$30</f>
+        <v>288.00000000000011</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="4"/>
-        <v>288.00000000000011</v>
+        <f>$E21*$F21*$B32*K$30</f>
+        <v>350.40000000000009</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="4"/>
+        <f>$E21*$F21*$B32*L$30</f>
         <v>384.00000000000011</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="4"/>
+        <f>$E21*$F21*$B32*M$30</f>
         <v>480.00000000000017</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" ref="N32" si="7">$E21*$F21*$B32*N$30</f>
+        <f>$E21*$F21*$B32*N$30</f>
         <v>556.80000000000018</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B33" s="1">
         <v>20</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>51.20000000000001</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>102.40000000000002</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>204.80000000000004</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>409.60000000000008</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>819.20000000000016</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1638.4000000000003</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" ref="I33" si="8">$E22*$F22*$B33*I$30</f>
-        <v>2191.3600000000006</v>
+        <f>$E22*$F22*$B33*I$30</f>
+        <v>2560.0000000000005</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="4"/>
-        <v>2560.0000000000005</v>
+        <f>$E22*$F22*$B33*J$30</f>
+        <v>3072.0000000000005</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="4"/>
-        <v>3072.0000000000005</v>
+        <f>$E22*$F22*$B33*K$30</f>
+        <v>3737.6000000000008</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="4"/>
+        <f>$E22*$F22*$B33*L$30</f>
         <v>4096.0000000000009</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="4"/>
+        <f>$E22*$F22*$B33*M$30</f>
         <v>5120.0000000000009</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" ref="N33" si="9">$E22*$F22*$B33*N$30</f>
+        <f>$E22*$F22*$B33*N$30</f>
         <v>5939.2000000000007</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B34" s="1">
         <v>20</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>25.600000000000005</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>51.20000000000001</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>102.40000000000002</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>204.80000000000004</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>409.60000000000008</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>819.20000000000016</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" ref="I34" si="10">$E23*$F23*$B34*I$30</f>
-        <v>1095.6800000000003</v>
+        <f>$E23*$F23*$B34*I$30</f>
+        <v>1280.0000000000002</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="4"/>
-        <v>1280.0000000000002</v>
+        <f>$E23*$F23*$B34*J$30</f>
+        <v>1536.0000000000002</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="4"/>
-        <v>1536.0000000000002</v>
+        <f>$E23*$F23*$B34*K$30</f>
+        <v>1868.8000000000004</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="4"/>
+        <f>$E23*$F23*$B34*L$30</f>
         <v>2048.0000000000005</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="4"/>
+        <f>$E23*$F23*$B34*M$30</f>
         <v>2560.0000000000005</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" ref="N34" si="11">$E23*$F23*$B34*N$30</f>
+        <f>$E23*$F23*$B34*N$30</f>
         <v>2969.6000000000004</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C35" s="7">
         <f>SUM(C31:C34)</f>
@@ -3613,32 +3642,32 @@
         <v>188.80000000000004</v>
       </c>
       <c r="E35" s="7">
-        <f t="shared" ref="E35:I35" si="12">SUM(E31:E34)</f>
+        <f t="shared" ref="E35:I35" si="4">SUM(E31:E34)</f>
         <v>377.60000000000008</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>755.20000000000016</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>1510.4000000000003</v>
       </c>
       <c r="H35" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>3020.8000000000006</v>
       </c>
       <c r="I35" s="7">
-        <f t="shared" si="12"/>
-        <v>4040.3200000000011</v>
+        <f t="shared" si="4"/>
+        <v>4720.0000000000009</v>
       </c>
       <c r="J35" s="7">
         <f>SUM(J31:J34)</f>
-        <v>4720.0000000000009</v>
+        <v>5664.0000000000009</v>
       </c>
       <c r="K35" s="7">
         <f>SUM(K31:K34)</f>
-        <v>5664.0000000000009</v>
+        <v>6891.2000000000016</v>
       </c>
       <c r="L35" s="7">
         <f>SUM(L31:L34)</f>
@@ -3655,43 +3684,43 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C36" s="3">
         <f>C$30*($G$24)</f>
         <v>5.6000000000000014</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" ref="D36:I36" si="13">D$30*($G$24)</f>
+        <f t="shared" ref="D36:H36" si="5">D$30*($G$24)</f>
         <v>11.200000000000003</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>22.400000000000006</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>44.800000000000011</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>89.600000000000023</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>179.20000000000005</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="13"/>
-        <v>239.68000000000006</v>
+        <f>I$30*($G$24)</f>
+        <v>280.00000000000006</v>
       </c>
       <c r="J36" s="3">
         <f>J$30*($G$24)</f>
-        <v>280.00000000000006</v>
+        <v>336.00000000000011</v>
       </c>
       <c r="K36" s="3">
         <f>K$30*($G$24)</f>
-        <v>336.00000000000011</v>
+        <v>408.80000000000013</v>
       </c>
       <c r="L36" s="3">
         <f>L$30*($G$24)</f>
@@ -3708,43 +3737,43 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C37">
         <f>C36/7</f>
         <v>0.80000000000000016</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:I37" si="14">D36/7</f>
+        <f t="shared" ref="D37:I37" si="6">D36/7</f>
         <v>1.6000000000000003</v>
       </c>
       <c r="E37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>3.2000000000000006</v>
       </c>
       <c r="F37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>6.4000000000000012</v>
       </c>
       <c r="G37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>12.800000000000002</v>
       </c>
       <c r="H37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>25.600000000000005</v>
       </c>
       <c r="I37">
-        <f t="shared" si="14"/>
-        <v>34.240000000000009</v>
+        <f t="shared" si="6"/>
+        <v>40.000000000000007</v>
       </c>
       <c r="J37">
         <f>J36/7</f>
-        <v>40.000000000000007</v>
+        <v>48.000000000000014</v>
       </c>
       <c r="K37">
         <f>K36/7</f>
-        <v>48.000000000000014</v>
+        <v>58.40000000000002</v>
       </c>
       <c r="L37">
         <f>L36/7</f>
@@ -3761,152 +3790,152 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" ref="C41:M41" si="15">C35*50</f>
+        <f t="shared" ref="C41:M41" si="7">C35*50</f>
         <v>4720.0000000000009</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>9440.0000000000018</v>
       </c>
       <c r="E41" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>18880.000000000004</v>
       </c>
       <c r="F41" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>37760.000000000007</v>
       </c>
       <c r="G41" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>75520.000000000015</v>
       </c>
       <c r="H41" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>151040.00000000003</v>
       </c>
       <c r="I41" s="7">
-        <f t="shared" si="15"/>
-        <v>202016.00000000006</v>
+        <f t="shared" si="7"/>
+        <v>236000.00000000006</v>
       </c>
       <c r="J41" s="7">
-        <f t="shared" si="15"/>
-        <v>236000.00000000006</v>
+        <f t="shared" si="7"/>
+        <v>283200.00000000006</v>
       </c>
       <c r="K41" s="7">
-        <f t="shared" si="15"/>
-        <v>283200.00000000006</v>
+        <f t="shared" si="7"/>
+        <v>344560.00000000006</v>
       </c>
       <c r="L41" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>377600.00000000012</v>
       </c>
       <c r="M41" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>472000.00000000012</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" ref="N41" si="16">N35*50</f>
+        <f t="shared" ref="N41" si="8">N35*50</f>
         <v>547520.00000000012</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B42" s="1">
         <v>40</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" ref="C42:N42" si="17">C$30*$B42*$A$25</f>
+        <f t="shared" ref="C42:H42" si="9">C$30*$B42*$A$25</f>
         <v>40</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="9"/>
         <v>160</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="9"/>
         <v>320</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="9"/>
         <v>640</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="9"/>
         <v>1280</v>
       </c>
       <c r="I42" s="7">
-        <f t="shared" si="17"/>
-        <v>1712</v>
+        <f>I$30*$B42*$A$25</f>
+        <v>2000</v>
       </c>
       <c r="J42" s="7">
-        <f t="shared" si="17"/>
-        <v>2000</v>
+        <f>J$30*$B42*$A$25</f>
+        <v>2400</v>
       </c>
       <c r="K42" s="7">
-        <f t="shared" si="17"/>
-        <v>2400</v>
+        <f>K$30*$B42*$A$25</f>
+        <v>2920</v>
       </c>
       <c r="L42" s="7">
-        <f t="shared" si="17"/>
+        <f>L$30*$B42*$A$25</f>
         <v>3200</v>
       </c>
       <c r="M42" s="7">
-        <f t="shared" si="17"/>
+        <f>M$30*$B42*$A$25</f>
         <v>4000</v>
       </c>
       <c r="N42" s="7">
-        <f t="shared" si="17"/>
+        <f>N$30*$B42*$A$25</f>
         <v>4640</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C43" s="7">
         <f>C42*12</f>
         <v>480</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" ref="D43:I43" si="18">D42*12</f>
+        <f t="shared" ref="D43:I43" si="10">D42*12</f>
         <v>960</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>1920</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>3840</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>7680</v>
       </c>
       <c r="H43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="10"/>
         <v>15360</v>
       </c>
       <c r="I43" s="7">
-        <f t="shared" si="18"/>
-        <v>20544</v>
+        <f t="shared" si="10"/>
+        <v>24000</v>
       </c>
       <c r="J43" s="7">
         <f>J42*12</f>
-        <v>24000</v>
+        <v>28800</v>
       </c>
       <c r="K43" s="7">
         <f>K42*12</f>
-        <v>28800</v>
+        <v>35040</v>
       </c>
       <c r="L43" s="7">
         <f>L42*12</f>
@@ -3923,54 +3952,54 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" ref="C45:M45" si="19">C43+C41</f>
+        <f t="shared" ref="C45:M45" si="11">C43+C41</f>
         <v>5200.0000000000009</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>10400.000000000002</v>
       </c>
       <c r="E45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>20800.000000000004</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>41600.000000000007</v>
       </c>
       <c r="G45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>83200.000000000015</v>
       </c>
       <c r="H45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>166400.00000000003</v>
       </c>
       <c r="I45" s="7">
-        <f t="shared" si="19"/>
-        <v>222560.00000000006</v>
+        <f t="shared" si="11"/>
+        <v>260000.00000000006</v>
       </c>
       <c r="J45" s="7">
-        <f t="shared" si="19"/>
-        <v>260000.00000000006</v>
+        <f t="shared" si="11"/>
+        <v>312000.00000000006</v>
       </c>
       <c r="K45" s="7">
-        <f t="shared" si="19"/>
-        <v>312000.00000000006</v>
+        <f t="shared" si="11"/>
+        <v>379600.00000000006</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>416000.00000000012</v>
       </c>
       <c r="M45" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="11"/>
         <v>520000.00000000012</v>
       </c>
       <c r="N45" s="7">
-        <f t="shared" ref="N45" si="20">N43+N41</f>
+        <f t="shared" ref="N45" si="12">N43+N41</f>
         <v>603200.00000000012</v>
       </c>
     </row>
@@ -3985,15 +4014,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
-  <dimension ref="A3:J13"/>
+  <dimension ref="A3:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -4003,27 +4032,27 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1">
         <f>C4/7</f>
@@ -4047,7 +4076,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1">
         <f>C5/7</f>
@@ -4072,7 +4101,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1">
         <f>200/30</f>
@@ -4097,7 +4126,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1">
         <f>400/30</f>
@@ -4122,7 +4151,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1">
         <f>100/30</f>
@@ -4147,7 +4176,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1">
         <f>C9/7</f>
@@ -4172,7 +4201,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" s="1">
         <f>C10/7</f>
@@ -4196,7 +4225,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" s="1">
         <f>C11/7</f>
@@ -4220,29 +4249,30 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B12" s="1">
         <f>C12/7</f>
-        <v>164.83516483516482</v>
+        <v>593.40659340659352</v>
       </c>
       <c r="C12" s="1">
         <f>F12/52</f>
-        <v>1153.8461538461538</v>
+        <v>4153.8461538461543</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>2307.6923076923076</v>
+        <v>8307.6923076923085</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>4615.3846153846152</v>
+        <v>16615.384615384617</v>
       </c>
       <c r="F12" s="1">
-        <v>60000</v>
+        <f>H13*12</f>
+        <v>216000</v>
       </c>
       <c r="H12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -4251,29 +4281,105 @@
       </c>
       <c r="B13" s="1">
         <f>SUM(B4:B12)</f>
-        <v>614.32234432234429</v>
+        <v>1042.8937728937731</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:F13" si="1">SUM(C4:C12)</f>
-        <v>4300.2564102564102</v>
+        <v>7300.2564102564111</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>10754.358974358973</v>
+        <v>16754.358974358976</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>21508.717948717946</v>
+        <v>33508.717948717953</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>222166.66666666666</v>
+        <v>378166.66666666663</v>
       </c>
       <c r="H13" s="6">
-        <v>5000</v>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C23" s="1">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E23" s="1">
+        <f>C23*D23</f>
+        <v>220000</v>
+      </c>
+      <c r="F23" s="1">
+        <f>E23/12</f>
+        <v>18333.333333333332</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>254</v>
+      </c>
+      <c r="C24" s="1">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E24" s="1">
+        <f>C24*D24</f>
+        <v>170000</v>
+      </c>
+      <c r="F24" s="1">
+        <f>E24/12</f>
+        <v>14166.666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="1">
+        <v>15000</v>
+      </c>
+      <c r="F27" s="1">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A26" r:id="rId1" xr:uid="{F79E9E73-FE81-49C9-AD29-E42F9F967839}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4301,21 +4407,21 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
         <v>106</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>107</v>
-      </c>
-      <c r="E1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -4339,7 +4445,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -4363,7 +4469,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -4387,7 +4493,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="4">
         <v>0.15</v>
@@ -4411,7 +4517,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4">
         <v>0.1</v>
@@ -4435,7 +4541,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4">
         <v>0.05</v>
@@ -4468,7 +4574,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -4488,7 +4594,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B12" s="1">
         <v>7.5</v>
@@ -4512,7 +4618,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -4520,7 +4626,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -4528,7 +4634,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B16" s="7">
         <f>B12*B15</f>
@@ -4537,7 +4643,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B17" s="7">
         <f>B14*B16</f>
@@ -4546,7 +4652,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="9">
         <v>0.2</v>
@@ -4554,7 +4660,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" s="7">
         <f>B17*(B18+1)</f>
@@ -4569,7 +4675,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B22" s="7"/>
     </row>
@@ -4582,8 +4688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4599,7 +4705,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B3" s="1">
         <v>50000</v>
@@ -4607,7 +4713,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1">
         <v>45000</v>
@@ -4615,7 +4721,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B5" s="1">
         <v>25000</v>
@@ -4632,7 +4738,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1">
         <f>B6/52</f>
@@ -4641,7 +4747,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="1">
         <f>B6/26</f>
@@ -4650,7 +4756,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" s="1">
         <f>B10*2</f>
@@ -4721,7 +4827,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -4782,7 +4888,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B8" s="1">
         <v>300</v>
@@ -4879,7 +4985,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1">
         <v>5000</v>
@@ -4887,7 +4993,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D6" s="1">
         <v>3000</v>
@@ -4895,7 +5001,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D8" s="7">
         <f>D3+D6</f>

</xml_diff>

<commit_message>
trying to fix branches
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1902" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{C292F9C4-F4DD-4655-A607-82185010C9E2}"/>
+  <xr:revisionPtr revIDLastSave="1828" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{13F8F6F8-F69B-41B3-805D-C363026AC50D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="249">
   <si>
     <t>Overhead</t>
   </si>
@@ -199,12 +199,18 @@
     <t>Wifi</t>
   </si>
   <si>
+    <t>laminate countertops per square foot</t>
+  </si>
+  <si>
     <t>Electrical outlets</t>
   </si>
   <si>
     <t>sink installation and plumbing</t>
   </si>
   <si>
+    <t>premium refrigerator</t>
+  </si>
+  <si>
     <t>shared kitchen appliances</t>
   </si>
   <si>
@@ -785,36 +791,6 @@
   </si>
   <si>
     <t>Total Overhead Costs</t>
-  </si>
-  <si>
-    <t>granite countertops</t>
-  </si>
-  <si>
-    <t>Commercial Triple Door Fridge</t>
-  </si>
-  <si>
-    <t>knife sharpener</t>
-  </si>
-  <si>
-    <t>rent in downtown newhaven area</t>
-  </si>
-  <si>
-    <t>per year</t>
-  </si>
-  <si>
-    <t>per sq ft</t>
-  </si>
-  <si>
-    <t>needed</t>
-  </si>
-  <si>
-    <t>per month</t>
-  </si>
-  <si>
-    <t>https://www.loopnet.com/Listing/57-Broadway-New-Haven-CT/18172597/</t>
-  </si>
-  <si>
-    <t>put it on broadway</t>
   </si>
 </sst>
 </file>
@@ -828,7 +804,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,22 +833,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -881,16 +843,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -898,17 +868,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -923,20 +906,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="6"/>
-    <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1252,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1264,48 +1249,48 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B4">
         <f>Net_And_Analysis!H5</f>
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <f>Net_And_Analysis!H5</f>
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B7">
         <f>Net_And_Analysis!I5</f>
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B8">
         <f>Net_And_Analysis!J5</f>
-        <v>365</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B9">
         <f>Net_And_Analysis!K5</f>
@@ -1314,7 +1299,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B10">
         <f>Net_And_Analysis!L5</f>
@@ -1323,7 +1308,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B11">
         <f>Net_And_Analysis!M5</f>
@@ -1332,18 +1317,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C14">
         <v>2018</v>
@@ -1351,7 +1336,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B15">
         <v>58809</v>
@@ -1359,7 +1344,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B16">
         <v>56453</v>
@@ -1367,7 +1352,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B17">
         <v>58645</v>
@@ -1375,7 +1360,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B18">
         <v>49754</v>
@@ -1383,7 +1368,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B19">
         <v>50741</v>
@@ -1391,7 +1376,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B20">
         <v>54969</v>
@@ -1399,7 +1384,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B21">
         <v>59755</v>
@@ -1407,7 +1392,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B22">
         <v>59073</v>
@@ -1415,7 +1400,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B23">
         <v>60768</v>
@@ -1423,7 +1408,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B24">
         <v>45951</v>
@@ -1431,7 +1416,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B25">
         <v>37199</v>
@@ -1448,7 +1433,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B29" s="11">
         <v>25000</v>
@@ -1456,12 +1441,12 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B31" s="12">
         <f>B28+B29</f>
@@ -1470,7 +1455,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B32" s="11">
         <v>620000</v>
@@ -1478,16 +1463,16 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B34" s="13">
         <f>$B$4/$B$31</f>
-        <v>4.0510956593320228E-4</v>
+        <v>3.4677378843882116E-4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B35" s="13">
         <f>$B$11/$B$28</f>
@@ -1505,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560605D-AE6F-456E-B5FE-7223BF3283FD}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,27 +1512,27 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>247</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1564,12 +1549,12 @@
       </c>
       <c r="G2" s="7">
         <f>(PRODUCT(B2:D2) +E2)*F2</f>
-        <v>4950</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B3" s="1">
         <v>700</v>
@@ -1584,7 +1569,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1">
         <v>300</v>
@@ -1599,7 +1584,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
@@ -1608,13 +1593,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G16" si="0">B5*C5</f>
+        <f t="shared" ref="G5:G15" si="0">B5*C5</f>
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1">
         <v>500</v>
@@ -1629,22 +1614,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B7" s="1">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B8" s="1">
         <v>8000</v>
@@ -1659,10 +1644,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B9" s="1">
-        <v>2500</v>
+        <v>350</v>
       </c>
       <c r="C9">
         <f>C7</f>
@@ -1670,27 +1655,28 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>248</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1">
-        <v>3900</v>
+        <v>900</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <f>$F$2</f>
+        <v>3</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>3900</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1">
         <v>1000</v>
@@ -1705,7 +1691,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1720,7 +1706,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1">
         <v>100</v>
@@ -1735,7 +1721,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1">
         <v>250</v>
@@ -1750,7 +1736,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1">
         <v>80</v>
@@ -1763,28 +1749,13 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>249</v>
-      </c>
-      <c r="B16" s="1">
-        <v>100</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="7">
-        <f>SUM(G2:G16)</f>
-        <v>39740</v>
+      <c r="G17" s="7">
+        <f>SUM(G2:G15)</f>
+        <v>27115</v>
       </c>
     </row>
   </sheetData>
@@ -1807,12 +1778,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
@@ -1820,7 +1791,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
@@ -1858,16 +1829,16 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>43</v>
@@ -1875,7 +1846,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <f>D3</f>
@@ -1898,7 +1869,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1920,7 +1891,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1942,7 +1913,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -2000,31 +1971,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>43</v>
@@ -2032,7 +2003,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -2072,7 +2043,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1">
         <v>400</v>
@@ -2080,7 +2051,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K4" s="1">
         <v>200</v>
@@ -2385,7 +2356,7 @@
   <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2399,7 +2370,7 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B3" s="7">
         <f>Gaming!D12</f>
@@ -2408,7 +2379,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B4" s="7">
         <f>Dance_Studio!D8</f>
@@ -2417,16 +2388,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B5" s="7">
-        <f>Kitchen!G18</f>
-        <v>39740</v>
+        <f>Kitchen!G17</f>
+        <v>27115</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B6" s="7">
         <f>Liabilities!B7</f>
@@ -2435,7 +2406,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B7" s="7">
         <f>decor!K7</f>
@@ -2444,7 +2415,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B8" s="7">
         <f>'Eating Area'!F10</f>
@@ -2453,16 +2424,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B10" s="7">
         <f>SUM(B3:B8)</f>
-        <v>80070</v>
+        <v>67445</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B11" s="6">
         <v>2000</v>
@@ -2470,7 +2441,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B12" s="1">
         <v>10000</v>
@@ -2478,25 +2449,25 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B13" s="7">
         <f>SUM(B10:B12)</f>
-        <v>92070</v>
+        <v>79445</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B15" s="7">
         <f>Operating_Costs!F13</f>
-        <v>378166.66666666663</v>
+        <v>222166.66666666666</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -2519,7 +2490,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B17">
         <f>B16/12</f>
@@ -2548,118 +2519,118 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B18" s="7">
         <f t="shared" ref="B18:G18" si="1">$B$15*B$17</f>
-        <v>189083.33333333331</v>
+        <v>111083.33333333333</v>
       </c>
       <c r="C18" s="7">
         <f t="shared" si="1"/>
-        <v>157569.44444444444</v>
+        <v>92569.444444444438</v>
       </c>
       <c r="D18" s="7">
         <f t="shared" si="1"/>
-        <v>126055.55555555553</v>
+        <v>74055.555555555547</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="1"/>
-        <v>94541.666666666657</v>
+        <v>55541.666666666664</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>63027.777777777766</v>
+        <v>37027.777777777774</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="1"/>
-        <v>31513.888888888883</v>
+        <v>18513.888888888887</v>
       </c>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B19" s="7">
         <f>$B$10+($B$15*B$17)+$B$12+$B$11</f>
-        <v>281153.33333333331</v>
+        <v>190528.33333333331</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:G19" si="2">$B$10+($B$15*C$17)+$B$12+$B$11</f>
-        <v>249639.44444444444</v>
+        <v>172014.44444444444</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="2"/>
-        <v>218125.55555555553</v>
+        <v>153500.55555555556</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="2"/>
-        <v>186611.66666666666</v>
+        <v>134986.66666666666</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="2"/>
-        <v>155097.77777777775</v>
+        <v>116472.77777777778</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="2"/>
-        <v>123583.88888888888</v>
+        <v>97958.888888888891</v>
       </c>
       <c r="H19" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2672,27 +2643,27 @@
   <dimension ref="A4:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J4" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>176</v>
+      <c r="H4" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2723,34 +2694,34 @@
         <f>Gross!H30</f>
         <v>160</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="16">
         <f>Gross!I30</f>
+        <v>214</v>
+      </c>
+      <c r="I5" s="17">
+        <f>Gross!J30</f>
         <v>250</v>
       </c>
-      <c r="I5">
-        <f>Gross!J30</f>
+      <c r="J5" s="17">
+        <f>Gross!K30</f>
         <v>300</v>
       </c>
-      <c r="J5" s="16">
-        <f>Gross!K30</f>
-        <v>365</v>
-      </c>
-      <c r="K5">
+      <c r="K5" s="14">
         <f>Gross!L30</f>
         <v>400</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="17">
         <f>Gross!M30</f>
         <v>500</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="18">
         <f>Gross!N30</f>
         <v>580</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B6" s="7">
         <f>Gross!C45</f>
@@ -2776,136 +2747,136 @@
         <f>Gross!H45</f>
         <v>166400.00000000003</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="19">
         <f>Gross!I45</f>
+        <v>222560.00000000006</v>
+      </c>
+      <c r="I6" s="20">
+        <f>Gross!J45</f>
         <v>260000.00000000006</v>
       </c>
-      <c r="I6">
-        <f>Gross!J45</f>
+      <c r="J6" s="20">
+        <f>Gross!K45</f>
         <v>312000.00000000006</v>
       </c>
-      <c r="J6" s="16">
-        <f>Gross!K45</f>
-        <v>379600.00000000006</v>
-      </c>
-      <c r="K6">
+      <c r="K6" s="15">
         <f>Gross!L45</f>
         <v>416000.00000000012</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="20">
         <f>Gross!M45</f>
         <v>520000.00000000012</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="21">
         <f>Gross!N45</f>
         <v>603200.00000000012</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B8" s="7">
         <f>Operating_Costs!F13</f>
-        <v>378166.66666666663</v>
+        <v>222166.66666666666</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B10" s="7">
         <f>B6-$B$8</f>
-        <v>-372966.66666666663</v>
+        <v>-216966.66666666666</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:L10" si="0">C6-$B$8</f>
-        <v>-367766.66666666663</v>
+        <v>-211766.66666666666</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>-357366.66666666663</v>
+        <v>-201366.66666666666</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>-336566.66666666663</v>
+        <v>-180566.66666666666</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
-        <v>-294966.66666666663</v>
+        <v>-138966.66666666663</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>-211766.6666666666</v>
-      </c>
-      <c r="H10" s="1">
+        <v>-55766.666666666628</v>
+      </c>
+      <c r="H10" s="19">
         <f t="shared" si="0"/>
-        <v>-118166.66666666657</v>
-      </c>
-      <c r="I10" s="1">
+        <v>393.33333333340124</v>
+      </c>
+      <c r="I10" s="20">
         <f t="shared" si="0"/>
-        <v>-66166.66666666657</v>
-      </c>
-      <c r="J10" s="17">
+        <v>37833.333333333401</v>
+      </c>
+      <c r="J10" s="20">
         <f t="shared" si="0"/>
-        <v>1433.3333333334303</v>
-      </c>
-      <c r="K10" s="1">
+        <v>89833.333333333401</v>
+      </c>
+      <c r="K10" s="15">
         <f t="shared" si="0"/>
-        <v>37833.333333333489</v>
-      </c>
-      <c r="L10" s="1">
+        <v>193833.33333333346</v>
+      </c>
+      <c r="L10" s="20">
         <f t="shared" si="0"/>
-        <v>141833.33333333349</v>
-      </c>
-      <c r="M10" s="18">
+        <v>297833.33333333349</v>
+      </c>
+      <c r="M10" s="21">
         <f t="shared" ref="M10" si="1">M6-$B$8</f>
-        <v>225033.33333333349</v>
+        <v>381033.33333333349</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12">
         <f>H5</f>
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B13">
         <f>Gross!I37</f>
-        <v>40.000000000000007</v>
+        <v>34.240000000000009</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B16">
         <f>M5</f>
         <v>580</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B17">
         <f>B16*0.2</f>
@@ -2918,7 +2889,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B18">
         <f>B16-(0.2*710)</f>
@@ -2927,7 +2898,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B20">
         <f>Gross!L37</f>
@@ -2936,7 +2907,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B21" s="9">
         <v>0.75</v>
@@ -2944,19 +2915,19 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B22">
         <f>B20*(1+B21)</f>
         <v>112.00000000000003</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B24">
         <f>Gross!B7</f>
@@ -2965,7 +2936,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2973,7 +2944,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B26">
         <f>B24*B25</f>
@@ -2982,7 +2953,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B28">
         <f>B26-B22</f>
@@ -2991,7 +2962,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B29">
         <f>C17-B28</f>
@@ -3007,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7959888-B526-4FAC-9FC1-7A03020906F6}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3027,36 +2998,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B3">
         <f>10</f>
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F3" s="9">
         <v>0.2</v>
@@ -3065,13 +3036,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F4" s="9">
         <v>0.8</v>
@@ -3079,7 +3050,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -3096,22 +3067,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C12" s="9">
         <v>0.2</v>
@@ -3122,7 +3093,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B13" s="1">
         <v>40</v>
@@ -3136,7 +3107,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
@@ -3150,7 +3121,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B15" s="1">
         <v>20</v>
@@ -3174,36 +3145,36 @@
     <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" t="s">
         <v>160</v>
       </c>
-      <c r="F19" t="s">
-        <v>158</v>
-      </c>
       <c r="G19" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
+      <c r="A20" s="22">
         <v>0.8</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D20" s="8">
         <v>0.8</v>
@@ -3221,12 +3192,12 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="22"/>
       <c r="B21">
         <v>0.2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D21" s="8">
         <v>0.2</v>
@@ -3244,12 +3215,12 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="22"/>
       <c r="B22">
         <v>0.8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D22" s="8">
         <v>0.8</v>
@@ -3267,12 +3238,12 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="22"/>
       <c r="B23">
         <v>0.8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D23" s="8">
         <v>0.2</v>
@@ -3304,17 +3275,17 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
+      <c r="A25" s="22">
         <v>0.2</v>
       </c>
       <c r="B25" s="8">
         <v>0.8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E25" s="3">
         <f>$A$25*$B25</f>
@@ -3325,15 +3296,15 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="8">
         <v>0.2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E26" s="3">
         <f>$A$25*$B26</f>
@@ -3357,16 +3328,16 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -3387,13 +3358,13 @@
         <v>160</v>
       </c>
       <c r="I30">
+        <v>214</v>
+      </c>
+      <c r="J30">
         <v>250</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>300</v>
-      </c>
-      <c r="K30">
-        <v>365</v>
       </c>
       <c r="L30">
         <v>400</v>
@@ -3407,7 +3378,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
@@ -3437,23 +3408,23 @@
         <v>409.60000000000008</v>
       </c>
       <c r="I31" s="1">
-        <f>$E20*$F20*$B31*I$30</f>
+        <f t="shared" ref="I31" si="3">$E20*$F20*$B31*I$30</f>
+        <v>547.84000000000015</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" ref="J31:M34" si="4">$E20*$F20*$B31*J$30</f>
         <v>640.00000000000011</v>
       </c>
-      <c r="J31" s="1">
-        <f>$E20*$F20*$B31*J$30</f>
+      <c r="K31" s="1">
+        <f t="shared" si="4"/>
         <v>768.00000000000011</v>
       </c>
-      <c r="K31" s="1">
-        <f>$E20*$F20*$B31*K$30</f>
-        <v>934.4000000000002</v>
-      </c>
       <c r="L31" s="1">
-        <f>$E20*$F20*$B31*L$30</f>
+        <f t="shared" si="4"/>
         <v>1024.0000000000002</v>
       </c>
       <c r="M31" s="1">
-        <f>$E20*$F20*$B31*M$30</f>
+        <f t="shared" si="4"/>
         <v>1280.0000000000002</v>
       </c>
       <c r="N31" s="1">
@@ -3463,175 +3434,175 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B32" s="1">
         <v>10</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" ref="C32:H34" si="3">$E21*$F21*$B32*C$30</f>
+        <f t="shared" ref="C32:H34" si="5">$E21*$F21*$B32*C$30</f>
         <v>4.8000000000000016</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.6000000000000032</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19.200000000000006</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>38.400000000000013</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>76.800000000000026</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>153.60000000000005</v>
       </c>
       <c r="I32" s="1">
-        <f>$E21*$F21*$B32*I$30</f>
+        <f t="shared" ref="I32" si="6">$E21*$F21*$B32*I$30</f>
+        <v>205.44000000000005</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="4"/>
         <v>240.00000000000009</v>
       </c>
-      <c r="J32" s="1">
-        <f>$E21*$F21*$B32*J$30</f>
+      <c r="K32" s="1">
+        <f t="shared" si="4"/>
         <v>288.00000000000011</v>
       </c>
-      <c r="K32" s="1">
-        <f>$E21*$F21*$B32*K$30</f>
-        <v>350.40000000000009</v>
-      </c>
       <c r="L32" s="1">
-        <f>$E21*$F21*$B32*L$30</f>
+        <f t="shared" si="4"/>
         <v>384.00000000000011</v>
       </c>
       <c r="M32" s="1">
-        <f>$E21*$F21*$B32*M$30</f>
+        <f t="shared" si="4"/>
         <v>480.00000000000017</v>
       </c>
       <c r="N32" s="1">
-        <f>$E21*$F21*$B32*N$30</f>
+        <f t="shared" ref="N32" si="7">$E21*$F21*$B32*N$30</f>
         <v>556.80000000000018</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B33" s="1">
         <v>20</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>51.20000000000001</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>102.40000000000002</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>204.80000000000004</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>409.60000000000008</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>819.20000000000016</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1638.4000000000003</v>
       </c>
       <c r="I33" s="1">
-        <f>$E22*$F22*$B33*I$30</f>
+        <f t="shared" ref="I33" si="8">$E22*$F22*$B33*I$30</f>
+        <v>2191.3600000000006</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="4"/>
         <v>2560.0000000000005</v>
       </c>
-      <c r="J33" s="1">
-        <f>$E22*$F22*$B33*J$30</f>
+      <c r="K33" s="1">
+        <f t="shared" si="4"/>
         <v>3072.0000000000005</v>
       </c>
-      <c r="K33" s="1">
-        <f>$E22*$F22*$B33*K$30</f>
-        <v>3737.6000000000008</v>
-      </c>
       <c r="L33" s="1">
-        <f>$E22*$F22*$B33*L$30</f>
+        <f t="shared" si="4"/>
         <v>4096.0000000000009</v>
       </c>
       <c r="M33" s="1">
-        <f>$E22*$F22*$B33*M$30</f>
+        <f t="shared" si="4"/>
         <v>5120.0000000000009</v>
       </c>
       <c r="N33" s="1">
-        <f>$E22*$F22*$B33*N$30</f>
+        <f t="shared" ref="N33" si="9">$E22*$F22*$B33*N$30</f>
         <v>5939.2000000000007</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B34" s="1">
         <v>20</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>25.600000000000005</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>51.20000000000001</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>102.40000000000002</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>204.80000000000004</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>409.60000000000008</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>819.20000000000016</v>
       </c>
       <c r="I34" s="1">
-        <f>$E23*$F23*$B34*I$30</f>
+        <f t="shared" ref="I34" si="10">$E23*$F23*$B34*I$30</f>
+        <v>1095.6800000000003</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="4"/>
         <v>1280.0000000000002</v>
       </c>
-      <c r="J34" s="1">
-        <f>$E23*$F23*$B34*J$30</f>
+      <c r="K34" s="1">
+        <f t="shared" si="4"/>
         <v>1536.0000000000002</v>
       </c>
-      <c r="K34" s="1">
-        <f>$E23*$F23*$B34*K$30</f>
-        <v>1868.8000000000004</v>
-      </c>
       <c r="L34" s="1">
-        <f>$E23*$F23*$B34*L$30</f>
+        <f t="shared" si="4"/>
         <v>2048.0000000000005</v>
       </c>
       <c r="M34" s="1">
-        <f>$E23*$F23*$B34*M$30</f>
+        <f t="shared" si="4"/>
         <v>2560.0000000000005</v>
       </c>
       <c r="N34" s="1">
-        <f>$E23*$F23*$B34*N$30</f>
+        <f t="shared" ref="N34" si="11">$E23*$F23*$B34*N$30</f>
         <v>2969.6000000000004</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C35" s="7">
         <f>SUM(C31:C34)</f>
@@ -3642,32 +3613,32 @@
         <v>188.80000000000004</v>
       </c>
       <c r="E35" s="7">
-        <f t="shared" ref="E35:I35" si="4">SUM(E31:E34)</f>
+        <f t="shared" ref="E35:I35" si="12">SUM(E31:E34)</f>
         <v>377.60000000000008</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>755.20000000000016</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1510.4000000000003</v>
       </c>
       <c r="H35" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>3020.8000000000006</v>
       </c>
       <c r="I35" s="7">
-        <f t="shared" si="4"/>
-        <v>4720.0000000000009</v>
+        <f t="shared" si="12"/>
+        <v>4040.3200000000011</v>
       </c>
       <c r="J35" s="7">
         <f>SUM(J31:J34)</f>
-        <v>5664.0000000000009</v>
+        <v>4720.0000000000009</v>
       </c>
       <c r="K35" s="7">
         <f>SUM(K31:K34)</f>
-        <v>6891.2000000000016</v>
+        <v>5664.0000000000009</v>
       </c>
       <c r="L35" s="7">
         <f>SUM(L31:L34)</f>
@@ -3684,43 +3655,43 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C36" s="3">
         <f>C$30*($G$24)</f>
         <v>5.6000000000000014</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" ref="D36:H36" si="5">D$30*($G$24)</f>
+        <f t="shared" ref="D36:I36" si="13">D$30*($G$24)</f>
         <v>11.200000000000003</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>22.400000000000006</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>44.800000000000011</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>89.600000000000023</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>179.20000000000005</v>
       </c>
       <c r="I36" s="3">
-        <f>I$30*($G$24)</f>
-        <v>280.00000000000006</v>
+        <f t="shared" si="13"/>
+        <v>239.68000000000006</v>
       </c>
       <c r="J36" s="3">
         <f>J$30*($G$24)</f>
-        <v>336.00000000000011</v>
+        <v>280.00000000000006</v>
       </c>
       <c r="K36" s="3">
         <f>K$30*($G$24)</f>
-        <v>408.80000000000013</v>
+        <v>336.00000000000011</v>
       </c>
       <c r="L36" s="3">
         <f>L$30*($G$24)</f>
@@ -3737,43 +3708,43 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C37">
         <f>C36/7</f>
         <v>0.80000000000000016</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:I37" si="6">D36/7</f>
+        <f t="shared" ref="D37:I37" si="14">D36/7</f>
         <v>1.6000000000000003</v>
       </c>
       <c r="E37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>3.2000000000000006</v>
       </c>
       <c r="F37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>6.4000000000000012</v>
       </c>
       <c r="G37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>12.800000000000002</v>
       </c>
       <c r="H37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="14"/>
         <v>25.600000000000005</v>
       </c>
       <c r="I37">
-        <f t="shared" si="6"/>
-        <v>40.000000000000007</v>
+        <f t="shared" si="14"/>
+        <v>34.240000000000009</v>
       </c>
       <c r="J37">
         <f>J36/7</f>
-        <v>48.000000000000014</v>
+        <v>40.000000000000007</v>
       </c>
       <c r="K37">
         <f>K36/7</f>
-        <v>58.40000000000002</v>
+        <v>48.000000000000014</v>
       </c>
       <c r="L37">
         <f>L36/7</f>
@@ -3790,152 +3761,152 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" ref="C41:M41" si="7">C35*50</f>
+        <f t="shared" ref="C41:M41" si="15">C35*50</f>
         <v>4720.0000000000009</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>9440.0000000000018</v>
       </c>
       <c r="E41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>18880.000000000004</v>
       </c>
       <c r="F41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>37760.000000000007</v>
       </c>
       <c r="G41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>75520.000000000015</v>
       </c>
       <c r="H41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>151040.00000000003</v>
       </c>
       <c r="I41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
+        <v>202016.00000000006</v>
+      </c>
+      <c r="J41" s="7">
+        <f t="shared" si="15"/>
         <v>236000.00000000006</v>
       </c>
-      <c r="J41" s="7">
-        <f t="shared" si="7"/>
+      <c r="K41" s="7">
+        <f t="shared" si="15"/>
         <v>283200.00000000006</v>
       </c>
-      <c r="K41" s="7">
-        <f t="shared" si="7"/>
-        <v>344560.00000000006</v>
-      </c>
       <c r="L41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>377600.00000000012</v>
       </c>
       <c r="M41" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>472000.00000000012</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" ref="N41" si="8">N35*50</f>
+        <f t="shared" ref="N41" si="16">N35*50</f>
         <v>547520.00000000012</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B42" s="1">
         <v>40</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" ref="C42:H42" si="9">C$30*$B42*$A$25</f>
+        <f t="shared" ref="C42:N42" si="17">C$30*$B42*$A$25</f>
         <v>40</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>80</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>160</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>320</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>640</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>1280</v>
       </c>
       <c r="I42" s="7">
-        <f>I$30*$B42*$A$25</f>
+        <f t="shared" si="17"/>
+        <v>1712</v>
+      </c>
+      <c r="J42" s="7">
+        <f t="shared" si="17"/>
         <v>2000</v>
       </c>
-      <c r="J42" s="7">
-        <f>J$30*$B42*$A$25</f>
+      <c r="K42" s="7">
+        <f t="shared" si="17"/>
         <v>2400</v>
       </c>
-      <c r="K42" s="7">
-        <f>K$30*$B42*$A$25</f>
-        <v>2920</v>
-      </c>
       <c r="L42" s="7">
-        <f>L$30*$B42*$A$25</f>
+        <f t="shared" si="17"/>
         <v>3200</v>
       </c>
       <c r="M42" s="7">
-        <f>M$30*$B42*$A$25</f>
+        <f t="shared" si="17"/>
         <v>4000</v>
       </c>
       <c r="N42" s="7">
-        <f>N$30*$B42*$A$25</f>
+        <f t="shared" si="17"/>
         <v>4640</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C43" s="7">
         <f>C42*12</f>
         <v>480</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" ref="D43:I43" si="10">D42*12</f>
+        <f t="shared" ref="D43:I43" si="18">D42*12</f>
         <v>960</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>1920</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3840</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>7680</v>
       </c>
       <c r="H43" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>15360</v>
       </c>
       <c r="I43" s="7">
-        <f t="shared" si="10"/>
-        <v>24000</v>
+        <f t="shared" si="18"/>
+        <v>20544</v>
       </c>
       <c r="J43" s="7">
         <f>J42*12</f>
-        <v>28800</v>
+        <v>24000</v>
       </c>
       <c r="K43" s="7">
         <f>K42*12</f>
-        <v>35040</v>
+        <v>28800</v>
       </c>
       <c r="L43" s="7">
         <f>L42*12</f>
@@ -3952,54 +3923,54 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" ref="C45:M45" si="11">C43+C41</f>
+        <f t="shared" ref="C45:M45" si="19">C43+C41</f>
         <v>5200.0000000000009</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>10400.000000000002</v>
       </c>
       <c r="E45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>20800.000000000004</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>41600.000000000007</v>
       </c>
       <c r="G45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>83200.000000000015</v>
       </c>
       <c r="H45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>166400.00000000003</v>
       </c>
       <c r="I45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
+        <v>222560.00000000006</v>
+      </c>
+      <c r="J45" s="7">
+        <f t="shared" si="19"/>
         <v>260000.00000000006</v>
       </c>
-      <c r="J45" s="7">
-        <f t="shared" si="11"/>
+      <c r="K45" s="7">
+        <f t="shared" si="19"/>
         <v>312000.00000000006</v>
       </c>
-      <c r="K45" s="7">
-        <f t="shared" si="11"/>
-        <v>379600.00000000006</v>
-      </c>
       <c r="L45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>416000.00000000012</v>
       </c>
       <c r="M45" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>520000.00000000012</v>
       </c>
       <c r="N45" s="7">
-        <f t="shared" ref="N45" si="12">N43+N41</f>
+        <f t="shared" ref="N45" si="20">N43+N41</f>
         <v>603200.00000000012</v>
       </c>
     </row>
@@ -4014,15 +3985,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
-  <dimension ref="A3:J27"/>
+  <dimension ref="A3:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -4032,27 +4003,27 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
         <v>124</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1">
         <f>C4/7</f>
@@ -4076,7 +4047,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1">
         <f>C5/7</f>
@@ -4101,7 +4072,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1">
         <f>200/30</f>
@@ -4126,7 +4097,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B7" s="1">
         <f>400/30</f>
@@ -4151,7 +4122,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1">
         <f>100/30</f>
@@ -4176,7 +4147,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1">
         <f>C9/7</f>
@@ -4201,7 +4172,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B10" s="1">
         <f>C10/7</f>
@@ -4225,7 +4196,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1">
         <f>C11/7</f>
@@ -4249,30 +4220,29 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B12" s="1">
         <f>C12/7</f>
-        <v>593.40659340659352</v>
+        <v>164.83516483516482</v>
       </c>
       <c r="C12" s="1">
         <f>F12/52</f>
-        <v>4153.8461538461543</v>
+        <v>1153.8461538461538</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>8307.6923076923085</v>
+        <v>2307.6923076923076</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>16615.384615384617</v>
+        <v>4615.3846153846152</v>
       </c>
       <c r="F12" s="1">
-        <f>H13*12</f>
-        <v>216000</v>
+        <v>60000</v>
       </c>
       <c r="H12" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -4281,105 +4251,29 @@
       </c>
       <c r="B13" s="1">
         <f>SUM(B4:B12)</f>
-        <v>1042.8937728937731</v>
+        <v>614.32234432234429</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:F13" si="1">SUM(C4:C12)</f>
-        <v>7300.2564102564111</v>
+        <v>4300.2564102564102</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>16754.358974358976</v>
+        <v>10754.358974358973</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>33508.717948717953</v>
+        <v>21508.717948717946</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>378166.66666666663</v>
+        <v>222166.66666666666</v>
       </c>
       <c r="H13" s="6">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>250</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>252</v>
-      </c>
-      <c r="C23" s="1">
-        <v>22</v>
-      </c>
-      <c r="D23" s="2">
-        <v>10000</v>
-      </c>
-      <c r="E23" s="1">
-        <f>C23*D23</f>
-        <v>220000</v>
-      </c>
-      <c r="F23" s="1">
-        <f>E23/12</f>
-        <v>18333.333333333332</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>254</v>
-      </c>
-      <c r="C24" s="1">
-        <v>17</v>
-      </c>
-      <c r="D24" s="2">
-        <v>10000</v>
-      </c>
-      <c r="E24" s="1">
-        <f>C24*D24</f>
-        <v>170000</v>
-      </c>
-      <c r="F24" s="1">
-        <f>E24/12</f>
-        <v>14166.666666666666</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E27" s="1">
-        <v>15000</v>
-      </c>
-      <c r="F27" s="1">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A26" r:id="rId1" xr:uid="{F79E9E73-FE81-49C9-AD29-E42F9F967839}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4407,21 +4301,21 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -4445,7 +4339,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -4469,7 +4363,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -4493,7 +4387,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4">
         <v>0.15</v>
@@ -4517,7 +4411,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B6" s="4">
         <v>0.1</v>
@@ -4541,7 +4435,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B7" s="4">
         <v>0.05</v>
@@ -4574,7 +4468,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -4594,7 +4488,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B12" s="1">
         <v>7.5</v>
@@ -4618,7 +4512,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -4626,7 +4520,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -4634,7 +4528,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B16" s="7">
         <f>B12*B15</f>
@@ -4643,7 +4537,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B17" s="7">
         <f>B14*B16</f>
@@ -4652,7 +4546,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B18" s="9">
         <v>0.2</v>
@@ -4660,7 +4554,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B19" s="7">
         <f>B17*(B18+1)</f>
@@ -4675,7 +4569,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B22" s="7"/>
     </row>
@@ -4688,8 +4582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4705,7 +4599,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B3" s="1">
         <v>50000</v>
@@ -4713,7 +4607,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1">
         <v>45000</v>
@@ -4721,7 +4615,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B5" s="1">
         <v>25000</v>
@@ -4738,7 +4632,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="1">
         <f>B6/52</f>
@@ -4747,7 +4641,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1">
         <f>B6/26</f>
@@ -4756,7 +4650,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B11" s="1">
         <f>B10*2</f>
@@ -4827,7 +4721,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -4888,7 +4782,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B8" s="1">
         <v>300</v>
@@ -4985,7 +4879,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1">
         <v>5000</v>
@@ -4993,7 +4887,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D6" s="1">
         <v>3000</v>
@@ -5001,7 +4895,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D8" s="7">
         <f>D3+D6</f>

</xml_diff>

<commit_message>
passed over all of the topics that I'll need for the business
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c2c6e3652e668e7/Work/Projects/dogen/Finances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1828" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{13F8F6F8-F69B-41B3-805D-C363026AC50D}"/>
+  <xr:revisionPtr revIDLastSave="1948" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3C18B96D-9568-4EB0-AEA3-9E99F89FA676}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="258">
   <si>
     <t>Overhead</t>
   </si>
@@ -199,18 +201,12 @@
     <t>Wifi</t>
   </si>
   <si>
-    <t>laminate countertops per square foot</t>
-  </si>
-  <si>
     <t>Electrical outlets</t>
   </si>
   <si>
     <t>sink installation and plumbing</t>
   </si>
   <si>
-    <t>premium refrigerator</t>
-  </si>
-  <si>
     <t>shared kitchen appliances</t>
   </si>
   <si>
@@ -685,9 +681,6 @@
     <t>Build the space</t>
   </si>
   <si>
-    <t>Dance groups arrive</t>
-  </si>
-  <si>
     <t>Month 4 -12</t>
   </si>
   <si>
@@ -791,6 +784,42 @@
   </si>
   <si>
     <t>Total Overhead Costs</t>
+  </si>
+  <si>
+    <t>knife sharpener</t>
+  </si>
+  <si>
+    <t>three-door fridge</t>
+  </si>
+  <si>
+    <t>granite counter tops per sq foot</t>
+  </si>
+  <si>
+    <t>low end</t>
+  </si>
+  <si>
+    <t>high end</t>
+  </si>
+  <si>
+    <t>Sq. feet I need</t>
+  </si>
+  <si>
+    <t>estimated cost</t>
+  </si>
+  <si>
+    <t>Rent in New Haven per sq. foot per year  is typically</t>
+  </si>
+  <si>
+    <t>Recruiting Instructors and businesses</t>
+  </si>
+  <si>
+    <t>Work-man's comp</t>
+  </si>
+  <si>
+    <t>Work-man's Comp multiplier</t>
+  </si>
+  <si>
+    <t>Workman's comp Estimate</t>
   </si>
 </sst>
 </file>
@@ -804,7 +833,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,8 +862,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -843,20 +886,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -884,14 +919,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -906,22 +943,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="6"/>
+    <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1237,192 +1273,192 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4">
+        <f>Net_And_Analysis!I5</f>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>191</v>
-      </c>
-      <c r="B4">
-        <f>Net_And_Analysis!H5</f>
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>193</v>
       </c>
       <c r="B6">
         <f>Net_And_Analysis!H5</f>
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B7">
         <f>Net_And_Analysis!I5</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B8">
         <f>Net_And_Analysis!J5</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B9">
         <f>Net_And_Analysis!K5</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B10">
         <f>Net_And_Analysis!L5</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B11">
         <f>Net_And_Analysis!M5</f>
         <v>580</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C14">
         <v>2018</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" s="11">
+        <v>58809</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" s="11">
+        <v>56453</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="11">
+        <v>58645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="11">
+        <v>49754</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" s="11">
+        <v>50741</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>234</v>
+      </c>
+      <c r="B20" s="11">
+        <v>54969</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>235</v>
+      </c>
+      <c r="B21" s="11">
+        <v>59755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>236</v>
       </c>
-      <c r="B15">
-        <v>58809</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>235</v>
-      </c>
-      <c r="B16">
-        <v>56453</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>234</v>
-      </c>
-      <c r="B17">
-        <v>58645</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18">
-        <v>49754</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>232</v>
-      </c>
-      <c r="B19">
-        <v>50741</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B22" s="11">
+        <v>59073</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>237</v>
       </c>
-      <c r="B20">
-        <v>54969</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B23" s="11">
+        <v>60768</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>238</v>
       </c>
-      <c r="B21">
-        <v>59755</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B24" s="11">
+        <v>45951</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>239</v>
       </c>
-      <c r="B22">
-        <v>59073</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>240</v>
-      </c>
-      <c r="B23">
-        <v>60768</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>241</v>
-      </c>
-      <c r="B24">
-        <v>45951</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>242</v>
-      </c>
-      <c r="B25">
+      <c r="B25" s="11">
         <v>37199</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1431,48 +1467,48 @@
         <v>592117</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B29" s="11">
         <v>25000</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>201</v>
       </c>
       <c r="B31" s="12">
         <f>B28+B29</f>
         <v>617117</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B32" s="11">
         <v>620000</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B34" s="13">
         <f>$B$4/$B$31</f>
-        <v>3.4677378843882116E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6.1576654021846752E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B35" s="13">
         <f>$B$11/$B$28</f>
@@ -1490,49 +1526,47 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560605D-AE6F-456E-B5FE-7223BF3283FD}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>248</v>
       </c>
       <c r="B2" s="1">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1549,27 +1583,27 @@
       </c>
       <c r="G2" s="7">
         <f>(PRODUCT(B2:D2) +E2)*F2</f>
-        <v>3825</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B3" s="1">
-        <v>700</v>
+        <v>2000</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="G3" s="7">
         <f>B3*C3</f>
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1">
         <v>300</v>
@@ -1582,9 +1616,9 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
@@ -1593,43 +1627,43 @@
         <v>4</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G15" si="0">B5*C5</f>
+        <f t="shared" ref="G5:G16" si="0">B5*C5</f>
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="G6" s="7">
         <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B7" s="1">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B8" s="1">
         <v>8000</v>
@@ -1642,12 +1676,12 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B9" s="1">
-        <v>350</v>
+        <v>2500</v>
       </c>
       <c r="C9">
         <f>C7</f>
@@ -1655,28 +1689,27 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>247</v>
       </c>
       <c r="B10" s="1">
-        <v>900</v>
+        <v>3900</v>
       </c>
       <c r="C10">
-        <f>$F$2</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1">
         <v>1000</v>
@@ -1689,9 +1722,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1704,9 +1737,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1">
         <v>100</v>
@@ -1719,9 +1752,9 @@
         <v>600</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1">
         <v>250</v>
@@ -1734,9 +1767,9 @@
         <v>750</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1">
         <v>80</v>
@@ -1749,13 +1782,28 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="1">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="7">
-        <f>SUM(G2:G15)</f>
-        <v>27115</v>
+      <c r="G20" s="7">
+        <f>SUM(G2:G16)</f>
+        <v>47315</v>
       </c>
     </row>
   </sheetData>
@@ -1771,33 +1819,33 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1819,34 +1867,34 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <f>D3</f>
@@ -1867,9 +1915,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1889,9 +1937,9 @@
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1911,9 +1959,9 @@
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1933,7 +1981,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1955,55 +2003,55 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>20</v>
@@ -2041,23 +2089,23 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K3" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K4" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2079,13 +2127,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2093,7 +2141,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2104,7 +2152,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2115,7 +2163,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2124,7 +2172,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2133,7 +2181,7 @@
         <v>8400</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2142,7 +2190,7 @@
         <v>107100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2150,7 +2198,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2161,7 +2209,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2169,7 +2217,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2177,7 +2225,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2185,7 +2233,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2194,7 +2242,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2203,12 +2251,12 @@
         <v>175500</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2216,7 +2264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2224,12 +2272,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2237,12 +2285,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -2250,7 +2298,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -2258,7 +2306,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
@@ -2267,7 +2315,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -2275,7 +2323,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
@@ -2283,7 +2331,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -2292,7 +2340,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -2301,7 +2349,7 @@
         <v>15750</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -2310,7 +2358,7 @@
         <v>63000</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -2319,7 +2367,7 @@
         <v>803250</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
@@ -2328,7 +2376,7 @@
         <v>200812.5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2385,7 @@
         <v>602437.5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
@@ -2356,118 +2404,117 @@
   <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B3" s="7">
         <f>Gaming!D12</f>
         <v>19680</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="7">
         <f>Dance_Studio!D8</f>
         <v>16500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="7">
-        <f>Kitchen!G17</f>
-        <v>27115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <f>Kitchen!G20</f>
+        <v>47315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="7">
         <f>Liabilities!B7</f>
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="7">
         <f>decor!K7</f>
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B8" s="7">
         <f>'Eating Area'!F10</f>
         <v>3200</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" s="7">
         <f>SUM(B3:B8)</f>
-        <v>67445</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>87645</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B11" s="6">
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B12" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B13" s="7">
         <f>SUM(B10:B12)</f>
-        <v>79445</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" s="7">
         <f>Operating_Costs!F13</f>
-        <v>222166.66666666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>393966.66666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -2488,9 +2535,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B17">
         <f>B16/12</f>
@@ -2517,120 +2564,120 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B18" s="7">
         <f t="shared" ref="B18:G18" si="1">$B$15*B$17</f>
-        <v>111083.33333333333</v>
+        <v>196983.33333333331</v>
       </c>
       <c r="C18" s="7">
         <f t="shared" si="1"/>
-        <v>92569.444444444438</v>
+        <v>164152.77777777778</v>
       </c>
       <c r="D18" s="7">
         <f t="shared" si="1"/>
-        <v>74055.555555555547</v>
+        <v>131322.22222222219</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="1"/>
-        <v>55541.666666666664</v>
+        <v>98491.666666666657</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>37027.777777777774</v>
+        <v>65661.111111111095</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="1"/>
-        <v>18513.888888888887</v>
+        <v>32830.555555555547</v>
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" s="7">
         <f>$B$10+($B$15*B$17)+$B$12+$B$11</f>
-        <v>190528.33333333331</v>
+        <v>296628.33333333331</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:G19" si="2">$B$10+($B$15*C$17)+$B$12+$B$11</f>
-        <v>172014.44444444444</v>
+        <v>263797.77777777775</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="2"/>
-        <v>153500.55555555556</v>
+        <v>230967.22222222219</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="2"/>
-        <v>134986.66666666666</v>
+        <v>198136.66666666666</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="2"/>
-        <v>116472.77777777778</v>
+        <v>165306.11111111109</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="2"/>
-        <v>97958.888888888891</v>
+        <v>132475.55555555556</v>
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>211</v>
       </c>
-      <c r="B22" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>207</v>
-      </c>
-      <c r="B23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>206</v>
-      </c>
-      <c r="B24" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>209</v>
-      </c>
-      <c r="B27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>214</v>
-      </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2642,31 +2689,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A112772E-1427-43D2-80C2-98741A931E56}">
   <dimension ref="A4:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H4" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I4" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2694,34 +2742,34 @@
         <f>Gross!H30</f>
         <v>160</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5">
         <f>Gross!I30</f>
-        <v>214</v>
-      </c>
-      <c r="I5" s="17">
+        <v>250</v>
+      </c>
+      <c r="I5" s="15">
         <f>Gross!J30</f>
-        <v>250</v>
-      </c>
-      <c r="J5" s="17">
+        <v>380</v>
+      </c>
+      <c r="J5">
         <f>Gross!K30</f>
-        <v>300</v>
-      </c>
-      <c r="K5" s="14">
+        <v>450</v>
+      </c>
+      <c r="K5">
         <f>Gross!L30</f>
-        <v>400</v>
-      </c>
-      <c r="L5" s="17">
+        <v>500</v>
+      </c>
+      <c r="L5">
         <f>Gross!M30</f>
-        <v>500</v>
-      </c>
-      <c r="M5" s="18">
+        <v>540</v>
+      </c>
+      <c r="M5" s="17">
         <f>Gross!N30</f>
         <v>580</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B6" s="7">
         <f>Gross!C45</f>
@@ -2747,136 +2795,155 @@
         <f>Gross!H45</f>
         <v>166400.00000000003</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="7">
         <f>Gross!I45</f>
-        <v>222560.00000000006</v>
-      </c>
-      <c r="I6" s="20">
+        <v>260000.00000000006</v>
+      </c>
+      <c r="I6" s="16">
         <f>Gross!J45</f>
-        <v>260000.00000000006</v>
-      </c>
-      <c r="J6" s="20">
+        <v>395200.00000000006</v>
+      </c>
+      <c r="J6" s="7">
         <f>Gross!K45</f>
-        <v>312000.00000000006</v>
-      </c>
-      <c r="K6" s="15">
+        <v>468000.00000000012</v>
+      </c>
+      <c r="K6" s="7">
         <f>Gross!L45</f>
-        <v>416000.00000000012</v>
-      </c>
-      <c r="L6" s="20">
+        <v>520000.00000000012</v>
+      </c>
+      <c r="L6" s="7">
         <f>Gross!M45</f>
-        <v>520000.00000000012</v>
-      </c>
-      <c r="M6" s="21">
+        <v>561600.00000000012</v>
+      </c>
+      <c r="M6" s="18">
         <f>Gross!N45</f>
         <v>603200.00000000012</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H7" s="7"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" s="7">
         <f>Operating_Costs!F13</f>
-        <v>222166.66666666666</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>393966.66666666663</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H9" s="7"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B10" s="7">
         <f>B6-$B$8</f>
-        <v>-216966.66666666666</v>
+        <v>-388766.66666666663</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:L10" si="0">C6-$B$8</f>
-        <v>-211766.66666666666</v>
+        <v>-383566.66666666663</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>-201366.66666666666</v>
+        <v>-373166.66666666663</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>-180566.66666666666</v>
+        <v>-352366.66666666663</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
-        <v>-138966.66666666663</v>
+        <v>-310766.66666666663</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>-55766.666666666628</v>
-      </c>
-      <c r="H10" s="19">
+        <v>-227566.6666666666</v>
+      </c>
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
-        <v>393.33333333340124</v>
-      </c>
-      <c r="I10" s="20">
+        <v>-133966.66666666657</v>
+      </c>
+      <c r="I10" s="16">
         <f t="shared" si="0"/>
-        <v>37833.333333333401</v>
-      </c>
-      <c r="J10" s="20">
+        <v>1233.3333333334303</v>
+      </c>
+      <c r="J10" s="7">
         <f t="shared" si="0"/>
-        <v>89833.333333333401</v>
-      </c>
-      <c r="K10" s="15">
+        <v>74033.333333333489</v>
+      </c>
+      <c r="K10" s="7">
         <f t="shared" si="0"/>
-        <v>193833.33333333346</v>
-      </c>
-      <c r="L10" s="20">
+        <v>126033.33333333349</v>
+      </c>
+      <c r="L10" s="7">
         <f t="shared" si="0"/>
-        <v>297833.33333333349</v>
-      </c>
-      <c r="M10" s="21">
+        <v>167633.33333333349</v>
+      </c>
+      <c r="M10" s="18">
         <f t="shared" ref="M10" si="1">M6-$B$8</f>
-        <v>381033.33333333349</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>209233.33333333349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <f>H5</f>
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B13">
         <f>Gross!I37</f>
-        <v>34.240000000000009</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>40.000000000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B16">
         <f>M5</f>
         <v>580</v>
       </c>
       <c r="C16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B17">
         <f>B16*0.2</f>
@@ -2887,86 +2954,86 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B18">
         <f>B16-(0.2*710)</f>
         <v>438</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B20">
         <f>Gross!L37</f>
-        <v>64.000000000000014</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>80.000000000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B21" s="9">
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B22">
         <f>B20*(1+B21)</f>
-        <v>112.00000000000003</v>
+        <v>140.00000000000003</v>
       </c>
       <c r="C22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B24">
         <f>Gross!B7</f>
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B26">
         <f>B24*B25</f>
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B28">
         <f>B26-B22</f>
-        <v>57.999999999999972</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>29.999999999999972</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B29">
         <f>C17-B28</f>
-        <v>0</v>
+        <v>28.000000000000028</v>
       </c>
     </row>
   </sheetData>
@@ -2979,84 +3046,84 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <f>10</f>
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F3" s="9">
         <v>0.2</v>
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F4" s="9">
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -3065,24 +3132,24 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C12" s="9">
         <v>0.2</v>
@@ -3091,9 +3158,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B13" s="1">
         <v>40</v>
@@ -3105,9 +3172,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
@@ -3119,9 +3186,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B15" s="1">
         <v>20</v>
@@ -3133,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D17" s="9">
         <v>0.2</v>
       </c>
@@ -3142,39 +3209,39 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" t="s">
         <v>161</v>
       </c>
-      <c r="B19" t="s">
-        <v>163</v>
-      </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
         <v>0.8</v>
       </c>
       <c r="B20">
         <v>0.2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D20" s="8">
         <v>0.8</v>
@@ -3191,13 +3258,13 @@
         <v>0.25600000000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
       <c r="B21">
         <v>0.2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D21" s="8">
         <v>0.2</v>
@@ -3214,13 +3281,13 @@
         <v>9.600000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
       <c r="B22">
         <v>0.8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D22" s="8">
         <v>0.8</v>
@@ -3237,13 +3304,13 @@
         <v>0.51200000000000012</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
       <c r="B23">
         <v>0.8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D23" s="8">
         <v>0.2</v>
@@ -3260,7 +3327,7 @@
         <v>0.25600000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="3">
         <f>SUM(E20:E23)</f>
@@ -3274,18 +3341,18 @@
         <v>1.1200000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="22">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
         <v>0.2</v>
       </c>
       <c r="B25" s="8">
         <v>0.8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E25" s="3">
         <f>$A$25*$B25</f>
@@ -3295,16 +3362,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
       <c r="B26" s="8">
         <v>0.2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E26" s="3">
         <f>$A$25*$B26</f>
@@ -3314,30 +3381,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E27">
         <f>SUM(E25:E26)</f>
         <v>0.20000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E28">
         <f>E24+E27</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -3358,27 +3425,27 @@
         <v>160</v>
       </c>
       <c r="I30">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="J30">
-        <v>250</v>
+        <v>380</v>
       </c>
       <c r="K30">
-        <v>300</v>
+        <v>450</v>
       </c>
       <c r="L30">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="M30">
-        <v>500</v>
+        <v>540</v>
       </c>
       <c r="N30">
         <v>580</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B31" s="1">
         <v>10</v>
@@ -3409,32 +3476,32 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" ref="I31" si="3">$E20*$F20*$B31*I$30</f>
-        <v>547.84000000000015</v>
+        <v>640.00000000000011</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" ref="J31:M34" si="4">$E20*$F20*$B31*J$30</f>
-        <v>640.00000000000011</v>
+        <v>972.80000000000018</v>
       </c>
       <c r="K31" s="1">
         <f t="shared" si="4"/>
-        <v>768.00000000000011</v>
+        <v>1152.0000000000002</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="4"/>
-        <v>1024.0000000000002</v>
+        <v>1280.0000000000002</v>
       </c>
       <c r="M31" s="1">
         <f t="shared" si="4"/>
-        <v>1280.0000000000002</v>
+        <v>1382.4000000000003</v>
       </c>
       <c r="N31" s="1">
         <f>$E20*$F20*$B31*N$30</f>
         <v>1484.8000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B32" s="1">
         <v>10</v>
@@ -3465,32 +3532,32 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" ref="I32" si="6">$E21*$F21*$B32*I$30</f>
-        <v>205.44000000000005</v>
+        <v>240.00000000000009</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="4"/>
-        <v>240.00000000000009</v>
+        <v>364.80000000000013</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="4"/>
-        <v>288.00000000000011</v>
+        <v>432.00000000000011</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="4"/>
-        <v>384.00000000000011</v>
+        <v>480.00000000000017</v>
       </c>
       <c r="M32" s="1">
         <f t="shared" si="4"/>
-        <v>480.00000000000017</v>
+        <v>518.4000000000002</v>
       </c>
       <c r="N32" s="1">
         <f t="shared" ref="N32" si="7">$E21*$F21*$B32*N$30</f>
         <v>556.80000000000018</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B33" s="1">
         <v>20</v>
@@ -3521,32 +3588,32 @@
       </c>
       <c r="I33" s="1">
         <f t="shared" ref="I33" si="8">$E22*$F22*$B33*I$30</f>
-        <v>2191.3600000000006</v>
+        <v>2560.0000000000005</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="4"/>
-        <v>2560.0000000000005</v>
+        <v>3891.2000000000007</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" si="4"/>
-        <v>3072.0000000000005</v>
+        <v>4608.0000000000009</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="4"/>
-        <v>4096.0000000000009</v>
+        <v>5120.0000000000009</v>
       </c>
       <c r="M33" s="1">
         <f t="shared" si="4"/>
-        <v>5120.0000000000009</v>
+        <v>5529.6000000000013</v>
       </c>
       <c r="N33" s="1">
         <f t="shared" ref="N33" si="9">$E22*$F22*$B33*N$30</f>
         <v>5939.2000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B34" s="1">
         <v>20</v>
@@ -3577,32 +3644,32 @@
       </c>
       <c r="I34" s="1">
         <f t="shared" ref="I34" si="10">$E23*$F23*$B34*I$30</f>
-        <v>1095.6800000000003</v>
+        <v>1280.0000000000002</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="4"/>
-        <v>1280.0000000000002</v>
+        <v>1945.6000000000004</v>
       </c>
       <c r="K34" s="1">
         <f t="shared" si="4"/>
-        <v>1536.0000000000002</v>
+        <v>2304.0000000000005</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="4"/>
-        <v>2048.0000000000005</v>
+        <v>2560.0000000000005</v>
       </c>
       <c r="M34" s="1">
         <f t="shared" si="4"/>
-        <v>2560.0000000000005</v>
+        <v>2764.8000000000006</v>
       </c>
       <c r="N34" s="1">
         <f t="shared" ref="N34" si="11">$E23*$F23*$B34*N$30</f>
         <v>2969.6000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C35" s="7">
         <f>SUM(C31:C34)</f>
@@ -3630,32 +3697,32 @@
       </c>
       <c r="I35" s="7">
         <f t="shared" si="12"/>
-        <v>4040.3200000000011</v>
+        <v>4720.0000000000009</v>
       </c>
       <c r="J35" s="7">
         <f>SUM(J31:J34)</f>
-        <v>4720.0000000000009</v>
+        <v>7174.4000000000015</v>
       </c>
       <c r="K35" s="7">
         <f>SUM(K31:K34)</f>
-        <v>5664.0000000000009</v>
+        <v>8496.0000000000018</v>
       </c>
       <c r="L35" s="7">
         <f>SUM(L31:L34)</f>
-        <v>7552.0000000000018</v>
+        <v>9440.0000000000018</v>
       </c>
       <c r="M35" s="7">
         <f>SUM(M31:M34)</f>
-        <v>9440.0000000000018</v>
+        <v>10195.200000000003</v>
       </c>
       <c r="N35" s="7">
         <f>SUM(N31:N34)</f>
         <v>10950.400000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C36" s="3">
         <f>C$30*($G$24)</f>
@@ -3683,32 +3750,32 @@
       </c>
       <c r="I36" s="3">
         <f t="shared" si="13"/>
-        <v>239.68000000000006</v>
+        <v>280.00000000000006</v>
       </c>
       <c r="J36" s="3">
         <f>J$30*($G$24)</f>
-        <v>280.00000000000006</v>
+        <v>425.60000000000014</v>
       </c>
       <c r="K36" s="3">
         <f>K$30*($G$24)</f>
-        <v>336.00000000000011</v>
+        <v>504.00000000000017</v>
       </c>
       <c r="L36" s="3">
         <f>L$30*($G$24)</f>
-        <v>448.00000000000011</v>
+        <v>560.00000000000011</v>
       </c>
       <c r="M36" s="3">
         <f>M$30*($G$24)</f>
-        <v>560.00000000000011</v>
+        <v>604.80000000000018</v>
       </c>
       <c r="N36" s="3">
         <f>N$30*($G$24)</f>
         <v>649.60000000000014</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C37">
         <f>C36/7</f>
@@ -3736,32 +3803,32 @@
       </c>
       <c r="I37">
         <f t="shared" si="14"/>
-        <v>34.240000000000009</v>
+        <v>40.000000000000007</v>
       </c>
       <c r="J37">
         <f>J36/7</f>
-        <v>40.000000000000007</v>
+        <v>60.800000000000018</v>
       </c>
       <c r="K37">
         <f>K36/7</f>
-        <v>48.000000000000014</v>
+        <v>72.000000000000028</v>
       </c>
       <c r="L37">
         <f>L36/7</f>
-        <v>64.000000000000014</v>
+        <v>80.000000000000014</v>
       </c>
       <c r="M37">
         <f>M36/7</f>
-        <v>80.000000000000014</v>
+        <v>86.40000000000002</v>
       </c>
       <c r="N37">
         <f>N36/7</f>
         <v>92.800000000000026</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C41" s="7">
         <f t="shared" ref="C41:M41" si="15">C35*50</f>
@@ -3789,32 +3856,32 @@
       </c>
       <c r="I41" s="7">
         <f t="shared" si="15"/>
-        <v>202016.00000000006</v>
+        <v>236000.00000000006</v>
       </c>
       <c r="J41" s="7">
         <f t="shared" si="15"/>
-        <v>236000.00000000006</v>
+        <v>358720.00000000006</v>
       </c>
       <c r="K41" s="7">
         <f t="shared" si="15"/>
-        <v>283200.00000000006</v>
+        <v>424800.00000000012</v>
       </c>
       <c r="L41" s="7">
         <f t="shared" si="15"/>
-        <v>377600.00000000012</v>
+        <v>472000.00000000012</v>
       </c>
       <c r="M41" s="7">
         <f t="shared" si="15"/>
-        <v>472000.00000000012</v>
+        <v>509760.00000000012</v>
       </c>
       <c r="N41" s="7">
         <f t="shared" ref="N41" si="16">N35*50</f>
         <v>547520.00000000012</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B42" s="1">
         <v>40</v>
@@ -3845,32 +3912,32 @@
       </c>
       <c r="I42" s="7">
         <f t="shared" si="17"/>
-        <v>1712</v>
+        <v>2000</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="17"/>
-        <v>2000</v>
+        <v>3040</v>
       </c>
       <c r="K42" s="7">
         <f t="shared" si="17"/>
-        <v>2400</v>
+        <v>3600</v>
       </c>
       <c r="L42" s="7">
         <f t="shared" si="17"/>
-        <v>3200</v>
+        <v>4000</v>
       </c>
       <c r="M42" s="7">
         <f t="shared" si="17"/>
-        <v>4000</v>
+        <v>4320</v>
       </c>
       <c r="N42" s="7">
         <f t="shared" si="17"/>
         <v>4640</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C43" s="7">
         <f>C42*12</f>
@@ -3898,32 +3965,32 @@
       </c>
       <c r="I43" s="7">
         <f t="shared" si="18"/>
-        <v>20544</v>
+        <v>24000</v>
       </c>
       <c r="J43" s="7">
         <f>J42*12</f>
-        <v>24000</v>
+        <v>36480</v>
       </c>
       <c r="K43" s="7">
         <f>K42*12</f>
-        <v>28800</v>
+        <v>43200</v>
       </c>
       <c r="L43" s="7">
         <f>L42*12</f>
-        <v>38400</v>
+        <v>48000</v>
       </c>
       <c r="M43" s="7">
         <f>M42*12</f>
-        <v>48000</v>
+        <v>51840</v>
       </c>
       <c r="N43" s="7">
         <f>N42*12</f>
         <v>55680</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C45" s="7">
         <f t="shared" ref="C45:M45" si="19">C43+C41</f>
@@ -3951,23 +4018,23 @@
       </c>
       <c r="I45" s="7">
         <f t="shared" si="19"/>
-        <v>222560.00000000006</v>
+        <v>260000.00000000006</v>
       </c>
       <c r="J45" s="7">
         <f t="shared" si="19"/>
-        <v>260000.00000000006</v>
+        <v>395200.00000000006</v>
       </c>
       <c r="K45" s="7">
         <f t="shared" si="19"/>
-        <v>312000.00000000006</v>
+        <v>468000.00000000012</v>
       </c>
       <c r="L45" s="7">
         <f t="shared" si="19"/>
-        <v>416000.00000000012</v>
+        <v>520000.00000000012</v>
       </c>
       <c r="M45" s="7">
         <f t="shared" si="19"/>
-        <v>520000.00000000012</v>
+        <v>561600.00000000012</v>
       </c>
       <c r="N45" s="7">
         <f t="shared" ref="N45" si="20">N43+N41</f>
@@ -3985,45 +4052,46 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
-  <dimension ref="A3:J13"/>
+  <dimension ref="A3:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="J3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1">
         <f>C4/7</f>
@@ -4034,45 +4102,45 @@
         <v>76.92307692307692</v>
       </c>
       <c r="D4" s="1">
-        <f>employees!B9</f>
-        <v>2307.6923076923076</v>
+        <f>employees!B11</f>
+        <v>2342.3076923076924</v>
       </c>
       <c r="E4" s="1">
         <f>D4*2</f>
-        <v>4615.3846153846152</v>
+        <v>4684.6153846153848</v>
       </c>
       <c r="F4" s="1">
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1">
         <f>C5/7</f>
-        <v>329.67032967032964</v>
+        <v>334.61538461538464</v>
       </c>
       <c r="C5" s="1">
-        <f>employees!B9</f>
-        <v>2307.6923076923076</v>
+        <f>employees!B11</f>
+        <v>2342.3076923076924</v>
       </c>
       <c r="D5" s="1">
-        <f>employees!B10</f>
-        <v>4615.3846153846152</v>
+        <f>employees!B12</f>
+        <v>4684.6153846153848</v>
       </c>
       <c r="E5" s="1">
         <f>D5*2</f>
-        <v>9230.7692307692305</v>
+        <v>9369.2307692307695</v>
       </c>
       <c r="F5" s="1">
-        <f>employees!B6</f>
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <f>employees!B8</f>
+        <v>121800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1">
         <f>200/30</f>
@@ -4095,9 +4163,9 @@
         <v>2333.3333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1">
         <f>400/30</f>
@@ -4120,9 +4188,9 @@
         <v>4666.666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1">
         <f>100/30</f>
@@ -4145,9 +4213,9 @@
         <v>1166.6666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="1">
         <f>C9/7</f>
@@ -4170,9 +4238,9 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" s="1">
         <f>C10/7</f>
@@ -4194,9 +4262,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" s="1">
         <f>C11/7</f>
@@ -4218,59 +4286,95 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B12" s="1">
         <f>C12/7</f>
-        <v>164.83516483516482</v>
+        <v>631.86813186813185</v>
       </c>
       <c r="C12" s="1">
         <f>F12/52</f>
-        <v>1153.8461538461538</v>
+        <v>4423.0769230769229</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>2307.6923076923076</v>
+        <v>8846.1538461538457</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>4615.3846153846152</v>
+        <v>17692.307692307691</v>
       </c>
       <c r="F12" s="1">
-        <v>60000</v>
+        <f>D16</f>
+        <v>230000</v>
       </c>
       <c r="H12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="1">
         <f>SUM(B4:B12)</f>
-        <v>614.32234432234429</v>
+        <v>1086.3003663003662</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ref="C13:F13" si="1">SUM(C4:C12)</f>
-        <v>4300.2564102564102</v>
+        <v>7604.1025641025644</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>10754.358974358973</v>
+        <v>17396.666666666664</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>21508.717948717946</v>
+        <v>34793.333333333328</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>222166.66666666666</v>
+        <v>393966.66666666663</v>
       </c>
       <c r="H13" s="6">
-        <v>5000</v>
+        <f>F12/12</f>
+        <v>19166.666666666668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="14">
+        <v>17</v>
+      </c>
+      <c r="C16" s="14">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1">
+        <f>B17*C16</f>
+        <v>230000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" s="11">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -4282,40 +4386,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72B0531-F9EA-4BB7-8657-7C884FA8D7D5}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
         <v>106</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -4337,9 +4439,9 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" s="4">
         <v>0.5</v>
@@ -4361,9 +4463,9 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -4385,9 +4487,9 @@
         <v>6750</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="4">
         <v>0.15</v>
@@ -4409,9 +4511,9 @@
         <v>3375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4">
         <v>0.1</v>
@@ -4433,9 +4535,9 @@
         <v>1687.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4">
         <v>0.05</v>
@@ -4457,7 +4559,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -4466,9 +4568,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -4486,9 +4588,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B12" s="1">
         <v>7.5</v>
@@ -4510,66 +4612,66 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B16" s="7">
         <f>B12*B15</f>
         <v>112.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B17" s="7">
         <f>B14*B16</f>
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="9">
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" s="7">
         <f>B17*(B18+1)</f>
         <v>540</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B22" s="7"/>
     </row>
@@ -4580,81 +4682,103 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1">
         <v>45000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B5" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6" s="1">
+        <f>C6*D6</f>
+        <v>1800</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="1">
-        <f>SUM(B2:B5)</f>
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="1">
-        <f>B6/52</f>
-        <v>2307.6923076923076</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" s="1">
-        <f>B6/26</f>
-        <v>4615.3846153846152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <f>SUM(B2:B6)</f>
+        <v>121800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1">
-        <f>B10*2</f>
-        <v>9230.7692307692305</v>
+        <f>B8/52</f>
+        <v>2342.3076923076924</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="1">
+        <f>B8/26</f>
+        <v>4684.6153846153848</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="1">
+        <f>B12*2</f>
+        <v>9369.2307692307695</v>
       </c>
     </row>
   </sheetData>
@@ -4670,15 +4794,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -4689,7 +4813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -4704,7 +4828,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4719,9 +4843,9 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -4735,7 +4859,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -4750,7 +4874,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -4765,7 +4889,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -4780,9 +4904,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B8" s="1">
         <v>300</v>
@@ -4795,7 +4919,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -4817,20 +4941,20 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>38</v>
       </c>
@@ -4841,7 +4965,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4859,7 +4983,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -4877,25 +5001,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D6" s="1">
         <v>3000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D8" s="7">
         <f>D3+D6</f>

</xml_diff>

<commit_message>
before I start working on business registration, I'd like to form a team first. Business registration changes depending on the team.
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2826" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D52A5555-B5C8-4D9D-9ACF-C847B8E263DE}"/>
+  <xr:revisionPtr revIDLastSave="2846" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{37585712-2CE9-46B5-BB9E-86EC3381AE8C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Assumptions_draft" sheetId="27" state="hidden" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="303">
   <si>
     <t>Overhead</t>
   </si>
@@ -953,16 +953,10 @@
     <t>Located in which Account?</t>
   </si>
   <si>
-    <t>Fed Coporate Income Tax Brackets</t>
-  </si>
-  <si>
-    <t>0-50k</t>
-  </si>
-  <si>
-    <t>50-75k</t>
-  </si>
-  <si>
-    <t>75-100k</t>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Summary: The following are scenarios for compounding % increases in the number of engaged community customers per month. The greater number of people we retain in the first month, the less of a struggle it will be to run the business in the future.</t>
   </si>
 </sst>
 </file>
@@ -5094,8 +5088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7438C7-F562-43B8-A4F8-A402353A65B3}">
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5181,26 +5175,13 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>301</v>
-      </c>
       <c r="D6" s="30" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>302</v>
-      </c>
-    </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
@@ -8872,7 +8853,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAAC8DE-41B9-46A0-BE44-EAAB92E58FB4}">
   <dimension ref="A3:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8975,7 +8958,7 @@
         <v>124</v>
       </c>
       <c r="B15" s="7">
-        <f>Operating_Costs!F12</f>
+        <f>Operating_Costs!G12</f>
         <v>366966.66666666663</v>
       </c>
     </row>
@@ -9156,7 +9139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A112772E-1427-43D2-80C2-98741A931E56}">
   <dimension ref="A4:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
@@ -9168,9 +9151,9 @@
     <col min="4" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -9299,7 +9282,7 @@
         <v>169</v>
       </c>
       <c r="B8" s="7">
-        <f>Operating_Costs!F12</f>
+        <f>Operating_Costs!G12</f>
         <v>366966.66666666663</v>
       </c>
       <c r="H8" s="7"/>
@@ -10552,10 +10535,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875F2472-3193-4419-B39A-ACA2F19F890D}">
-  <dimension ref="A3:F19"/>
+  <dimension ref="A3:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10566,10 +10549,11 @@
     <col min="4" max="4" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>95</v>
       </c>
@@ -10583,10 +10567,13 @@
         <v>122</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -10595,7 +10582,7 @@
         <v>10.989010989010989</v>
       </c>
       <c r="C4" s="1">
-        <f>F4/52</f>
+        <f>G4/52</f>
         <v>76.92307692307692</v>
       </c>
       <c r="D4" s="1">
@@ -10607,10 +10594,14 @@
         <v>4684.6153846153848</v>
       </c>
       <c r="F4" s="1">
+        <f>C4*(52/12)</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="G4" s="1">
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -10631,11 +10622,15 @@
         <v>9369.2307692307695</v>
       </c>
       <c r="F5" s="1">
+        <f t="shared" ref="F5:F12" si="0">C5*(52/12)</f>
+        <v>10150</v>
+      </c>
+      <c r="G5" s="1">
         <f>employees!B8</f>
         <v>121800</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -10656,11 +10651,15 @@
         <v>186.66666666666669</v>
       </c>
       <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>202.22222222222223</v>
+      </c>
+      <c r="G6" s="1">
         <f>C6*50</f>
         <v>2333.3333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -10681,11 +10680,15 @@
         <v>373.33333333333337</v>
       </c>
       <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>404.44444444444446</v>
+      </c>
+      <c r="G7" s="1">
         <f>C7*50</f>
         <v>4666.666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -10706,11 +10709,15 @@
         <v>93.333333333333343</v>
       </c>
       <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>101.11111111111111</v>
+      </c>
+      <c r="G8" s="1">
         <f>C8*50</f>
         <v>1166.6666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -10722,19 +10729,23 @@
         <v>20</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D9:E11" si="0">C9*2</f>
+        <f t="shared" ref="D9:E11" si="1">C9*2</f>
         <v>40</v>
       </c>
       <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="F9" s="1">
+        <v>86.666666666666657</v>
+      </c>
+      <c r="G9" s="1">
         <f>C9*50</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -10743,22 +10754,26 @@
         <v>5.4945054945054945</v>
       </c>
       <c r="C10" s="1">
-        <f>F10/52</f>
+        <f>G10/52</f>
         <v>38.46153846153846</v>
       </c>
       <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>76.92307692307692</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>153.84615384615384</v>
+      </c>
+      <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>76.92307692307692</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>153.84615384615384</v>
-      </c>
-      <c r="F10" s="1">
+        <v>166.66666666666666</v>
+      </c>
+      <c r="G10" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>210</v>
       </c>
@@ -10767,23 +10782,27 @@
         <v>631.86813186813185</v>
       </c>
       <c r="C11" s="1">
-        <f>F11/52</f>
+        <f>G11/52</f>
         <v>4423.0769230769229</v>
       </c>
       <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>8846.1538461538457</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>17692.307692307691</v>
+      </c>
+      <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>8846.1538461538457</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>17692.307692307691</v>
-      </c>
-      <c r="F11" s="1">
+        <v>19166.666666666664</v>
+      </c>
+      <c r="G11" s="1">
         <f>D15</f>
         <v>230000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -10792,23 +10811,27 @@
         <v>1009.1575091575091</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" ref="C12:F12" si="1">SUM(C4:C11)</f>
+        <f t="shared" ref="C12:F12" si="2">SUM(C4:C11)</f>
         <v>7064.1025641025644</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16316.666666666668</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32633.333333333336</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>30611.111111111109</v>
+      </c>
+      <c r="G12" s="1">
+        <f>SUM(G4:G11)</f>
         <v>366966.66666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>246</v>
       </c>
@@ -10819,7 +10842,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>250</v>
       </c>
@@ -10834,7 +10857,7 @@
         <v>230000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -10847,7 +10870,7 @@
         <v>211</v>
       </c>
       <c r="B17" s="6">
-        <f>F11/12</f>
+        <f>G11/12</f>
         <v>19166.666666666668</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on finances a bit. Added connections. Included dishwasher, removed gas ranges, added induction cooking, removed expensive ventilation. I need to create an email loop.
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2846" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{37585712-2CE9-46B5-BB9E-86EC3381AE8C}"/>
+  <xr:revisionPtr revIDLastSave="2912" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{66EBD01C-DFC4-4C60-AFD2-9DDA64F39633}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="12" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Assumptions_draft" sheetId="27" state="hidden" r:id="rId1"/>
     <sheet name="Community_Engagement" sheetId="28" state="hidden" r:id="rId2"/>
     <sheet name="Revenue_Profit_Balance" sheetId="19" r:id="rId3"/>
-    <sheet name="Sources_of_Funds" sheetId="23" r:id="rId4"/>
+    <sheet name="Funding_And_Connections" sheetId="23" r:id="rId4"/>
     <sheet name="Comprehensive" sheetId="3" r:id="rId5"/>
     <sheet name="Overhead" sheetId="2" r:id="rId6"/>
     <sheet name="Net_And_Analysis" sheetId="18" r:id="rId7"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="321">
   <si>
     <t>Overhead</t>
   </si>
@@ -692,15 +692,6 @@
     <t>Business Management/Maintenance</t>
   </si>
   <si>
-    <t>gas range</t>
-  </si>
-  <si>
-    <t>range hoods</t>
-  </si>
-  <si>
-    <t>hood installations</t>
-  </si>
-  <si>
     <t>White board and markers</t>
   </si>
   <si>
@@ -957,6 +948,69 @@
   </si>
   <si>
     <t>Summary: The following are scenarios for compounding % increases in the number of engaged community customers per month. The greater number of people we retain in the first month, the less of a struggle it will be to run the business in the future.</t>
+  </si>
+  <si>
+    <t>electric induction cooking range and oven</t>
+  </si>
+  <si>
+    <t>big dishwasher</t>
+  </si>
+  <si>
+    <t>Tier 2 Investors</t>
+  </si>
+  <si>
+    <t>Tier 1 Investors</t>
+  </si>
+  <si>
+    <t>Sweat Equity</t>
+  </si>
+  <si>
+    <t>Contributions</t>
+  </si>
+  <si>
+    <t>Tier 3 Investors</t>
+  </si>
+  <si>
+    <t>keep updated</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Brenton Brown</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>landscaping company owner</t>
+  </si>
+  <si>
+    <t>brentonb050@gmail.com</t>
+  </si>
+  <si>
+    <t>psychology grad student</t>
+  </si>
+  <si>
+    <t>Ray Charles Capanzana</t>
+  </si>
+  <si>
+    <t>rayccpnzn@gmail.com</t>
+  </si>
+  <si>
+    <t>ernohott@gmail.com</t>
+  </si>
+  <si>
+    <t>Erno</t>
+  </si>
+  <si>
+    <t>Mom's friend</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>fb</t>
   </si>
 </sst>
 </file>
@@ -3162,7 +3216,7 @@
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B2" s="4">
         <v>0.13</v>
@@ -3170,21 +3224,21 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="L3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B4">
         <v>36</v>
@@ -3221,7 +3275,7 @@
         <v>407.18706153581047</v>
       </c>
       <c r="F7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G7">
         <f>Gross!J30</f>
@@ -3244,16 +3298,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -3264,7 +3318,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3878,10 +3932,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3902,7 +3956,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B5" s="1">
         <v>25000</v>
@@ -3910,7 +3964,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B6" s="1">
         <f>C6*D6</f>
@@ -4023,7 +4077,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>
@@ -4084,7 +4138,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B8" s="1">
         <v>300</v>
@@ -4115,8 +4169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6007EBCF-A6A9-4054-90A6-E709ADB7E2B5}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4189,7 +4243,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D6" s="1">
         <v>3000</v>
@@ -4197,7 +4251,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D8" s="7">
         <f>D3+D6</f>
@@ -4211,13 +4265,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560605D-AE6F-456E-B5FE-7223BF3283FD}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
@@ -4248,7 +4304,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B2" s="1">
         <v>55</v>
@@ -4273,7 +4329,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1">
         <v>2000</v>
@@ -4312,7 +4368,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" ref="G5:G16" si="0">B5*C5</f>
+        <f t="shared" ref="G5:G9" si="0">B5*C5</f>
         <v>200</v>
       </c>
     </row>
@@ -4333,7 +4389,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>300</v>
       </c>
       <c r="B7" s="1">
         <v>1000</v>
@@ -4348,147 +4404,131 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B8" s="1">
-        <v>8000</v>
+        <v>3900</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>301</v>
       </c>
       <c r="B9" s="1">
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="C9">
-        <f>C7</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1">
-        <v>3900</v>
+        <v>1000</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" si="0"/>
-        <v>3900</v>
+        <f>B10*C10</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="G11" s="7">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <f>B11*C11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G12" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B12*C12</f>
+        <v>600</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="0"/>
-        <v>600</v>
+        <f>B13*C13</f>
+        <v>750</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1">
-        <v>250</v>
+        <v>80</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="0"/>
-        <v>750</v>
+        <f>B14*C14</f>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>240</v>
       </c>
       <c r="B15" s="1">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15" s="7">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>243</v>
-      </c>
-      <c r="B16" s="1">
+        <f>B15*C15</f>
         <v>100</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="7">
-        <f>SUM(G2:G16)</f>
-        <v>47315</v>
+      <c r="G18" s="7">
+        <f>SUM(G2:G15)</f>
+        <v>33315</v>
       </c>
     </row>
   </sheetData>
@@ -5089,7 +5129,7 @@
   <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5117,76 +5157,76 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B1" s="15">
         <f>Key_Assumptions_draft!G7</f>
         <v>355</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B2" s="15">
         <f>Gross!N30</f>
         <v>600</v>
       </c>
       <c r="C2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B3" s="16">
         <f>Overhead!B15/12</f>
         <v>30580.555555555551</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B4" s="16">
         <f>Overhead!B18</f>
         <v>183483.33333333331</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D6" s="30" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B13" s="32">
         <v>0.5</v>
@@ -5206,7 +5246,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B14" s="33">
         <f>B17</f>
@@ -5231,7 +5271,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B15" s="31">
         <v>9</v>
@@ -5251,67 +5291,67 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G16" t="s">
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="L16" t="s">
         <v>4</v>
       </c>
       <c r="M16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="N16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="O16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="Q16" t="s">
         <v>4</v>
       </c>
       <c r="R16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="S16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="T16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="V16" t="s">
         <v>4</v>
       </c>
       <c r="W16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="X16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="Y16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
@@ -8527,69 +8567,153 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1ED5F7-7D0A-4613-B246-76BB506BCE91}">
-  <dimension ref="A3:F19"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H1" t="s">
+        <v>303</v>
+      </c>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E2" t="s">
         <v>295</v>
       </c>
-      <c r="D3" t="s">
-        <v>296</v>
-      </c>
-      <c r="E3" t="s">
-        <v>298</v>
-      </c>
-      <c r="F3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F2" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
+      <c r="J6" t="s">
+        <v>306</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="L6" t="s">
+        <v>319</v>
+      </c>
+      <c r="M6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>307</v>
+      </c>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>309</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="L8" t="s">
+        <v>320</v>
+      </c>
+      <c r="M8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="J9" t="s">
+        <v>314</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="L9" t="s">
+        <v>320</v>
+      </c>
+      <c r="M9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>317</v>
+      </c>
+      <c r="K10" t="s">
+        <v>316</v>
+      </c>
+      <c r="L10" t="s">
+        <v>320</v>
+      </c>
+      <c r="M10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>294</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K8" r:id="rId1" xr:uid="{07E53557-BDF7-4F7E-9ECE-28FFB50A67B4}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{5581E50E-8D2A-4C99-848C-B9855F0143A5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8598,8 +8722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D328D9-1DCE-4B51-AE60-9CCAF40EB9F8}">
   <dimension ref="A3:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8681,10 +8805,10 @@
         <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -8697,7 +8821,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B15" s="11">
         <v>58809</v>
@@ -8705,7 +8829,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B16" s="11">
         <v>56453</v>
@@ -8713,7 +8837,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B17" s="11">
         <v>58645</v>
@@ -8721,7 +8845,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B18" s="11">
         <v>49754</v>
@@ -8729,7 +8853,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B19" s="11">
         <v>50741</v>
@@ -8737,7 +8861,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B20" s="11">
         <v>54969</v>
@@ -8745,7 +8869,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B21" s="11">
         <v>59755</v>
@@ -8753,7 +8877,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B22" s="11">
         <v>59073</v>
@@ -8761,7 +8885,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B23" s="11">
         <v>60768</v>
@@ -8769,7 +8893,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B24" s="11">
         <v>45951</v>
@@ -8777,7 +8901,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B25" s="11">
         <v>37199</v>
@@ -8816,7 +8940,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B32" s="11">
         <v>620000</v>
@@ -8867,7 +8991,7 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B3" s="7">
         <f>PCs!D12</f>
@@ -8876,7 +9000,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B4" s="7">
         <f>Dance_Studio!D8</f>
@@ -8888,8 +9012,8 @@
         <v>76</v>
       </c>
       <c r="B5" s="7">
-        <f>Kitchen!G20</f>
-        <v>47315</v>
+        <f>Kitchen!G18</f>
+        <v>33315</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -8925,12 +9049,12 @@
       </c>
       <c r="B10" s="7">
         <f>SUM(B3:B8)</f>
-        <v>87645</v>
+        <v>73645</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B11" s="6">
         <v>2000</v>
@@ -8938,7 +9062,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B12" s="1">
         <v>10000</v>
@@ -8946,11 +9070,11 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B13" s="7">
         <f>SUM(B10:B12)</f>
-        <v>99645</v>
+        <v>85645</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -9016,7 +9140,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B18" s="7">
         <f t="shared" ref="B18:G18" si="1">$B$15*B$17</f>
@@ -9050,27 +9174,27 @@
       </c>
       <c r="B19" s="7">
         <f>$B$10+($B$15*B$17)+$B$12+$B$11</f>
-        <v>283128.33333333331</v>
+        <v>269128.33333333331</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:G19" si="2">$B$10+($B$15*C$17)+$B$12+$B$11</f>
-        <v>252547.77777777778</v>
+        <v>238547.77777777778</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="2"/>
-        <v>221967.22222222219</v>
+        <v>207967.22222222219</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="2"/>
-        <v>191386.66666666666</v>
+        <v>177386.66666666666</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="2"/>
-        <v>160806.11111111109</v>
+        <v>146806.11111111109</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="2"/>
-        <v>130225.55555555555</v>
+        <v>116225.55555555555</v>
       </c>
       <c r="H19" s="7"/>
     </row>
@@ -9119,7 +9243,7 @@
         <v>204</v>
       </c>
       <c r="B27" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -9139,8 +9263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A112772E-1427-43D2-80C2-98741A931E56}">
   <dimension ref="A4:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9158,7 +9282,7 @@
   <sheetData>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I4" s="15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M4" s="17" t="s">
         <v>174</v>
@@ -9479,7 +9603,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B29">
         <f>C17-B28</f>
@@ -9779,7 +9903,7 @@
         <v>0.25600000000000006</v>
       </c>
       <c r="L23" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -9796,7 +9920,7 @@
         <v>1.1200000000000003</v>
       </c>
       <c r="K24" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L24" s="19">
         <f>$B$31*($G$20+$G$21)+$B$33*($G$22+$G$23)</f>
@@ -9824,7 +9948,7 @@
         <v>3</v>
       </c>
       <c r="K25" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="L25" s="3">
         <f>A25*B42</f>
@@ -9850,7 +9974,7 @@
         <v>5</v>
       </c>
       <c r="K26" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="L26">
         <f>52/12</f>
@@ -9863,7 +9987,7 @@
         <v>0.20000000000000004</v>
       </c>
       <c r="K27" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="L27">
         <f>L24*L26+L25</f>
@@ -10538,7 +10662,7 @@
   <dimension ref="A3:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10567,7 +10691,7 @@
         <v>122</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>97</v>
@@ -10811,7 +10935,7 @@
         <v>1009.1575091575091</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" ref="C12:F12" si="2">SUM(C4:C11)</f>
+        <f t="shared" ref="C12:E12" si="2">SUM(C4:C11)</f>
         <v>7064.1025641025644</v>
       </c>
       <c r="D12" s="1">
@@ -10833,18 +10957,18 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B15" s="14">
         <v>17</v>
@@ -10859,7 +10983,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B16" s="11">
         <v>10000</v>
@@ -10881,7 +11005,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Scott's email. He likes the idea.
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2912" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{66EBD01C-DFC4-4C60-AFD2-9DDA64F39633}"/>
+  <xr:revisionPtr revIDLastSave="2918" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{F97758D7-8735-47C5-9069-46DFD3906E9D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="12" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Assumptions_draft" sheetId="27" state="hidden" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="325">
   <si>
     <t>Overhead</t>
   </si>
@@ -1011,6 +1011,18 @@
   </si>
   <si>
     <t>fb</t>
+  </si>
+  <si>
+    <t>swermann@gmail.com </t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>MHK senior co-worker</t>
+  </si>
+  <si>
+    <t>Scott Wermann</t>
   </si>
 </sst>
 </file>
@@ -4169,7 +4181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6007EBCF-A6A9-4054-90A6-E709ADB7E2B5}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -4443,7 +4455,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="7">
-        <f>B10*C10</f>
+        <f t="shared" ref="G10:G15" si="1">B10*C10</f>
         <v>1000</v>
       </c>
     </row>
@@ -4458,7 +4470,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="7">
-        <f>B11*C11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4473,7 +4485,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="7">
-        <f>B12*C12</f>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
@@ -4488,7 +4500,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="7">
-        <f>B13*C13</f>
+        <f t="shared" si="1"/>
         <v>750</v>
       </c>
     </row>
@@ -4503,7 +4515,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="7">
-        <f>B14*C14</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
     </row>
@@ -4518,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="7">
-        <f>B15*C15</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -8569,8 +8581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1ED5F7-7D0A-4613-B246-76BB506BCE91}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8692,6 +8704,20 @@
       </c>
       <c r="M10" t="s">
         <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>324</v>
+      </c>
+      <c r="K11" t="s">
+        <v>321</v>
+      </c>
+      <c r="L11" t="s">
+        <v>322</v>
+      </c>
+      <c r="M11" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Working on the real financial projections Spreadsheet
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2918" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{F97758D7-8735-47C5-9069-46DFD3906E9D}"/>
+  <xr:revisionPtr revIDLastSave="3078" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4CBC68A-467C-48AB-83A7-CC7DBCC1979C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="740" firstSheet="3" activeTab="7" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Assumptions_draft" sheetId="27" state="hidden" r:id="rId1"/>
@@ -24,13 +24,16 @@
     <sheet name="Operating_Costs" sheetId="4" r:id="rId9"/>
     <sheet name="food" sheetId="15" state="hidden" r:id="rId10"/>
     <sheet name="employees" sheetId="10" r:id="rId11"/>
-    <sheet name="PCs" sheetId="7" r:id="rId12"/>
-    <sheet name="Dance_Studio" sheetId="8" r:id="rId13"/>
-    <sheet name="Kitchen" sheetId="9" r:id="rId14"/>
-    <sheet name="Liabilities" sheetId="12" r:id="rId15"/>
-    <sheet name="Eating Area" sheetId="13" r:id="rId16"/>
-    <sheet name="decor" sheetId="11" r:id="rId17"/>
-    <sheet name="Initial" sheetId="1" r:id="rId18"/>
+    <sheet name="Leasehold_Improvements" sheetId="29" r:id="rId12"/>
+    <sheet name="PCs" sheetId="7" r:id="rId13"/>
+    <sheet name="Equipment" sheetId="30" r:id="rId14"/>
+    <sheet name="Furniture_and_Fixtures" sheetId="31" r:id="rId15"/>
+    <sheet name="Dance_Studio" sheetId="8" r:id="rId16"/>
+    <sheet name="Kitchen" sheetId="9" r:id="rId17"/>
+    <sheet name="Liabilities" sheetId="12" r:id="rId18"/>
+    <sheet name="Eating Area" sheetId="13" r:id="rId19"/>
+    <sheet name="decor" sheetId="11" r:id="rId20"/>
+    <sheet name="Initial" sheetId="1" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="344">
   <si>
     <t>Overhead</t>
   </si>
@@ -1023,6 +1026,63 @@
   </si>
   <si>
     <t>Scott Wermann</t>
+  </si>
+  <si>
+    <t>Leasehold Improvements</t>
+  </si>
+  <si>
+    <t>Improvement</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Equipment Costs</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>PC and Gaming</t>
+  </si>
+  <si>
+    <t>Eating Area</t>
+  </si>
+  <si>
+    <t>All equipment are improvements</t>
+  </si>
+  <si>
+    <t>speakers don't need to be included because usually people bring their own.</t>
+  </si>
+  <si>
+    <t>Décor</t>
+  </si>
+  <si>
+    <t>Furniture and Fixtures</t>
+  </si>
+  <si>
+    <t>Furniture or Fixture</t>
+  </si>
+  <si>
+    <t>Eating</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>maybe a disco ball for fun someday</t>
+  </si>
+  <si>
+    <t>none since this is all furniture</t>
+  </si>
+  <si>
+    <t>six months salary combined</t>
+  </si>
+  <si>
+    <t>per week</t>
+  </si>
+  <si>
+    <t>per hour</t>
   </si>
 </sst>
 </file>
@@ -3926,9 +3986,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1068B3A-A81C-4168-AA3E-DAD4781E4B82}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3937,44 +3999,74 @@
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>250</v>
       </c>
       <c r="D2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>213</v>
       </c>
       <c r="B3" s="1">
         <v>50000</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G3" s="7">
+        <f>B3/51</f>
+        <v>980.39215686274508</v>
+      </c>
+      <c r="H3" s="7">
+        <f>G3/40</f>
+        <v>24.509803921568626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="1">
         <v>45000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G4" s="7">
+        <f>B4/51</f>
+        <v>882.35294117647061</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" ref="H4:H5" si="0">G4/40</f>
+        <v>22.058823529411764</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>234</v>
       </c>
       <c r="B5" s="1">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18000</v>
+      </c>
+      <c r="G5" s="7">
+        <f>B5/51</f>
+        <v>352.94117647058823</v>
+      </c>
+      <c r="H5" s="7">
+        <f>G5/16</f>
+        <v>22.058823529411764</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>249</v>
       </c>
@@ -3989,40 +4081,49 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="1">
         <f>SUM(B2:B6)</f>
-        <v>121800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>114800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>93</v>
       </c>
       <c r="B11" s="1">
         <f>B8/52</f>
-        <v>2342.3076923076924</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2207.6923076923076</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>94</v>
       </c>
       <c r="B12" s="1">
         <f>B8/26</f>
-        <v>4684.6153846153848</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4415.3846153846152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="1">
         <f>B12*2</f>
-        <v>9369.2307692307695</v>
+        <v>8830.7692307692305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>341</v>
+      </c>
+      <c r="B18" s="1">
+        <f>B8*0.5</f>
+        <v>57400</v>
       </c>
     </row>
   </sheetData>
@@ -4031,11 +4132,132 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F82D85A-4F0C-4E7C-B387-6C1D4414D45A}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="str">
+        <f>Kitchen!A2</f>
+        <v>granite counter tops per sq foot</v>
+      </c>
+      <c r="C3" s="7">
+        <f>Kitchen!G2</f>
+        <v>5325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="str">
+        <f>Kitchen!A3</f>
+        <v>counter installation</v>
+      </c>
+      <c r="C4" s="7">
+        <f>Kitchen!G3</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="str">
+        <f>Kitchen!A4</f>
+        <v>double basin sinks</v>
+      </c>
+      <c r="C5" s="7">
+        <f>Kitchen!G4</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="str">
+        <f>Kitchen!A5</f>
+        <v>Electrical outlets</v>
+      </c>
+      <c r="C6" s="7">
+        <f>Kitchen!G5</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="str">
+        <f>Kitchen!A6</f>
+        <v>sink installation and plumbing</v>
+      </c>
+      <c r="C7" s="7">
+        <f>Kitchen!G6</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="str">
+        <f>Dance_Studio!A3</f>
+        <v>sprung wood flooring per square feet</v>
+      </c>
+      <c r="C9" s="7">
+        <f>Dance_Studio!D3</f>
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="str">
+        <f>Dance_Studio!A6</f>
+        <v>mirror</v>
+      </c>
+      <c r="C10" s="7">
+        <f>Dance_Studio!D6</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="7">
+        <f>SUM(C3:C11)</f>
+        <v>35225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E8F79C-848E-45C7-B440-BCF016365DF9}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4177,7 +4399,384 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEA9098-80F9-4D65-B579-EC820EC08891}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="str">
+        <f>Kitchen!A10</f>
+        <v>shared kitchen appliances</v>
+      </c>
+      <c r="C3" s="7">
+        <f>Kitchen!G10</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="str">
+        <f>Kitchen!A11</f>
+        <v>plates and utensils</v>
+      </c>
+      <c r="C4" s="7">
+        <f>Kitchen!G11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="str">
+        <f>Kitchen!A12</f>
+        <v>kitchen shelves</v>
+      </c>
+      <c r="C5" s="7">
+        <f>Kitchen!G12</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="str">
+        <f>Kitchen!A13</f>
+        <v>stainless steel cookware</v>
+      </c>
+      <c r="C6" s="7">
+        <f>Kitchen!G13</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="str">
+        <f>Kitchen!A14</f>
+        <v>knives</v>
+      </c>
+      <c r="C7" s="7">
+        <f>Kitchen!G14</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="str">
+        <f>Kitchen!A15</f>
+        <v>knife sharpener</v>
+      </c>
+      <c r="C8" s="7">
+        <f>Kitchen!G15</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>330</v>
+      </c>
+      <c r="B13" t="str">
+        <f>PCs!A5</f>
+        <v>Games fund</v>
+      </c>
+      <c r="C13" s="7">
+        <f>PCs!D5</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <f>PCs!A6</f>
+        <v>Cleaning Supplies</v>
+      </c>
+      <c r="C14" s="7">
+        <f>PCs!D6</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <f>PCs!A7</f>
+        <v>Wifi</v>
+      </c>
+      <c r="C15" s="7">
+        <f>PCs!D7</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" t="s">
+        <v>340</v>
+      </c>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>334</v>
+      </c>
+      <c r="B19" t="str">
+        <f>decor!A2</f>
+        <v>paint per 1 gal</v>
+      </c>
+      <c r="C19" s="7">
+        <f>decor!K2</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <f>decor!A3</f>
+        <v>decorations</v>
+      </c>
+      <c r="C20" s="7">
+        <f>decor!K3</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <f>decor!A4</f>
+        <v>cleaning supplies</v>
+      </c>
+      <c r="C21" s="7">
+        <f>decor!K4</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="7">
+        <f>SUM(C3:C21)</f>
+        <v>4290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E1ED6D-054C-4B7C-A88D-F5493FF873D6}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="str">
+        <f>Kitchen!A7</f>
+        <v>electric induction cooking range and oven</v>
+      </c>
+      <c r="C4" s="7">
+        <f>Kitchen!G7</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="str">
+        <f>Kitchen!A8</f>
+        <v>three-door fridge</v>
+      </c>
+      <c r="C5" s="7">
+        <f>Kitchen!G8</f>
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="str">
+        <f>Kitchen!A9</f>
+        <v>big dishwasher</v>
+      </c>
+      <c r="C6" s="7">
+        <f>Kitchen!G9</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>337</v>
+      </c>
+      <c r="B11" t="str">
+        <f>'Eating Area'!A3</f>
+        <v>chairs</v>
+      </c>
+      <c r="C11" s="7">
+        <f>'Eating Area'!F3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <f>'Eating Area'!A4</f>
+        <v>8 seater tables</v>
+      </c>
+      <c r="C12" s="7">
+        <f>'Eating Area'!F4</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <f>'Eating Area'!A5</f>
+        <v>4 seater tables</v>
+      </c>
+      <c r="C13" s="7">
+        <f>'Eating Area'!F5</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <f>'Eating Area'!A6</f>
+        <v>2 seater tables</v>
+      </c>
+      <c r="C14" s="7">
+        <f>'Eating Area'!F6</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>330</v>
+      </c>
+      <c r="B16" t="str">
+        <f>PCs!A2</f>
+        <v>per PC, accessories, and software</v>
+      </c>
+      <c r="C16" s="7">
+        <f>PCs!D2</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="str">
+        <f>PCs!A3</f>
+        <v>long table, fits three PCs, 3x8 ft^2 design</v>
+      </c>
+      <c r="C17" s="7">
+        <f>PCs!D3</f>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <f>PCs!A4</f>
+        <v>Comfy office chairs</v>
+      </c>
+      <c r="C18" s="7">
+        <f>PCs!D4</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <f>PCs!A8</f>
+        <v>White board and markers</v>
+      </c>
+      <c r="C19" s="7">
+        <f>PCs!D8</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="7">
+        <f>SUM(C4:C20)</f>
+        <v>33980</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6007EBCF-A6A9-4054-90A6-E709ADB7E2B5}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -4275,7 +4874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560605D-AE6F-456E-B5FE-7223BF3283FD}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -4548,7 +5147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36F18DE-64EC-418D-B15A-DB7866B424E3}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -4596,7 +5195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725D3AE5-3953-4739-93F6-EFB9BCC1B4E0}">
   <dimension ref="A2:F10"/>
   <sheetViews>
@@ -4732,7 +5331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A6F31-02C3-4DB3-8520-6CC51B52F01A}">
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -4856,292 +5455,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E200A4BF-7444-461A-A7D9-DCB85EAD9C4B}">
-  <dimension ref="A2:C38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1">
-        <v>700</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1">
-        <f>B4*B3</f>
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1">
-        <f>B5*4</f>
-        <v>8400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1">
-        <f>B5*51</f>
-        <v>107100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <f>SUM(B8:B12)</f>
-        <v>5700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1">
-        <f>B13*12+B7</f>
-        <v>175500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="1">
-        <f>B19*B25*B26*B22</f>
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="5">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="1">
-        <f>B22*B18*B29*B30</f>
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="1">
-        <f>B27+B31</f>
-        <v>15750</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="1">
-        <f>B33*4</f>
-        <v>63000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="1">
-        <f>B33*51</f>
-        <v>803250</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="1">
-        <f>B35*0.25</f>
-        <v>200812.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="1">
-        <f>B35-B36</f>
-        <v>602437.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="1">
-        <f>B37-B14</f>
-        <v>426937.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7438C7-F562-43B8-A4F8-A402353A65B3}">
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5200,7 +5519,7 @@
       </c>
       <c r="B3" s="16">
         <f>Overhead!B15/12</f>
-        <v>30580.555555555551</v>
+        <v>29997.222222222223</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>281</v>
@@ -5212,7 +5531,7 @@
       </c>
       <c r="B4" s="16">
         <f>Overhead!B18</f>
-        <v>183483.33333333331</v>
+        <v>179983.33333333334</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>270</v>
@@ -5379,11 +5698,11 @@
       </c>
       <c r="D17" s="7">
         <f t="shared" ref="D17:D53" si="0">C17-$B$3</f>
-        <v>-29233.35555555555</v>
+        <v>-28650.022222222222</v>
       </c>
       <c r="E17" s="7">
         <f>D17</f>
-        <v>-29233.35555555555</v>
+        <v>-28650.022222222222</v>
       </c>
       <c r="G17" s="20">
         <v>25</v>
@@ -5394,11 +5713,11 @@
       </c>
       <c r="I17" s="7">
         <f t="shared" ref="I17:I53" si="1">H17-$B$3</f>
-        <v>-28335.222222222219</v>
+        <v>-27751.888888888891</v>
       </c>
       <c r="J17" s="7">
         <f>I17</f>
-        <v>-28335.222222222219</v>
+        <v>-27751.888888888891</v>
       </c>
       <c r="L17" s="20">
         <v>35</v>
@@ -5409,11 +5728,11 @@
       </c>
       <c r="N17" s="7">
         <f t="shared" ref="N17:N53" si="2">M17-$B$3</f>
-        <v>-27437.088888888884</v>
+        <v>-26853.755555555555</v>
       </c>
       <c r="O17" s="7">
         <f>N17</f>
-        <v>-27437.088888888884</v>
+        <v>-26853.755555555555</v>
       </c>
       <c r="Q17" s="20">
         <v>55</v>
@@ -5424,11 +5743,11 @@
       </c>
       <c r="S17" s="7">
         <f t="shared" ref="S17:S53" si="3">R17-$B$3</f>
-        <v>-25640.822222222218</v>
+        <v>-25057.488888888889</v>
       </c>
       <c r="T17" s="7">
         <f>S17</f>
-        <v>-25640.822222222218</v>
+        <v>-25057.488888888889</v>
       </c>
       <c r="V17" s="11">
         <v>100</v>
@@ -5439,11 +5758,11 @@
       </c>
       <c r="X17" s="7">
         <f t="shared" ref="X17:X53" si="4">W17-$B$3</f>
-        <v>-21599.222222222215</v>
+        <v>-21015.888888888887</v>
       </c>
       <c r="Y17" s="7">
         <f>X17</f>
-        <v>-21599.222222222215</v>
+        <v>-21015.888888888887</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
@@ -5460,11 +5779,11 @@
       </c>
       <c r="D18" s="7">
         <f t="shared" si="0"/>
-        <v>-28559.755555555552</v>
+        <v>-27976.422222222223</v>
       </c>
       <c r="E18" s="7">
         <f>E17+D18</f>
-        <v>-57793.111111111102</v>
+        <v>-56626.444444444445</v>
       </c>
       <c r="G18" s="20">
         <f t="shared" ref="G18:G53" si="6">G17*(1+$G$13)</f>
@@ -5476,11 +5795,11 @@
       </c>
       <c r="I18" s="7">
         <f t="shared" si="1"/>
-        <v>-27437.088888888884</v>
+        <v>-26853.755555555555</v>
       </c>
       <c r="J18" s="7">
         <f>J17+I18</f>
-        <v>-55772.311111111107</v>
+        <v>-54605.64444444445</v>
       </c>
       <c r="L18" s="20">
         <f t="shared" ref="L18:L53" si="7">L17*(1+$L$13)</f>
@@ -5492,11 +5811,11 @@
       </c>
       <c r="N18" s="7">
         <f t="shared" si="2"/>
-        <v>-26494.048888888883</v>
+        <v>-25910.715555555555</v>
       </c>
       <c r="O18" s="7">
         <f>O17+N18</f>
-        <v>-53931.137777777767</v>
+        <v>-52764.47111111111</v>
       </c>
       <c r="Q18" s="20">
         <f t="shared" ref="Q18:Q53" si="8">Q17*(1+$Q$13)</f>
@@ -5508,11 +5827,11 @@
       </c>
       <c r="S18" s="7">
         <f t="shared" si="3"/>
-        <v>-24652.875555555547</v>
+        <v>-24069.542222222219</v>
       </c>
       <c r="T18" s="7">
         <f>T17+S18</f>
-        <v>-50293.697777777765</v>
+        <v>-49127.031111111108</v>
       </c>
       <c r="V18" s="11">
         <f t="shared" ref="V18:V53" si="9">V17*(1+$V$13)</f>
@@ -5524,11 +5843,11 @@
       </c>
       <c r="X18" s="7">
         <f t="shared" si="4"/>
-        <v>-20701.08888888888</v>
+        <v>-20117.755555555552</v>
       </c>
       <c r="Y18" s="7">
         <f>Y17+X18</f>
-        <v>-42300.311111111092</v>
+        <v>-41133.644444444435</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
@@ -5545,11 +5864,11 @@
       </c>
       <c r="D19" s="7">
         <f t="shared" si="0"/>
-        <v>-27549.35555555555</v>
+        <v>-26966.022222222222</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" ref="E19:E53" si="10">E18+D19</f>
-        <v>-85342.466666666645</v>
+        <v>-83592.466666666674</v>
       </c>
       <c r="G19" s="20">
         <f t="shared" si="6"/>
@@ -5561,11 +5880,11 @@
       </c>
       <c r="I19" s="7">
         <f t="shared" si="1"/>
-        <v>-26179.702222222215</v>
+        <v>-25596.368888888886</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" ref="J19:J53" si="11">J18+I19</f>
-        <v>-81952.013333333321</v>
+        <v>-80202.013333333336</v>
       </c>
       <c r="L19" s="20">
         <f t="shared" si="7"/>
@@ -5577,11 +5896,11 @@
       </c>
       <c r="N19" s="7">
         <f t="shared" si="2"/>
-        <v>-25268.096888888882</v>
+        <v>-24684.763555555553</v>
       </c>
       <c r="O19" s="7">
         <f t="shared" ref="O19:O53" si="12">O18+N19</f>
-        <v>-79199.234666666656</v>
+        <v>-77449.234666666656</v>
       </c>
       <c r="Q19" s="20">
         <f t="shared" si="8"/>
@@ -5593,11 +5912,11 @@
       </c>
       <c r="S19" s="7">
         <f t="shared" si="3"/>
-        <v>-23467.339555555547</v>
+        <v>-22884.006222222219</v>
       </c>
       <c r="T19" s="7">
         <f t="shared" ref="T19:T53" si="13">T18+S19</f>
-        <v>-73761.037333333312</v>
+        <v>-72011.037333333326</v>
       </c>
       <c r="V19" s="11">
         <f t="shared" si="9"/>
@@ -5609,11 +5928,11 @@
       </c>
       <c r="X19" s="7">
         <f t="shared" si="4"/>
-        <v>-19713.14222222221</v>
+        <v>-19129.808888888881</v>
       </c>
       <c r="Y19" s="7">
         <f t="shared" ref="Y19:Y53" si="14">Y18+X19</f>
-        <v>-62013.453333333302</v>
+        <v>-60263.453333333317</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
@@ -5630,11 +5949,11 @@
       </c>
       <c r="D20" s="7">
         <f t="shared" si="0"/>
-        <v>-26033.755555555552</v>
+        <v>-25450.422222222223</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="10"/>
-        <v>-111376.22222222219</v>
+        <v>-109042.88888888891</v>
       </c>
       <c r="G20" s="20">
         <f t="shared" si="6"/>
@@ -5646,11 +5965,11 @@
       </c>
       <c r="I20" s="7">
         <f t="shared" si="1"/>
-        <v>-24419.360888888885</v>
+        <v>-23836.027555555556</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="11"/>
-        <v>-106371.37422222221</v>
+        <v>-104038.04088888889</v>
       </c>
       <c r="L20" s="20">
         <f t="shared" si="7"/>
@@ -5662,11 +5981,11 @@
       </c>
       <c r="N20" s="7">
         <f t="shared" si="2"/>
-        <v>-23674.359288888882</v>
+        <v>-23091.025955555553</v>
       </c>
       <c r="O20" s="7">
         <f t="shared" si="12"/>
-        <v>-102873.59395555554</v>
+        <v>-100540.26062222221</v>
       </c>
       <c r="Q20" s="20">
         <f t="shared" si="8"/>
@@ -5678,11 +5997,11 @@
       </c>
       <c r="S20" s="7">
         <f t="shared" si="3"/>
-        <v>-22044.696355555549</v>
+        <v>-21461.36302222222</v>
       </c>
       <c r="T20" s="7">
         <f t="shared" si="13"/>
-        <v>-95805.733688888868</v>
+        <v>-93472.400355555554</v>
       </c>
       <c r="V20" s="11">
         <f t="shared" si="9"/>
@@ -5694,11 +6013,11 @@
       </c>
       <c r="X20" s="7">
         <f t="shared" si="4"/>
-        <v>-18626.400888888878</v>
+        <v>-18043.06755555555</v>
       </c>
       <c r="Y20" s="7">
         <f t="shared" si="14"/>
-        <v>-80639.854222222173</v>
+        <v>-78306.520888888859</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
@@ -5715,11 +6034,11 @@
       </c>
       <c r="D21" s="7">
         <f t="shared" si="0"/>
-        <v>-23760.35555555555</v>
+        <v>-23177.022222222222</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" si="10"/>
-        <v>-135136.57777777774</v>
+        <v>-132219.91111111111</v>
       </c>
       <c r="G21" s="20">
         <f t="shared" si="6"/>
@@ -5731,11 +6050,11 @@
       </c>
       <c r="I21" s="7">
         <f t="shared" si="1"/>
-        <v>-21954.883022222217</v>
+        <v>-21371.549688888888</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="11"/>
-        <v>-128326.25724444442</v>
+        <v>-125409.59057777778</v>
       </c>
       <c r="L21" s="20">
         <f t="shared" si="7"/>
@@ -5747,11 +6066,11 @@
       </c>
       <c r="N21" s="7">
         <f t="shared" si="2"/>
-        <v>-21602.500408888882</v>
+        <v>-21019.167075555553</v>
       </c>
       <c r="O21" s="7">
         <f t="shared" si="12"/>
-        <v>-124476.09436444442</v>
+        <v>-121559.42769777776</v>
       </c>
       <c r="Q21" s="20">
         <f t="shared" si="8"/>
@@ -5763,11 +6082,11 @@
       </c>
       <c r="S21" s="7">
         <f t="shared" si="3"/>
-        <v>-20337.524515555546</v>
+        <v>-19754.191182222217</v>
       </c>
       <c r="T21" s="7">
         <f t="shared" si="13"/>
-        <v>-116143.25820444441</v>
+        <v>-113226.59153777777</v>
       </c>
       <c r="V21" s="11">
         <f t="shared" si="9"/>
@@ -5779,11 +6098,11 @@
       </c>
       <c r="X21" s="7">
         <f t="shared" si="4"/>
-        <v>-17430.985422222206</v>
+        <v>-16847.652088888877</v>
       </c>
       <c r="Y21" s="7">
         <f t="shared" si="14"/>
-        <v>-98070.839644444379</v>
+        <v>-95154.172977777736</v>
       </c>
     </row>
     <row r="22" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -5800,11 +6119,11 @@
       </c>
       <c r="D22" s="24">
         <f t="shared" si="0"/>
-        <v>-20350.255555555548</v>
+        <v>-19766.92222222222</v>
       </c>
       <c r="E22" s="24">
         <f t="shared" si="10"/>
-        <v>-155486.83333333328</v>
+        <v>-151986.83333333334</v>
       </c>
       <c r="G22" s="23">
         <f t="shared" si="6"/>
@@ -5816,11 +6135,11 @@
       </c>
       <c r="I22" s="24">
         <f t="shared" si="1"/>
-        <v>-18504.614008888882</v>
+        <v>-17921.280675555554</v>
       </c>
       <c r="J22" s="24">
         <f t="shared" si="11"/>
-        <v>-146830.87125333332</v>
+        <v>-143330.87125333335</v>
       </c>
       <c r="L22" s="23">
         <f t="shared" si="7"/>
@@ -5832,11 +6151,11 @@
       </c>
       <c r="N22" s="24">
         <f t="shared" si="2"/>
-        <v>-18909.083864888882</v>
+        <v>-18325.750531555554</v>
       </c>
       <c r="O22" s="24">
         <f t="shared" si="12"/>
-        <v>-143385.17822933331</v>
+        <v>-139885.17822933331</v>
       </c>
       <c r="Q22" s="23">
         <f t="shared" si="8"/>
@@ -5848,11 +6167,11 @@
       </c>
       <c r="S22" s="24">
         <f t="shared" si="3"/>
-        <v>-18288.918307555548</v>
+        <v>-17705.58497422222</v>
       </c>
       <c r="T22" s="24">
         <f t="shared" si="13"/>
-        <v>-134432.17651199998</v>
+        <v>-130932.17651199999</v>
       </c>
       <c r="V22" s="25">
         <f t="shared" si="9"/>
@@ -5864,11 +6183,11 @@
       </c>
       <c r="X22" s="24">
         <f t="shared" si="4"/>
-        <v>-16116.028408888871</v>
+        <v>-15532.695075555543</v>
       </c>
       <c r="Y22" s="24">
         <f t="shared" si="14"/>
-        <v>-114186.86805333325</v>
+        <v>-110686.86805333328</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
@@ -5885,11 +6204,11 @@
       </c>
       <c r="D23" s="7">
         <f t="shared" si="0"/>
-        <v>-15235.105555555547</v>
+        <v>-14651.772222222218</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="10"/>
-        <v>-170721.93888888884</v>
+        <v>-166638.60555555555</v>
       </c>
       <c r="G23" s="20">
         <f t="shared" si="6"/>
@@ -5901,11 +6220,11 @@
       </c>
       <c r="I23" s="7">
         <f t="shared" si="1"/>
-        <v>-13674.237390222213</v>
+        <v>-13090.904056888885</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="11"/>
-        <v>-160505.10864355552</v>
+        <v>-156421.77531022223</v>
       </c>
       <c r="L23" s="20">
         <f t="shared" si="7"/>
@@ -5917,11 +6236,11 @@
       </c>
       <c r="N23" s="7">
         <f t="shared" si="2"/>
-        <v>-15407.642357688877</v>
+        <v>-14824.309024355549</v>
       </c>
       <c r="O23" s="7">
         <f t="shared" si="12"/>
-        <v>-158792.82058702217</v>
+        <v>-154709.48725368886</v>
       </c>
       <c r="Q23" s="20">
         <f t="shared" si="8"/>
@@ -5933,11 +6252,11 @@
       </c>
       <c r="S23" s="7">
         <f t="shared" si="3"/>
-        <v>-15830.590857955547</v>
+        <v>-15247.257524622219</v>
       </c>
       <c r="T23" s="7">
         <f t="shared" si="13"/>
-        <v>-150262.76736995552</v>
+        <v>-146179.4340366222</v>
       </c>
       <c r="V23" s="11">
         <f t="shared" si="9"/>
@@ -5949,11 +6268,11 @@
       </c>
       <c r="X23" s="7">
         <f t="shared" si="4"/>
-        <v>-14669.575694222201</v>
+        <v>-14086.242360888873</v>
       </c>
       <c r="Y23" s="7">
         <f t="shared" si="14"/>
-        <v>-128856.44374755546</v>
+        <v>-124773.11041422216</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
@@ -5970,11 +6289,11 @@
       </c>
       <c r="D24" s="7">
         <f t="shared" si="0"/>
-        <v>-7562.3805555555446</v>
+        <v>-6979.0472222222161</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="10"/>
-        <v>-178284.31944444438</v>
+        <v>-173617.65277777775</v>
       </c>
       <c r="G24" s="20">
         <f t="shared" si="6"/>
@@ -5986,11 +6305,11 @@
       </c>
       <c r="I24" s="7">
         <f t="shared" si="1"/>
-        <v>-6911.7101240888805</v>
+        <v>-6328.3767907555521</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="11"/>
-        <v>-167416.81876764441</v>
+        <v>-162750.15210097778</v>
       </c>
       <c r="L24" s="20">
         <f t="shared" si="7"/>
@@ -6002,11 +6321,11 @@
       </c>
       <c r="N24" s="7">
         <f t="shared" si="2"/>
-        <v>-10855.768398328877</v>
+        <v>-10272.435064995549</v>
       </c>
       <c r="O24" s="7">
         <f t="shared" si="12"/>
-        <v>-169648.58898535106</v>
+        <v>-164981.9223186844</v>
       </c>
       <c r="Q24" s="20">
         <f t="shared" si="8"/>
@@ -6018,11 +6337,11 @@
       </c>
       <c r="S24" s="7">
         <f t="shared" si="3"/>
-        <v>-12880.597918435546</v>
+        <v>-12297.264585102217</v>
       </c>
       <c r="T24" s="7">
         <f t="shared" si="13"/>
-        <v>-163143.36528839107</v>
+        <v>-158476.69862172441</v>
       </c>
       <c r="V24" s="11">
         <f t="shared" si="9"/>
@@ -6034,11 +6353,11 @@
       </c>
       <c r="X24" s="7">
         <f t="shared" si="4"/>
-        <v>-13078.477708088867</v>
+        <v>-12495.144374755539</v>
       </c>
       <c r="Y24" s="7">
         <f t="shared" si="14"/>
-        <v>-141934.92145564433</v>
+        <v>-137268.25478897771</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
@@ -6055,11 +6374,11 @@
       </c>
       <c r="D25" s="7">
         <f t="shared" si="0"/>
-        <v>3946.7069444444605</v>
+        <v>4530.040277777789</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="10"/>
-        <v>-174337.61249999993</v>
+        <v>-169087.61249999996</v>
       </c>
       <c r="G25" s="20">
         <f t="shared" si="6"/>
@@ -6071,11 +6390,11 @@
       </c>
       <c r="I25" s="7">
         <f t="shared" si="1"/>
-        <v>2555.8280484977913</v>
+        <v>3139.1613818311198</v>
       </c>
       <c r="J25" s="7">
         <f t="shared" si="11"/>
-        <v>-164860.99071914662</v>
+        <v>-159610.99071914665</v>
       </c>
       <c r="L25" s="20">
         <f t="shared" si="7"/>
@@ -6087,11 +6406,11 @@
       </c>
       <c r="N25" s="7">
         <f t="shared" si="2"/>
-        <v>-4938.3322511608749</v>
+        <v>-4354.9989178275464</v>
       </c>
       <c r="O25" s="7">
         <f t="shared" si="12"/>
-        <v>-174586.92123651193</v>
+        <v>-169336.92123651196</v>
       </c>
       <c r="Q25" s="20">
         <f t="shared" si="8"/>
@@ -6103,11 +6422,11 @@
       </c>
       <c r="S25" s="7">
         <f t="shared" si="3"/>
-        <v>-9340.6063910115481</v>
+        <v>-8757.2730576782196</v>
       </c>
       <c r="T25" s="7">
         <f t="shared" si="13"/>
-        <v>-172483.97167940263</v>
+        <v>-167233.97167940263</v>
       </c>
       <c r="V25" s="11">
         <f t="shared" si="9"/>
@@ -6119,11 +6438,11 @@
       </c>
       <c r="X25" s="7">
         <f t="shared" si="4"/>
-        <v>-11328.269923342195</v>
+        <v>-10744.936590008867</v>
       </c>
       <c r="Y25" s="7">
         <f t="shared" si="14"/>
-        <v>-153263.19137898652</v>
+        <v>-148013.19137898658</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
@@ -6140,11 +6459,11 @@
       </c>
       <c r="D26" s="7">
         <f t="shared" si="0"/>
-        <v>21210.338194444466</v>
+        <v>21793.671527777795</v>
       </c>
       <c r="E26" s="7">
         <f t="shared" si="10"/>
-        <v>-153127.27430555547</v>
+        <v>-147293.94097222216</v>
       </c>
       <c r="G26" s="20">
         <f t="shared" si="6"/>
@@ -6156,11 +6475,11 @@
       </c>
       <c r="I26" s="7">
         <f t="shared" si="1"/>
-        <v>15810.381490119118</v>
+        <v>16393.714823452447</v>
       </c>
       <c r="J26" s="7">
         <f t="shared" si="11"/>
-        <v>-149050.6092290275</v>
+        <v>-143217.27589569421</v>
       </c>
       <c r="L26" s="20">
         <f t="shared" si="7"/>
@@ -6172,11 +6491,11 @@
       </c>
       <c r="N26" s="7">
         <f t="shared" si="2"/>
-        <v>2754.3347401575338</v>
+        <v>3337.6680734908623</v>
       </c>
       <c r="O26" s="7">
         <f t="shared" si="12"/>
-        <v>-171832.5864963544</v>
+        <v>-165999.25316302109</v>
       </c>
       <c r="Q26" s="20">
         <f t="shared" si="8"/>
@@ -6188,11 +6507,11 @@
       </c>
       <c r="S26" s="7">
         <f t="shared" si="3"/>
-        <v>-5092.616558102749</v>
+        <v>-4509.2832247694205</v>
       </c>
       <c r="T26" s="7">
         <f t="shared" si="13"/>
-        <v>-177576.58823750538</v>
+        <v>-171743.25490417206</v>
       </c>
       <c r="V26" s="11">
         <f t="shared" si="9"/>
@@ -6204,11 +6523,11 @@
       </c>
       <c r="X26" s="7">
         <f t="shared" si="4"/>
-        <v>-9403.0413601208566</v>
+        <v>-8819.7080267875281</v>
       </c>
       <c r="Y26" s="7">
         <f t="shared" si="14"/>
-        <v>-162666.23273910739</v>
+        <v>-156832.89940577411</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
@@ -6225,11 +6544,11 @@
       </c>
       <c r="D27" s="7">
         <f t="shared" si="0"/>
-        <v>47105.785069444479</v>
+        <v>47689.118402777807</v>
       </c>
       <c r="E27" s="7">
         <f t="shared" si="10"/>
-        <v>-106021.489236111</v>
+        <v>-99604.822569444354</v>
       </c>
       <c r="G27" s="20">
         <f t="shared" si="6"/>
@@ -6241,11 +6560,11 @@
       </c>
       <c r="I27" s="7">
         <f t="shared" si="1"/>
-        <v>34366.756308388984</v>
+        <v>34950.089641722312</v>
       </c>
       <c r="J27" s="7">
         <f t="shared" si="11"/>
-        <v>-114683.85292063851</v>
+        <v>-108267.1862539719</v>
       </c>
       <c r="L27" s="20">
         <f t="shared" si="7"/>
@@ -6257,11 +6576,11 @@
       </c>
       <c r="N27" s="7">
         <f t="shared" si="2"/>
-        <v>12754.801828871456</v>
+        <v>13338.135162204784</v>
       </c>
       <c r="O27" s="7">
         <f t="shared" si="12"/>
-        <v>-159077.78466748295</v>
+        <v>-152661.11800081629</v>
       </c>
       <c r="Q27" s="20">
         <f t="shared" si="8"/>
@@ -6273,11 +6592,11 @@
       </c>
       <c r="S27" s="7">
         <f t="shared" si="3"/>
-        <v>4.9712413878114603</v>
+        <v>588.30457472113994</v>
       </c>
       <c r="T27" s="7">
         <f t="shared" si="13"/>
-        <v>-177571.61699611758</v>
+        <v>-171154.95032945092</v>
       </c>
       <c r="V27" s="11">
         <f t="shared" si="9"/>
@@ -6289,11 +6608,11 @@
       </c>
       <c r="X27" s="7">
         <f t="shared" si="4"/>
-        <v>-7285.289940577386</v>
+        <v>-6701.9566072440575</v>
       </c>
       <c r="Y27" s="7">
         <f t="shared" si="14"/>
-        <v>-169951.52267968477</v>
+        <v>-163534.85601301817</v>
       </c>
     </row>
     <row r="28" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -6310,11 +6629,11 @@
       </c>
       <c r="D28" s="28">
         <f t="shared" si="0"/>
-        <v>85948.955381944485</v>
+        <v>86532.288715277813</v>
       </c>
       <c r="E28" s="28">
         <f t="shared" si="10"/>
-        <v>-20072.533854166511</v>
+        <v>-13072.533854166541</v>
       </c>
       <c r="G28" s="27">
         <f t="shared" si="6"/>
@@ -6326,11 +6645,11 @@
       </c>
       <c r="I28" s="28">
         <f t="shared" si="1"/>
-        <v>60345.681053966808</v>
+        <v>60929.014387300136</v>
       </c>
       <c r="J28" s="28">
         <f t="shared" si="11"/>
-        <v>-54338.171866671706</v>
+        <v>-47338.171866671764</v>
       </c>
       <c r="L28" s="27">
         <f t="shared" si="7"/>
@@ -6342,11 +6661,11 @@
       </c>
       <c r="N28" s="28">
         <f t="shared" si="2"/>
-        <v>25755.409044199569</v>
+        <v>26338.742377532897</v>
       </c>
       <c r="O28" s="28">
         <f t="shared" si="12"/>
-        <v>-133322.37562328338</v>
+        <v>-126322.3756232834</v>
       </c>
       <c r="Q28" s="27">
         <f t="shared" si="8"/>
@@ -6358,11 +6677,11 @@
       </c>
       <c r="S28" s="28">
         <f t="shared" si="3"/>
-        <v>6122.0766007764796</v>
+        <v>6705.4099341098081</v>
       </c>
       <c r="T28" s="28">
         <f t="shared" si="13"/>
-        <v>-171449.54039534109</v>
+        <v>-164449.54039534112</v>
       </c>
       <c r="V28" s="29">
         <f t="shared" si="9"/>
@@ -6374,11 +6693,11 @@
       </c>
       <c r="X28" s="28">
         <f t="shared" si="4"/>
-        <v>-4955.7633790795699</v>
+        <v>-4372.4300457462414</v>
       </c>
       <c r="Y28" s="28">
         <f t="shared" si="14"/>
-        <v>-174907.28605876435</v>
+        <v>-167907.28605876441</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
@@ -6395,11 +6714,11 @@
       </c>
       <c r="D29" s="7">
         <f t="shared" si="0"/>
-        <v>144213.71085069448</v>
+        <v>144797.04418402782</v>
       </c>
       <c r="E29" s="7">
         <f>E28+D29</f>
-        <v>124141.17699652797</v>
+        <v>131724.51032986128</v>
       </c>
       <c r="G29" s="20">
         <f t="shared" si="6"/>
@@ -6411,11 +6730,11 @@
       </c>
       <c r="I29" s="7">
         <f t="shared" si="1"/>
-        <v>96716.175697775718</v>
+        <v>97299.509031109046</v>
       </c>
       <c r="J29" s="7">
         <f t="shared" si="11"/>
-        <v>42378.003831104012</v>
+        <v>49961.337164437282</v>
       </c>
       <c r="L29" s="20">
         <f t="shared" si="7"/>
@@ -6427,11 +6746,11 @@
       </c>
       <c r="N29" s="7">
         <f t="shared" si="2"/>
-        <v>42656.198424126109</v>
+        <v>43239.531757459437</v>
       </c>
       <c r="O29" s="7">
         <f t="shared" si="12"/>
-        <v>-90666.177199157275</v>
+        <v>-83082.843865823961</v>
       </c>
       <c r="Q29" s="20">
         <f t="shared" si="8"/>
@@ -6443,11 +6762,11 @@
       </c>
       <c r="S29" s="7">
         <f t="shared" si="3"/>
-        <v>13462.603032042887</v>
+        <v>14045.936365376216</v>
       </c>
       <c r="T29" s="7">
         <f t="shared" si="13"/>
-        <v>-157986.9373632982</v>
+        <v>-150403.60402996489</v>
       </c>
       <c r="V29" s="11">
         <f t="shared" si="9"/>
@@ -6459,11 +6778,11 @@
       </c>
       <c r="X29" s="7">
         <f t="shared" si="4"/>
-        <v>-2393.2841614319696</v>
+        <v>-1809.9508280986411</v>
       </c>
       <c r="Y29" s="7">
         <f t="shared" si="14"/>
-        <v>-177300.57022019633</v>
+        <v>-169717.23688686304</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
@@ -6480,11 +6799,11 @@
       </c>
       <c r="D30" s="7">
         <f t="shared" si="0"/>
-        <v>231610.84405381954</v>
+        <v>232194.17738715289</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="10"/>
-        <v>355752.02105034748</v>
+        <v>363918.68771701417</v>
       </c>
       <c r="G30" s="20">
         <f t="shared" si="6"/>
@@ -6496,11 +6815,11 @@
       </c>
       <c r="I30" s="7">
         <f t="shared" si="1"/>
-        <v>147634.8681991082</v>
+        <v>148218.20153244154</v>
       </c>
       <c r="J30" s="7">
         <f t="shared" si="11"/>
-        <v>190012.87203021219</v>
+        <v>198179.53869687882</v>
       </c>
       <c r="L30" s="20">
         <f t="shared" si="7"/>
@@ -6512,11 +6831,11 @@
       </c>
       <c r="N30" s="7">
         <f t="shared" si="2"/>
-        <v>64627.22461803061</v>
+        <v>65210.557951363939</v>
       </c>
       <c r="O30" s="7">
         <f t="shared" si="12"/>
-        <v>-26038.952581126665</v>
+        <v>-17872.285914460022</v>
       </c>
       <c r="Q30" s="20">
         <f t="shared" si="8"/>
@@ -6528,11 +6847,11 @@
       </c>
       <c r="S30" s="7">
         <f t="shared" si="3"/>
-        <v>22271.234749562576</v>
+        <v>22854.568082895905</v>
       </c>
       <c r="T30" s="7">
         <f t="shared" si="13"/>
-        <v>-135715.70261373563</v>
+        <v>-127549.03594706899</v>
       </c>
       <c r="V30" s="11">
         <f t="shared" si="9"/>
@@ -6544,11 +6863,11 @@
       </c>
       <c r="X30" s="7">
         <f t="shared" si="4"/>
-        <v>425.44297798039042</v>
+        <v>1008.7763113137189</v>
       </c>
       <c r="Y30" s="7">
         <f t="shared" si="14"/>
-        <v>-176875.12724221594</v>
+        <v>-168708.46057554934</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
@@ -6565,11 +6884,11 @@
       </c>
       <c r="D31" s="7">
         <f t="shared" si="0"/>
-        <v>362706.54385850707</v>
+        <v>363289.87719184038</v>
       </c>
       <c r="E31" s="7">
         <f t="shared" si="10"/>
-        <v>718458.56490885455</v>
+        <v>727208.56490885455</v>
       </c>
       <c r="G31" s="20">
         <f t="shared" si="6"/>
@@ -6581,11 +6900,11 @@
       </c>
       <c r="I31" s="7">
         <f t="shared" si="1"/>
-        <v>218921.03770097368</v>
+        <v>219504.37103430703</v>
       </c>
       <c r="J31" s="7">
         <f t="shared" si="11"/>
-        <v>408933.90973118588</v>
+        <v>417683.90973118588</v>
       </c>
       <c r="L31" s="20">
         <f t="shared" si="7"/>
@@ -6597,11 +6916,11 @@
       </c>
       <c r="N31" s="7">
         <f t="shared" si="2"/>
-        <v>93189.55867010646</v>
+        <v>93772.892003439789</v>
       </c>
       <c r="O31" s="7">
         <f t="shared" si="12"/>
-        <v>67150.606088979795</v>
+        <v>75900.606088979766</v>
       </c>
       <c r="Q31" s="20">
         <f t="shared" si="8"/>
@@ -6613,11 +6932,11 @@
       </c>
       <c r="S31" s="7">
         <f t="shared" si="3"/>
-        <v>32841.592810586197</v>
+        <v>33424.926143919525</v>
       </c>
       <c r="T31" s="7">
         <f t="shared" si="13"/>
-        <v>-102874.10980314943</v>
+        <v>-94124.109803149462</v>
       </c>
       <c r="V31" s="11">
         <f t="shared" si="9"/>
@@ -6629,11 +6948,11 @@
       </c>
       <c r="X31" s="7">
         <f t="shared" si="4"/>
-        <v>3526.0428313339835</v>
+        <v>4109.376164667312</v>
       </c>
       <c r="Y31" s="7">
         <f t="shared" si="14"/>
-        <v>-173349.08441088194</v>
+        <v>-164599.08441088203</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
@@ -6650,11 +6969,11 @@
       </c>
       <c r="D32" s="7">
         <f t="shared" si="0"/>
-        <v>559350.09356553841</v>
+        <v>559933.42689887166</v>
       </c>
       <c r="E32" s="7">
         <f t="shared" si="10"/>
-        <v>1277808.658474393</v>
+        <v>1287141.9918077262</v>
       </c>
       <c r="G32" s="20">
         <f t="shared" si="6"/>
@@ -6666,11 +6985,11 @@
       </c>
       <c r="I32" s="7">
         <f t="shared" si="1"/>
-        <v>318721.67500358535</v>
+        <v>319305.00833691866</v>
       </c>
       <c r="J32" s="7">
         <f t="shared" si="11"/>
-        <v>727655.58473477117</v>
+        <v>736988.91806810454</v>
       </c>
       <c r="L32" s="20">
         <f t="shared" si="7"/>
@@ -6682,11 +7001,11 @@
       </c>
       <c r="N32" s="7">
         <f t="shared" si="2"/>
-        <v>130320.59293780506</v>
+        <v>130903.92627113839</v>
       </c>
       <c r="O32" s="7">
         <f t="shared" si="12"/>
-        <v>197471.19902678486</v>
+        <v>206804.53236011817</v>
       </c>
       <c r="Q32" s="20">
         <f t="shared" si="8"/>
@@ -6698,11 +7017,11 @@
       </c>
       <c r="S32" s="7">
         <f t="shared" si="3"/>
-        <v>45526.022483814537</v>
+        <v>46109.355817147865</v>
       </c>
       <c r="T32" s="7">
         <f t="shared" si="13"/>
-        <v>-57348.087319334896</v>
+        <v>-48014.753986001597</v>
       </c>
       <c r="V32" s="11">
         <f t="shared" si="9"/>
@@ -6714,11 +7033,11 @@
       </c>
       <c r="X32" s="7">
         <f t="shared" si="4"/>
-        <v>6936.7026700229435</v>
+        <v>7520.036003356272</v>
       </c>
       <c r="Y32" s="7">
         <f t="shared" si="14"/>
-        <v>-166412.38174085901</v>
+        <v>-157079.04840752576</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
@@ -6735,11 +7054,11 @@
       </c>
       <c r="D33" s="7">
         <f t="shared" si="0"/>
-        <v>854315.41812608542</v>
+        <v>854898.75145941868</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" si="10"/>
-        <v>2132124.0766004785</v>
+        <v>2142040.743267145</v>
       </c>
       <c r="G33" s="20">
         <f t="shared" si="6"/>
@@ -6751,11 +7070,11 @@
       </c>
       <c r="I33" s="7">
         <f t="shared" si="1"/>
-        <v>458442.5672272417</v>
+        <v>459025.90056057501</v>
       </c>
       <c r="J33" s="7">
         <f t="shared" si="11"/>
-        <v>1186098.151962013</v>
+        <v>1196014.8186286795</v>
       </c>
       <c r="L33" s="20">
         <f t="shared" si="7"/>
@@ -6767,11 +7086,11 @@
       </c>
       <c r="N33" s="7">
         <f t="shared" si="2"/>
-        <v>178590.93748581325</v>
+        <v>179174.27081914659</v>
       </c>
       <c r="O33" s="7">
         <f t="shared" si="12"/>
-        <v>376062.13651259814</v>
+        <v>385978.80317926477</v>
       </c>
       <c r="Q33" s="20">
         <f t="shared" si="8"/>
@@ -6783,11 +7102,11 @@
       </c>
       <c r="S33" s="7">
         <f t="shared" si="3"/>
-        <v>60747.338091688551</v>
+        <v>61330.671425021879</v>
       </c>
       <c r="T33" s="7">
         <f t="shared" si="13"/>
-        <v>3399.2507723536546</v>
+        <v>13315.917439020282</v>
       </c>
       <c r="V33" s="11">
         <f t="shared" si="9"/>
@@ -6799,11 +7118,11 @@
       </c>
       <c r="X33" s="7">
         <f t="shared" si="4"/>
-        <v>10688.428492580799</v>
+        <v>11271.761825914127</v>
       </c>
       <c r="Y33" s="7">
         <f t="shared" si="14"/>
-        <v>-155723.95324827821</v>
+        <v>-145807.28658161164</v>
       </c>
     </row>
     <row r="34" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -6820,11 +7139,11 @@
       </c>
       <c r="D34" s="28">
         <f t="shared" si="0"/>
-        <v>1296763.4049669059</v>
+        <v>1297346.7383002392</v>
       </c>
       <c r="E34" s="28">
         <f t="shared" si="10"/>
-        <v>3428887.4815673847</v>
+        <v>3439387.4815673842</v>
       </c>
       <c r="G34" s="27">
         <f t="shared" si="6"/>
@@ -6836,11 +7155,11 @@
       </c>
       <c r="I34" s="28">
         <f t="shared" si="1"/>
-        <v>654051.81634036067</v>
+        <v>654635.14967369393</v>
       </c>
       <c r="J34" s="28">
         <f t="shared" si="11"/>
-        <v>1840149.9683023738</v>
+        <v>1850649.9683023733</v>
       </c>
       <c r="L34" s="27">
         <f t="shared" si="7"/>
@@ -6852,11 +7171,11 @@
       </c>
       <c r="N34" s="28">
         <f t="shared" si="2"/>
-        <v>241342.38539822388</v>
+        <v>241925.71873155722</v>
       </c>
       <c r="O34" s="28">
         <f t="shared" si="12"/>
-        <v>617404.52191082202</v>
+        <v>627904.52191082202</v>
       </c>
       <c r="Q34" s="27">
         <f t="shared" si="8"/>
@@ -6868,11 +7187,11 @@
       </c>
       <c r="S34" s="28">
         <f t="shared" si="3"/>
-        <v>79012.916821137376</v>
+        <v>79596.250154470705</v>
       </c>
       <c r="T34" s="28">
         <f t="shared" si="13"/>
-        <v>82412.167593491031</v>
+        <v>92912.167593490987</v>
       </c>
       <c r="V34" s="29">
         <f t="shared" si="9"/>
@@ -6884,11 +7203,11 @@
       </c>
       <c r="X34" s="28">
         <f t="shared" si="4"/>
-        <v>14815.326897394432</v>
+        <v>15398.660230727761</v>
       </c>
       <c r="Y34" s="28">
         <f t="shared" si="14"/>
-        <v>-140908.62635088377</v>
+        <v>-130408.62635088387</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
@@ -6905,11 +7224,11 @@
       </c>
       <c r="D35" s="7">
         <f t="shared" si="0"/>
-        <v>1960435.3852281366</v>
+        <v>1961018.7185614698</v>
       </c>
       <c r="E35" s="7">
         <f t="shared" si="10"/>
-        <v>5389322.8667955212</v>
+        <v>5400406.2001288543</v>
       </c>
       <c r="G35" s="20">
         <f t="shared" si="6"/>
@@ -6921,11 +7240,11 @@
       </c>
       <c r="I35" s="7">
         <f t="shared" si="1"/>
-        <v>927904.76509872708</v>
+        <v>928488.09843206033</v>
       </c>
       <c r="J35" s="7">
         <f t="shared" si="11"/>
-        <v>2768054.7334011011</v>
+        <v>2779138.0667344336</v>
       </c>
       <c r="L35" s="20">
         <f t="shared" si="7"/>
@@ -6937,11 +7256,11 @@
       </c>
       <c r="N35" s="7">
         <f t="shared" si="2"/>
-        <v>322919.26768435771</v>
+        <v>323502.60101769102</v>
       </c>
       <c r="O35" s="7">
         <f t="shared" si="12"/>
-        <v>940323.78959517973</v>
+        <v>951407.12292851298</v>
       </c>
       <c r="Q35" s="20">
         <f t="shared" si="8"/>
@@ -6953,11 +7272,11 @@
       </c>
       <c r="S35" s="7">
         <f t="shared" si="3"/>
-        <v>100931.61129647597</v>
+        <v>101514.9446298093</v>
       </c>
       <c r="T35" s="7">
         <f t="shared" si="13"/>
-        <v>183343.77888996701</v>
+        <v>194427.11222330027</v>
       </c>
       <c r="V35" s="11">
         <f t="shared" si="9"/>
@@ -6969,11 +7288,11 @@
       </c>
       <c r="X35" s="7">
         <f t="shared" si="4"/>
-        <v>19354.915142689435</v>
+        <v>19938.248476022763</v>
       </c>
       <c r="Y35" s="7">
         <f t="shared" si="14"/>
-        <v>-121553.71120819433</v>
+        <v>-110470.37787486111</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
@@ -6990,11 +7309,11 @@
       </c>
       <c r="D36" s="7">
         <f t="shared" si="0"/>
-        <v>2955943.3556199824</v>
+        <v>2956526.6889533158</v>
       </c>
       <c r="E36" s="7">
         <f t="shared" si="10"/>
-        <v>8345266.2224155031</v>
+        <v>8356932.8890821701</v>
       </c>
       <c r="G36" s="20">
         <f t="shared" si="6"/>
@@ -7006,11 +7325,11 @@
       </c>
       <c r="I36" s="7">
         <f t="shared" si="1"/>
-        <v>1311298.8933604402</v>
+        <v>1311882.2266937734</v>
       </c>
       <c r="J36" s="7">
         <f t="shared" si="11"/>
-        <v>4079353.6267615412</v>
+        <v>4091020.2934282068</v>
       </c>
       <c r="L36" s="20">
         <f t="shared" si="7"/>
@@ -7022,11 +7341,11 @@
       </c>
       <c r="N36" s="7">
         <f t="shared" si="2"/>
-        <v>428969.21465633175</v>
+        <v>429552.54798966506</v>
       </c>
       <c r="O36" s="7">
         <f t="shared" si="12"/>
-        <v>1369293.0042515115</v>
+        <v>1380959.670918178</v>
       </c>
       <c r="Q36" s="20">
         <f t="shared" si="8"/>
@@ -7038,11 +7357,11 @@
       </c>
       <c r="S36" s="7">
         <f t="shared" si="3"/>
-        <v>127234.04466688224</v>
+        <v>127817.37800021557</v>
       </c>
       <c r="T36" s="7">
         <f t="shared" si="13"/>
-        <v>310577.82355684927</v>
+        <v>322244.49022351584</v>
       </c>
       <c r="V36" s="11">
         <f t="shared" si="9"/>
@@ -7054,11 +7373,11 @@
       </c>
       <c r="X36" s="7">
         <f t="shared" si="4"/>
-        <v>24348.462212513939</v>
+        <v>24931.795545847268</v>
       </c>
       <c r="Y36" s="7">
         <f t="shared" si="14"/>
-        <v>-97205.248995680391</v>
+        <v>-85538.582329013836</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
@@ -7075,11 +7394,11 @@
       </c>
       <c r="D37" s="7">
         <f t="shared" si="0"/>
-        <v>4449205.3112077508</v>
+        <v>4449788.6445410848</v>
       </c>
       <c r="E37" s="7">
         <f t="shared" si="10"/>
-        <v>12794471.533623254</v>
+        <v>12806721.533623256</v>
       </c>
       <c r="G37" s="20">
         <f t="shared" si="6"/>
@@ -7091,11 +7410,11 @@
       </c>
       <c r="I37" s="7">
         <f t="shared" si="1"/>
-        <v>1848050.6729268383</v>
+        <v>1848634.0062601715</v>
       </c>
       <c r="J37" s="7">
         <f t="shared" si="11"/>
-        <v>5927404.2996883793</v>
+        <v>5939654.2996883783</v>
       </c>
       <c r="L37" s="20">
         <f t="shared" si="7"/>
@@ -7107,11 +7426,11 @@
       </c>
       <c r="N37" s="7">
         <f t="shared" si="2"/>
-        <v>566834.14571989805</v>
+        <v>567417.47905323131</v>
       </c>
       <c r="O37" s="7">
         <f t="shared" si="12"/>
-        <v>1936127.1499714097</v>
+        <v>1948377.1499714092</v>
       </c>
       <c r="Q37" s="20">
         <f t="shared" si="8"/>
@@ -7123,11 +7442,11 @@
       </c>
       <c r="S37" s="7">
         <f t="shared" si="3"/>
-        <v>158796.9647113698</v>
+        <v>159380.29804470314</v>
       </c>
       <c r="T37" s="7">
         <f t="shared" si="13"/>
-        <v>469374.7882682191</v>
+        <v>481624.78826821898</v>
       </c>
       <c r="V37" s="11">
         <f t="shared" si="9"/>
@@ -7139,11 +7458,11 @@
       </c>
       <c r="X37" s="7">
         <f t="shared" si="4"/>
-        <v>29841.363989320886</v>
+        <v>30424.697322654214</v>
       </c>
       <c r="Y37" s="7">
         <f t="shared" si="14"/>
-        <v>-67363.885006359502</v>
+        <v>-55113.885006359618</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
@@ -7160,11 +7479,11 @@
       </c>
       <c r="D38" s="7">
         <f t="shared" si="0"/>
-        <v>6689098.2445894042</v>
+        <v>6689681.5779227382</v>
       </c>
       <c r="E38" s="7">
         <f t="shared" si="10"/>
-        <v>19483569.778212659</v>
+        <v>19496403.111545995</v>
       </c>
       <c r="G38" s="20">
         <f t="shared" si="6"/>
@@ -7176,11 +7495,11 @@
       </c>
       <c r="I38" s="7">
         <f t="shared" si="1"/>
-        <v>2599503.1643197956</v>
+        <v>2600086.497653129</v>
       </c>
       <c r="J38" s="7">
         <f t="shared" si="11"/>
-        <v>8526907.4640081748</v>
+        <v>8539740.7973415069</v>
       </c>
       <c r="L38" s="20">
         <f t="shared" si="7"/>
@@ -7192,11 +7511,11 @@
       </c>
       <c r="N38" s="7">
         <f t="shared" si="2"/>
-        <v>746058.55610253417</v>
+        <v>746641.88943586743</v>
       </c>
       <c r="O38" s="7">
         <f t="shared" si="12"/>
-        <v>2682185.706073944</v>
+        <v>2695019.0394072765</v>
       </c>
       <c r="Q38" s="20">
         <f t="shared" si="8"/>
@@ -7208,11 +7527,11 @@
       </c>
       <c r="S38" s="7">
         <f t="shared" si="3"/>
-        <v>196672.46876475489</v>
+        <v>197255.80209808823</v>
       </c>
       <c r="T38" s="7">
         <f t="shared" si="13"/>
-        <v>666047.25703297392</v>
+        <v>678880.59036630718</v>
       </c>
       <c r="V38" s="11">
         <f t="shared" si="9"/>
@@ -7224,11 +7543,11 @@
       </c>
       <c r="X38" s="7">
         <f t="shared" si="4"/>
-        <v>35883.555943808533</v>
+        <v>36466.889277141861</v>
       </c>
       <c r="Y38" s="7">
         <f t="shared" si="14"/>
-        <v>-31480.329062550969</v>
+        <v>-18646.995729217757</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
@@ -7245,11 +7564,11 @@
       </c>
       <c r="D39" s="7">
         <f t="shared" si="0"/>
-        <v>10048937.644661885</v>
+        <v>10049520.977995219</v>
       </c>
       <c r="E39" s="7">
         <f t="shared" si="10"/>
-        <v>29532507.422874544</v>
+        <v>29545924.089541212</v>
       </c>
       <c r="G39" s="20">
         <f t="shared" si="6"/>
@@ -7261,11 +7580,11 @@
       </c>
       <c r="I39" s="7">
         <f t="shared" si="1"/>
-        <v>3651536.6522699357</v>
+        <v>3652119.9856032692</v>
       </c>
       <c r="J39" s="7">
         <f t="shared" si="11"/>
-        <v>12178444.11627811</v>
+        <v>12191860.782944776</v>
       </c>
       <c r="L39" s="20">
         <f t="shared" si="7"/>
@@ -7277,11 +7596,11 @@
       </c>
       <c r="N39" s="7">
         <f t="shared" si="2"/>
-        <v>979050.28959996114</v>
+        <v>979633.62293329439</v>
       </c>
       <c r="O39" s="7">
         <f t="shared" si="12"/>
-        <v>3661235.9956739051</v>
+        <v>3674652.6623405712</v>
       </c>
       <c r="Q39" s="20">
         <f t="shared" si="8"/>
@@ -7293,11 +7612,11 @@
       </c>
       <c r="S39" s="7">
         <f t="shared" si="3"/>
-        <v>242123.07362881693</v>
+        <v>242706.40696215027</v>
       </c>
       <c r="T39" s="7">
         <f t="shared" si="13"/>
-        <v>908170.33066179091</v>
+        <v>921586.99732845742</v>
       </c>
       <c r="V39" s="11">
         <f t="shared" si="9"/>
@@ -7309,11 +7628,11 @@
       </c>
       <c r="X39" s="7">
         <f t="shared" si="4"/>
-        <v>42529.967093744955</v>
+        <v>43113.300427078284</v>
       </c>
       <c r="Y39" s="7">
         <f t="shared" si="14"/>
-        <v>11049.638031193987</v>
+        <v>24466.304697860527</v>
       </c>
     </row>
     <row r="40" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -7330,11 +7649,11 @@
       </c>
       <c r="D40" s="28">
         <f t="shared" si="0"/>
-        <v>15088696.744770605</v>
+        <v>15089280.078103939</v>
       </c>
       <c r="E40" s="28">
         <f t="shared" si="10"/>
-        <v>44621204.167645149</v>
+        <v>44635204.167645149</v>
       </c>
       <c r="G40" s="27">
         <f t="shared" si="6"/>
@@ -7346,11 +7665,11 @@
       </c>
       <c r="I40" s="28">
         <f t="shared" si="1"/>
-        <v>5124383.5354001317</v>
+        <v>5124966.8687334657</v>
       </c>
       <c r="J40" s="28">
         <f t="shared" si="11"/>
-        <v>17302827.651678242</v>
+        <v>17316827.651678242</v>
       </c>
       <c r="L40" s="27">
         <f t="shared" si="7"/>
@@ -7362,11 +7681,11 @@
       </c>
       <c r="N40" s="28">
         <f t="shared" si="2"/>
-        <v>1281939.5431466161</v>
+        <v>1282522.8764799493</v>
       </c>
       <c r="O40" s="28">
         <f t="shared" si="12"/>
-        <v>4943175.538820521</v>
+        <v>4957175.53882052</v>
       </c>
       <c r="Q40" s="27">
         <f t="shared" si="8"/>
@@ -7378,11 +7697,11 @@
       </c>
       <c r="S40" s="28">
         <f t="shared" si="3"/>
-        <v>296663.79946569144</v>
+        <v>297247.13279902475</v>
       </c>
       <c r="T40" s="28">
         <f t="shared" si="13"/>
-        <v>1204834.1301274823</v>
+        <v>1218834.1301274821</v>
       </c>
       <c r="V40" s="29">
         <f t="shared" si="9"/>
@@ -7394,11 +7713,11 @@
       </c>
       <c r="X40" s="28">
         <f t="shared" si="4"/>
-        <v>49841.01935867501</v>
+        <v>50424.352692008339</v>
       </c>
       <c r="Y40" s="28">
         <f t="shared" si="14"/>
-        <v>60890.657389868997</v>
+        <v>74890.657389868866</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
@@ -7415,11 +7734,11 @@
       </c>
       <c r="D41" s="7">
         <f t="shared" si="0"/>
-        <v>22648335.394933686</v>
+        <v>22648918.728267018</v>
       </c>
       <c r="E41" s="7">
         <f t="shared" si="10"/>
-        <v>67269539.562578827</v>
+        <v>67284122.89591217</v>
       </c>
       <c r="G41" s="20">
         <f t="shared" si="6"/>
@@ -7431,11 +7750,11 @@
       </c>
       <c r="I41" s="7">
         <f t="shared" si="1"/>
-        <v>7186369.171782406</v>
+        <v>7186952.50511574</v>
       </c>
       <c r="J41" s="7">
         <f t="shared" si="11"/>
-        <v>24489196.823460646</v>
+        <v>24503780.156793982</v>
       </c>
       <c r="L41" s="20">
         <f t="shared" si="7"/>
@@ -7447,11 +7766,11 @@
       </c>
       <c r="N41" s="7">
         <f t="shared" si="2"/>
-        <v>1675695.5727572676</v>
+        <v>1676278.9060906009</v>
       </c>
       <c r="O41" s="7">
         <f t="shared" si="12"/>
-        <v>6618871.1115777884</v>
+        <v>6633454.4449111205</v>
       </c>
       <c r="Q41" s="20">
         <f t="shared" si="8"/>
@@ -7463,11 +7782,11 @@
       </c>
       <c r="S41" s="7">
         <f t="shared" si="3"/>
-        <v>362112.67046994081</v>
+        <v>362696.00380327413</v>
       </c>
       <c r="T41" s="7">
         <f t="shared" si="13"/>
-        <v>1566946.8005974232</v>
+        <v>1581530.1339307562</v>
       </c>
       <c r="V41" s="11">
         <f t="shared" si="9"/>
@@ -7479,11 +7798,11 @@
       </c>
       <c r="X41" s="7">
         <f t="shared" si="4"/>
-        <v>57883.176850098083</v>
+        <v>58466.510183431412</v>
       </c>
       <c r="Y41" s="7">
         <f t="shared" si="14"/>
-        <v>118773.83423996708</v>
+        <v>133357.16757330028</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
@@ -7500,11 +7819,11 @@
       </c>
       <c r="D42" s="7">
         <f t="shared" si="0"/>
-        <v>33987793.370178312</v>
+        <v>33988376.70351164</v>
       </c>
       <c r="E42" s="7">
         <f t="shared" si="10"/>
-        <v>101257332.93275714</v>
+        <v>101272499.59942381</v>
       </c>
       <c r="G42" s="20">
         <f t="shared" si="6"/>
@@ -7516,11 +7835,11 @@
       </c>
       <c r="I42" s="7">
         <f t="shared" si="1"/>
-        <v>10073149.06271759</v>
+        <v>10073732.396050924</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="11"/>
-        <v>34562345.88617824</v>
+        <v>34577512.552844904</v>
       </c>
       <c r="L42" s="20">
         <f t="shared" si="7"/>
@@ -7532,11 +7851,11 @@
       </c>
       <c r="N42" s="7">
         <f t="shared" si="2"/>
-        <v>2187578.4112511147</v>
+        <v>2188161.7445844482</v>
       </c>
       <c r="O42" s="7">
         <f t="shared" si="12"/>
-        <v>8806449.522828903</v>
+        <v>8821616.1894955691</v>
       </c>
       <c r="Q42" s="20">
         <f t="shared" si="8"/>
@@ -7548,11 +7867,11 @@
       </c>
       <c r="S42" s="7">
         <f t="shared" si="3"/>
-        <v>440651.31567504012</v>
+        <v>441234.64900837344</v>
       </c>
       <c r="T42" s="7">
         <f t="shared" si="13"/>
-        <v>2007598.1162724635</v>
+        <v>2022764.7829391297</v>
       </c>
       <c r="V42" s="11">
         <f t="shared" si="9"/>
@@ -7564,11 +7883,11 @@
       </c>
       <c r="X42" s="7">
         <f t="shared" si="4"/>
-        <v>66729.550090663441</v>
+        <v>67312.883423996769</v>
       </c>
       <c r="Y42" s="7">
         <f t="shared" si="14"/>
-        <v>185503.38433063054</v>
+        <v>200670.05099729705</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.3">
@@ -7585,11 +7904,11 @@
       </c>
       <c r="D43" s="7">
         <f t="shared" si="0"/>
-        <v>50996980.333045244</v>
+        <v>50997563.666378573</v>
       </c>
       <c r="E43" s="7">
         <f t="shared" si="10"/>
-        <v>152254313.26580238</v>
+        <v>152270063.26580238</v>
       </c>
       <c r="G43" s="20">
         <f t="shared" si="6"/>
@@ -7601,11 +7920,11 @@
       </c>
       <c r="I43" s="7">
         <f t="shared" si="1"/>
-        <v>14114640.910026848</v>
+        <v>14115224.243360182</v>
       </c>
       <c r="J43" s="7">
         <f t="shared" si="11"/>
-        <v>48676986.796205088</v>
+        <v>48692736.796205088</v>
       </c>
       <c r="L43" s="20">
         <f t="shared" si="7"/>
@@ -7617,11 +7936,11 @@
       </c>
       <c r="N43" s="7">
         <f t="shared" si="2"/>
-        <v>2853026.1012931159</v>
+        <v>2853609.4346264494</v>
       </c>
       <c r="O43" s="7">
         <f t="shared" si="12"/>
-        <v>11659475.62412202</v>
+        <v>11675225.624122018</v>
       </c>
       <c r="Q43" s="20">
         <f t="shared" si="8"/>
@@ -7633,11 +7952,11 @@
       </c>
       <c r="S43" s="7">
         <f t="shared" si="3"/>
-        <v>534897.6899211593</v>
+        <v>535481.02325449255</v>
       </c>
       <c r="T43" s="7">
         <f t="shared" si="13"/>
-        <v>2542495.8061936228</v>
+        <v>2558245.8061936223</v>
       </c>
       <c r="V43" s="11">
         <f t="shared" si="9"/>
@@ -7649,11 +7968,11 @@
       </c>
       <c r="X43" s="7">
         <f t="shared" si="4"/>
-        <v>76460.560655285342</v>
+        <v>77043.893988618671</v>
       </c>
       <c r="Y43" s="7">
         <f t="shared" si="14"/>
-        <v>261963.94498591588</v>
+        <v>277713.94498591573</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.3">
@@ -7670,11 +7989,11 @@
       </c>
       <c r="D44" s="7">
         <f t="shared" si="0"/>
-        <v>76510760.777345642</v>
+        <v>76511344.110678971</v>
       </c>
       <c r="E44" s="7">
         <f t="shared" si="10"/>
-        <v>228765074.04314804</v>
+        <v>228781407.37648135</v>
       </c>
       <c r="G44" s="20">
         <f t="shared" si="6"/>
@@ -7686,11 +8005,11 @@
       </c>
       <c r="I44" s="7">
         <f t="shared" si="1"/>
-        <v>19772729.496259809</v>
+        <v>19773312.829593141</v>
       </c>
       <c r="J44" s="7">
         <f t="shared" si="11"/>
-        <v>68449716.292464897</v>
+        <v>68466049.625798225</v>
       </c>
       <c r="L44" s="20">
         <f t="shared" si="7"/>
@@ -7702,11 +8021,11 @@
       </c>
       <c r="N44" s="7">
         <f t="shared" si="2"/>
-        <v>3718108.0983477174</v>
+        <v>3718691.4316810509</v>
       </c>
       <c r="O44" s="7">
         <f t="shared" si="12"/>
-        <v>15377583.722469738</v>
+        <v>15393917.055803068</v>
       </c>
       <c r="Q44" s="20">
         <f t="shared" si="8"/>
@@ -7718,11 +8037,11 @@
       </c>
       <c r="S44" s="7">
         <f t="shared" si="3"/>
-        <v>647993.33901650226</v>
+        <v>648576.67234983551</v>
       </c>
       <c r="T44" s="7">
         <f t="shared" si="13"/>
-        <v>3190489.145210125</v>
+        <v>3206822.4785434576</v>
       </c>
       <c r="V44" s="11">
         <f t="shared" si="9"/>
@@ -7734,11 +8053,11 @@
       </c>
       <c r="X44" s="7">
         <f t="shared" si="4"/>
-        <v>87164.672276369456</v>
+        <v>87748.005609702785</v>
       </c>
       <c r="Y44" s="7">
         <f t="shared" si="14"/>
-        <v>349128.61726228532</v>
+        <v>365461.95059561852</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.3">
@@ -7755,11 +8074,11 @@
       </c>
       <c r="D45" s="7">
         <f t="shared" si="0"/>
-        <v>114781431.44379623</v>
+        <v>114782014.77712956</v>
       </c>
       <c r="E45" s="7">
         <f t="shared" si="10"/>
-        <v>343546505.48694426</v>
+        <v>343563422.15361094</v>
       </c>
       <c r="G45" s="20">
         <f t="shared" si="6"/>
@@ -7771,11 +8090,11 @@
       </c>
       <c r="I45" s="7">
         <f t="shared" si="1"/>
-        <v>27694053.516985953</v>
+        <v>27694636.850319285</v>
       </c>
       <c r="J45" s="7">
         <f t="shared" si="11"/>
-        <v>96143769.80945085</v>
+        <v>96160686.476117507</v>
       </c>
       <c r="L45" s="20">
         <f t="shared" si="7"/>
@@ -7787,11 +8106,11 @@
       </c>
       <c r="N45" s="7">
         <f t="shared" si="2"/>
-        <v>4842714.6945186993</v>
+        <v>4843298.0278520333</v>
       </c>
       <c r="O45" s="7">
         <f t="shared" si="12"/>
-        <v>20220298.416988436</v>
+        <v>20237215.0836551</v>
       </c>
       <c r="Q45" s="20">
         <f t="shared" si="8"/>
@@ -7803,11 +8122,11 @@
       </c>
       <c r="S45" s="7">
         <f t="shared" si="3"/>
-        <v>783708.11793091381</v>
+        <v>784291.45126424707</v>
       </c>
       <c r="T45" s="7">
         <f t="shared" si="13"/>
-        <v>3974197.2631410388</v>
+        <v>3991113.9298077049</v>
       </c>
       <c r="V45" s="11">
         <f t="shared" si="9"/>
@@ -7819,11 +8138,11 @@
       </c>
       <c r="X45" s="7">
         <f t="shared" si="4"/>
-        <v>98939.195059561971</v>
+        <v>99522.528392895299</v>
       </c>
       <c r="Y45" s="7">
         <f t="shared" si="14"/>
-        <v>448067.8123218473</v>
+        <v>464984.47898851382</v>
       </c>
     </row>
     <row r="46" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -7840,11 +8159,11 @@
       </c>
       <c r="D46" s="28">
         <f t="shared" si="0"/>
-        <v>172187437.44347212</v>
+        <v>172188020.77680546</v>
       </c>
       <c r="E46" s="28">
         <f t="shared" si="10"/>
-        <v>515733942.93041635</v>
+        <v>515751442.93041641</v>
       </c>
       <c r="G46" s="27">
         <f t="shared" si="6"/>
@@ -7856,11 +8175,11 @@
       </c>
       <c r="I46" s="28">
         <f t="shared" si="1"/>
-        <v>38783907.146002561</v>
+        <v>38784490.479335889</v>
       </c>
       <c r="J46" s="28">
         <f t="shared" si="11"/>
-        <v>134927676.9554534</v>
+        <v>134945176.9554534</v>
       </c>
       <c r="L46" s="27">
         <f t="shared" si="7"/>
@@ -7872,11 +8191,11 @@
       </c>
       <c r="N46" s="28">
         <f t="shared" si="2"/>
-        <v>6304703.2695409767</v>
+        <v>6305286.6028743107</v>
       </c>
       <c r="O46" s="28">
         <f t="shared" si="12"/>
-        <v>26525001.686529413</v>
+        <v>26542501.686529413</v>
       </c>
       <c r="Q46" s="27">
         <f t="shared" si="8"/>
@@ -7888,11 +8207,11 @@
       </c>
       <c r="S46" s="28">
         <f t="shared" si="3"/>
-        <v>946565.85262820765</v>
+        <v>947149.1859615409</v>
       </c>
       <c r="T46" s="28">
         <f t="shared" si="13"/>
-        <v>4920763.1157692466</v>
+        <v>4938263.1157692457</v>
       </c>
       <c r="V46" s="29">
         <f t="shared" si="9"/>
@@ -7904,11 +8223,11 @@
       </c>
       <c r="X46" s="28">
         <f t="shared" si="4"/>
-        <v>111891.17012107374</v>
+        <v>112474.50345440707</v>
       </c>
       <c r="Y46" s="28">
         <f t="shared" si="14"/>
-        <v>559958.98244292103</v>
+        <v>577458.98244292091</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.3">
@@ -7925,11 +8244,11 @@
       </c>
       <c r="D47" s="7">
         <f t="shared" si="0"/>
-        <v>258296446.44298598</v>
+        <v>258297029.77631932</v>
       </c>
       <c r="E47" s="7">
         <f t="shared" si="10"/>
-        <v>774030389.37340236</v>
+        <v>774048472.70673573</v>
       </c>
       <c r="G47" s="20">
         <f t="shared" si="6"/>
@@ -7941,11 +8260,11 @@
       </c>
       <c r="I47" s="7">
         <f t="shared" si="1"/>
-        <v>54309702.2266258</v>
+        <v>54310285.559959128</v>
       </c>
       <c r="J47" s="7">
         <f t="shared" si="11"/>
-        <v>189237379.1820792</v>
+        <v>189255462.51541251</v>
       </c>
       <c r="L47" s="20">
         <f t="shared" si="7"/>
@@ -7957,11 +8276,11 @@
       </c>
       <c r="N47" s="7">
         <f t="shared" si="2"/>
-        <v>8205288.4170699362</v>
+        <v>8205871.7504032701</v>
       </c>
       <c r="O47" s="7">
         <f t="shared" si="12"/>
-        <v>34730290.103599347</v>
+        <v>34748373.436932683</v>
       </c>
       <c r="Q47" s="20">
         <f t="shared" si="8"/>
@@ -7973,11 +8292,11 @@
       </c>
       <c r="S47" s="7">
         <f t="shared" si="3"/>
-        <v>1141995.1342649604</v>
+        <v>1142578.4675982937</v>
       </c>
       <c r="T47" s="7">
         <f t="shared" si="13"/>
-        <v>6062758.2500342075</v>
+        <v>6080841.5833675396</v>
       </c>
       <c r="V47" s="11">
         <f t="shared" si="9"/>
@@ -7989,11 +8308,11 @@
       </c>
       <c r="X47" s="7">
         <f t="shared" si="4"/>
-        <v>126138.34268873669</v>
+        <v>126721.67602207002</v>
       </c>
       <c r="Y47" s="7">
         <f t="shared" si="14"/>
-        <v>686097.32513165777</v>
+        <v>704180.65846499091</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.3">
@@ -8010,11 +8329,11 @@
       </c>
       <c r="D48" s="7">
         <f t="shared" si="0"/>
-        <v>387459959.94225663</v>
+        <v>387460543.27559</v>
       </c>
       <c r="E48" s="7">
         <f t="shared" si="10"/>
-        <v>1161490349.315659</v>
+        <v>1161509015.9823258</v>
       </c>
       <c r="G48" s="20">
         <f t="shared" si="6"/>
@@ -8026,11 +8345,11 @@
       </c>
       <c r="I48" s="7">
         <f t="shared" si="1"/>
-        <v>76045815.339498341</v>
+        <v>76046398.672831669</v>
       </c>
       <c r="J48" s="7">
         <f t="shared" si="11"/>
-        <v>265283194.52157754</v>
+        <v>265301861.18824416</v>
       </c>
       <c r="L48" s="20">
         <f t="shared" si="7"/>
@@ -8042,11 +8361,11 @@
       </c>
       <c r="N48" s="7">
         <f t="shared" si="2"/>
-        <v>10676049.108857585</v>
+        <v>10676632.442190919</v>
       </c>
       <c r="O48" s="7">
         <f t="shared" si="12"/>
-        <v>45406339.212456934</v>
+        <v>45425005.879123598</v>
       </c>
       <c r="Q48" s="20">
         <f t="shared" si="8"/>
@@ -8058,11 +8377,11 @@
       </c>
       <c r="S48" s="7">
         <f t="shared" si="3"/>
-        <v>1376510.2722290636</v>
+        <v>1377093.6055623968</v>
       </c>
       <c r="T48" s="7">
         <f t="shared" si="13"/>
-        <v>7439268.5222632708</v>
+        <v>7457935.1889299359</v>
       </c>
       <c r="V48" s="11">
         <f t="shared" si="9"/>
@@ -8074,11 +8393,11 @@
       </c>
       <c r="X48" s="7">
         <f t="shared" si="4"/>
-        <v>141810.23251316589</v>
+        <v>142393.56584649923</v>
       </c>
       <c r="Y48" s="7">
         <f t="shared" si="14"/>
-        <v>827907.55764482368</v>
+        <v>846574.22431149008</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
@@ -8095,11 +8414,11 @@
       </c>
       <c r="D49" s="7">
         <f t="shared" si="0"/>
-        <v>581205230.19116282</v>
+        <v>581205813.5244962</v>
       </c>
       <c r="E49" s="7">
         <f t="shared" si="10"/>
-        <v>1742695579.5068219</v>
+        <v>1742714829.5068221</v>
       </c>
       <c r="G49" s="20">
         <f t="shared" si="6"/>
@@ -8111,11 +8430,11 @@
       </c>
       <c r="I49" s="7">
         <f t="shared" si="1"/>
-        <v>106476373.69751988</v>
+        <v>106476957.03085321</v>
       </c>
       <c r="J49" s="7">
         <f t="shared" si="11"/>
-        <v>371759568.21909744</v>
+        <v>371778818.21909738</v>
       </c>
       <c r="L49" s="20">
         <f t="shared" si="7"/>
@@ -8127,11 +8446,11 @@
       </c>
       <c r="N49" s="7">
         <f t="shared" si="2"/>
-        <v>13888038.008181527</v>
+        <v>13888621.341514861</v>
       </c>
       <c r="O49" s="7">
         <f t="shared" si="12"/>
-        <v>59294377.220638461</v>
+        <v>59313627.220638461</v>
       </c>
       <c r="Q49" s="20">
         <f t="shared" si="8"/>
@@ -8143,11 +8462,11 @@
       </c>
       <c r="S49" s="7">
         <f t="shared" si="3"/>
-        <v>1657928.4377859873</v>
+        <v>1658511.7711193205</v>
       </c>
       <c r="T49" s="7">
         <f t="shared" si="13"/>
-        <v>9097196.9600492585</v>
+        <v>9116446.9600492567</v>
       </c>
       <c r="V49" s="11">
         <f t="shared" si="9"/>
@@ -8159,11 +8478,11 @@
       </c>
       <c r="X49" s="7">
         <f t="shared" si="4"/>
-        <v>159049.31132003805</v>
+        <v>159632.64465337139</v>
       </c>
       <c r="Y49" s="7">
         <f t="shared" si="14"/>
-        <v>986956.86896486173</v>
+        <v>1006206.8689648615</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.3">
@@ -8180,11 +8499,11 @@
       </c>
       <c r="D50" s="7">
         <f t="shared" si="0"/>
-        <v>871823135.56452191</v>
+        <v>871823718.89785528</v>
       </c>
       <c r="E50" s="7">
         <f t="shared" si="10"/>
-        <v>2614518715.0713439</v>
+        <v>2614538548.4046774</v>
       </c>
       <c r="G50" s="20">
         <f t="shared" si="6"/>
@@ -8196,11 +8515,11 @@
       </c>
       <c r="I50" s="7">
         <f t="shared" si="1"/>
-        <v>149079155.39875007</v>
+        <v>149079738.73208341</v>
       </c>
       <c r="J50" s="7">
         <f t="shared" si="11"/>
-        <v>520838723.6178475</v>
+        <v>520858556.95118082</v>
       </c>
       <c r="L50" s="20">
         <f t="shared" si="7"/>
@@ -8212,11 +8531,11 @@
       </c>
       <c r="N50" s="7">
         <f t="shared" si="2"/>
-        <v>18063623.577302653</v>
+        <v>18064206.910635985</v>
       </c>
       <c r="O50" s="7">
         <f t="shared" si="12"/>
-        <v>77358000.797941118</v>
+        <v>77377834.131274447</v>
       </c>
       <c r="Q50" s="20">
         <f t="shared" si="8"/>
@@ -8228,11 +8547,11 @@
       </c>
       <c r="S50" s="7">
         <f t="shared" si="3"/>
-        <v>1995630.2364542959</v>
+        <v>1996213.5697876292</v>
       </c>
       <c r="T50" s="7">
         <f t="shared" si="13"/>
-        <v>11092827.196503554</v>
+        <v>11112660.529836886</v>
       </c>
       <c r="V50" s="11">
         <f t="shared" si="9"/>
@@ -8244,11 +8563,11 @@
       </c>
       <c r="X50" s="7">
         <f t="shared" si="4"/>
-        <v>178012.29800759739</v>
+        <v>178595.63134093073</v>
       </c>
       <c r="Y50" s="7">
         <f t="shared" si="14"/>
-        <v>1164969.1669724591</v>
+        <v>1184802.5003057923</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
@@ -8265,11 +8584,11 @@
       </c>
       <c r="D51" s="7">
         <f t="shared" si="0"/>
-        <v>1307749993.6245606</v>
+        <v>1307750576.9578938</v>
       </c>
       <c r="E51" s="7">
         <f t="shared" si="10"/>
-        <v>3922268708.6959047</v>
+        <v>3922289125.3625712</v>
       </c>
       <c r="G51" s="20">
         <f t="shared" si="6"/>
@@ -8281,11 +8600,11 @@
       </c>
       <c r="I51" s="7">
         <f t="shared" si="1"/>
-        <v>208723049.78047228</v>
+        <v>208723633.11380562</v>
       </c>
       <c r="J51" s="7">
         <f t="shared" si="11"/>
-        <v>729561773.39831972</v>
+        <v>729582190.06498647</v>
       </c>
       <c r="L51" s="20">
         <f t="shared" si="7"/>
@@ -8297,11 +8616,11 @@
       </c>
       <c r="N51" s="7">
         <f t="shared" si="2"/>
-        <v>23491884.817160115</v>
+        <v>23492468.150493447</v>
       </c>
       <c r="O51" s="7">
         <f t="shared" si="12"/>
-        <v>100849885.61510123</v>
+        <v>100870302.28176789</v>
       </c>
       <c r="Q51" s="20">
         <f t="shared" si="8"/>
@@ -8313,11 +8632,11 @@
       </c>
       <c r="S51" s="7">
         <f t="shared" si="3"/>
-        <v>2400872.3948562657</v>
+        <v>2401455.7281895992</v>
       </c>
       <c r="T51" s="7">
         <f t="shared" si="13"/>
-        <v>13493699.59135982</v>
+        <v>13514116.258026484</v>
       </c>
       <c r="V51" s="11">
         <f t="shared" si="9"/>
@@ -8329,11 +8648,11 @@
       </c>
       <c r="X51" s="7">
         <f t="shared" si="4"/>
-        <v>198871.58336391271</v>
+        <v>199454.91669724605</v>
       </c>
       <c r="Y51" s="7">
         <f t="shared" si="14"/>
-        <v>1363840.7503363718</v>
+        <v>1384257.4170030383</v>
       </c>
     </row>
     <row r="52" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.3">
@@ -8350,11 +8669,11 @@
       </c>
       <c r="D52" s="28">
         <f t="shared" si="0"/>
-        <v>1961640280.7146187</v>
+        <v>1961640864.0479519</v>
       </c>
       <c r="E52" s="28">
         <f t="shared" si="10"/>
-        <v>5883908989.4105234</v>
+        <v>5883929989.4105234</v>
       </c>
       <c r="G52" s="27">
         <f t="shared" si="6"/>
@@ -8366,11 +8685,11 @@
       </c>
       <c r="I52" s="28">
         <f t="shared" si="1"/>
-        <v>292224501.91488338</v>
+        <v>292225085.24821675</v>
       </c>
       <c r="J52" s="28">
         <f t="shared" si="11"/>
-        <v>1021786275.3132031</v>
+        <v>1021807275.3132032</v>
       </c>
       <c r="L52" s="27">
         <f t="shared" si="7"/>
@@ -8382,11 +8701,11 @@
       </c>
       <c r="N52" s="28">
         <f t="shared" si="2"/>
-        <v>30548624.428974818</v>
+        <v>30549207.762308151</v>
       </c>
       <c r="O52" s="28">
         <f t="shared" si="12"/>
-        <v>131398510.04407606</v>
+        <v>131419510.04407604</v>
       </c>
       <c r="Q52" s="27">
         <f t="shared" si="8"/>
@@ -8398,11 +8717,11 @@
       </c>
       <c r="S52" s="28">
         <f t="shared" si="3"/>
-        <v>2887162.9849386299</v>
+        <v>2887746.3182719634</v>
       </c>
       <c r="T52" s="28">
         <f t="shared" si="13"/>
-        <v>16380862.576298449</v>
+        <v>16401862.576298447</v>
       </c>
       <c r="V52" s="29">
         <f t="shared" si="9"/>
@@ -8414,11 +8733,11 @@
       </c>
       <c r="X52" s="28">
         <f t="shared" si="4"/>
-        <v>221816.79725585959</v>
+        <v>222400.13058919294</v>
       </c>
       <c r="Y52" s="28">
         <f t="shared" si="14"/>
-        <v>1585657.5475922315</v>
+        <v>1606657.5475922313</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.3">
@@ -8435,11 +8754,11 @@
       </c>
       <c r="D53" s="7">
         <f t="shared" si="0"/>
-        <v>2942475711.3497057</v>
+        <v>2942476294.6830387</v>
       </c>
       <c r="E53" s="7">
         <f t="shared" si="10"/>
-        <v>8826384700.7602291</v>
+        <v>8826406284.0935631</v>
       </c>
       <c r="G53" s="20">
         <f t="shared" si="6"/>
@@ -8451,11 +8770,11 @@
       </c>
       <c r="I53" s="7">
         <f t="shared" si="1"/>
-        <v>409126534.90305889</v>
+        <v>409127118.23639226</v>
       </c>
       <c r="J53" s="7">
         <f t="shared" si="11"/>
-        <v>1430912810.2162619</v>
+        <v>1430934393.5495954</v>
       </c>
       <c r="L53" s="20">
         <f t="shared" si="7"/>
@@ -8467,11 +8786,11 @@
       </c>
       <c r="N53" s="7">
         <f t="shared" si="2"/>
-        <v>39722385.924333937</v>
+        <v>39722969.257667266</v>
       </c>
       <c r="O53" s="7">
         <f t="shared" si="12"/>
-        <v>171120895.96840999</v>
+        <v>171142479.3017433</v>
       </c>
       <c r="Q53" s="20">
         <f t="shared" si="8"/>
@@ -8483,11 +8802,11 @@
       </c>
       <c r="S53" s="7">
         <f t="shared" si="3"/>
-        <v>3470711.6930374666</v>
+        <v>3471295.0263708001</v>
       </c>
       <c r="T53" s="7">
         <f t="shared" si="13"/>
-        <v>19851574.269335914</v>
+        <v>19873157.602669246</v>
       </c>
       <c r="V53" s="11">
         <f t="shared" si="9"/>
@@ -8499,11 +8818,11 @@
       </c>
       <c r="X53" s="7">
         <f t="shared" si="4"/>
-        <v>247056.53253700113</v>
+        <v>247639.86587033447</v>
       </c>
       <c r="Y53" s="7">
         <f t="shared" si="14"/>
-        <v>1832714.0801292327</v>
+        <v>1854297.4134625657</v>
       </c>
     </row>
   </sheetData>
@@ -8577,12 +8896,292 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E200A4BF-7444-461A-A7D9-DCB85EAD9C4B}">
+  <dimension ref="A2:C38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>700</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4*B3</f>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1">
+        <f>B5*4</f>
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
+        <f>B5*51</f>
+        <v>107100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <f>SUM(B8:B12)</f>
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <f>B13*12+B7</f>
+        <v>175500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <f>B19*B25*B26*B22</f>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="1">
+        <f>B22*B18*B29*B30</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1">
+        <f>B27+B31</f>
+        <v>15750</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1">
+        <f>B33*4</f>
+        <v>63000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1">
+        <f>B33*51</f>
+        <v>803250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1">
+        <f>B35*0.25</f>
+        <v>200812.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="1">
+        <f>B35-B36</f>
+        <v>602437.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1">
+        <f>B37-B14</f>
+        <v>426937.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1ED5F7-7D0A-4613-B246-76BB506BCE91}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9004,7 +9603,7 @@
   <dimension ref="A3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9109,7 +9708,7 @@
       </c>
       <c r="B15" s="7">
         <f>Operating_Costs!G12</f>
-        <v>366966.66666666663</v>
+        <v>359966.66666666669</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -9170,27 +9769,27 @@
       </c>
       <c r="B18" s="7">
         <f t="shared" ref="B18:G18" si="1">$B$15*B$17</f>
-        <v>183483.33333333331</v>
+        <v>179983.33333333334</v>
       </c>
       <c r="C18" s="7">
         <f t="shared" si="1"/>
-        <v>152902.77777777778</v>
+        <v>149986.11111111112</v>
       </c>
       <c r="D18" s="7">
         <f t="shared" si="1"/>
-        <v>122322.2222222222</v>
+        <v>119988.88888888889</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="1"/>
-        <v>91741.666666666657</v>
+        <v>89991.666666666672</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>61161.111111111102</v>
+        <v>59994.444444444445</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="1"/>
-        <v>30580.555555555551</v>
+        <v>29997.222222222223</v>
       </c>
       <c r="H18" s="7"/>
     </row>
@@ -9200,27 +9799,27 @@
       </c>
       <c r="B19" s="7">
         <f>$B$10+($B$15*B$17)+$B$12+$B$11</f>
-        <v>269128.33333333331</v>
+        <v>265628.33333333337</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:G19" si="2">$B$10+($B$15*C$17)+$B$12+$B$11</f>
-        <v>238547.77777777778</v>
+        <v>235631.11111111112</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="2"/>
-        <v>207967.22222222219</v>
+        <v>205633.88888888888</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="2"/>
-        <v>177386.66666666666</v>
+        <v>175636.66666666669</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="2"/>
-        <v>146806.11111111109</v>
+        <v>145639.44444444444</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="2"/>
-        <v>116225.55555555555</v>
+        <v>115642.22222222222</v>
       </c>
       <c r="H19" s="7"/>
     </row>
@@ -9433,7 +10032,7 @@
       </c>
       <c r="B8" s="7">
         <f>Operating_Costs!G12</f>
-        <v>366966.66666666663</v>
+        <v>359966.66666666669</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="16"/>
@@ -9454,51 +10053,51 @@
       </c>
       <c r="B10" s="7">
         <f>B6-$B$8</f>
-        <v>-361766.66666666663</v>
+        <v>-354766.66666666669</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:L10" si="0">C6-$B$8</f>
-        <v>-356566.66666666663</v>
+        <v>-349566.66666666669</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>-346166.66666666663</v>
+        <v>-339166.66666666669</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>-325366.66666666663</v>
+        <v>-318366.66666666669</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
-        <v>-283766.66666666663</v>
+        <v>-276766.66666666669</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>-200566.6666666666</v>
+        <v>-193566.66666666666</v>
       </c>
       <c r="H10" s="7">
         <f t="shared" si="0"/>
-        <v>-106966.66666666657</v>
+        <v>-99966.666666666628</v>
       </c>
       <c r="I10" s="16">
         <f t="shared" si="0"/>
-        <v>2233.3333333334303</v>
+        <v>9233.3333333333721</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="0"/>
-        <v>101033.33333333349</v>
+        <v>108033.33333333343</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="0"/>
-        <v>153033.33333333349</v>
+        <v>160033.33333333343</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="0"/>
-        <v>205033.33333333349</v>
+        <v>212033.33333333343</v>
       </c>
       <c r="M10" s="18">
         <f t="shared" ref="M10" si="1">M6-$B$8</f>
-        <v>257033.33333333349</v>
+        <v>264033.33333333343</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -9645,8 +10244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7959888-B526-4FAC-9FC1-7A03020906F6}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10688,7 +11287,7 @@
   <dimension ref="A3:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10737,11 +11336,11 @@
       </c>
       <c r="D4" s="1">
         <f>employees!B11</f>
-        <v>2342.3076923076924</v>
+        <v>2207.6923076923076</v>
       </c>
       <c r="E4" s="1">
         <f>D4*2</f>
-        <v>4684.6153846153848</v>
+        <v>4415.3846153846152</v>
       </c>
       <c r="F4" s="1">
         <f>C4*(52/12)</f>
@@ -10757,27 +11356,27 @@
       </c>
       <c r="B5" s="1">
         <f>C5/7</f>
-        <v>334.61538461538464</v>
+        <v>315.38461538461536</v>
       </c>
       <c r="C5" s="1">
         <f>employees!B11</f>
-        <v>2342.3076923076924</v>
+        <v>2207.6923076923076</v>
       </c>
       <c r="D5" s="1">
         <f>employees!B12</f>
-        <v>4684.6153846153848</v>
+        <v>4415.3846153846152</v>
       </c>
       <c r="E5" s="1">
         <f>D5*2</f>
-        <v>9369.2307692307695</v>
+        <v>8830.7692307692305</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F12" si="0">C5*(52/12)</f>
-        <v>10150</v>
+        <v>9566.6666666666661</v>
       </c>
       <c r="G5" s="1">
         <f>employees!B8</f>
-        <v>121800</v>
+        <v>114800</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -10958,27 +11557,27 @@
       </c>
       <c r="B12" s="1">
         <f>SUM(B4:B11)</f>
-        <v>1009.1575091575091</v>
+        <v>989.92673992673986</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ref="C12:E12" si="2">SUM(C4:C11)</f>
-        <v>7064.1025641025644</v>
+        <v>6929.4871794871797</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>16316.666666666668</v>
+        <v>15912.820512820512</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>32633.333333333336</v>
+        <v>31825.641025641024</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>30611.111111111109</v>
+        <v>30027.777777777777</v>
       </c>
       <c r="G12" s="1">
         <f>SUM(G4:G11)</f>
-        <v>366966.66666666663</v>
+        <v>359966.66666666669</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
completed most of what I can for Projections
</commit_message>
<xml_diff>
--- a/Finances/Custom_Calculations.xlsx
+++ b/Finances/Custom_Calculations.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tfrancis\OneDrive - Hearst\Documents\Custom Office Templates\dogen\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3078" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4CBC68A-467C-48AB-83A7-CC7DBCC1979C}"/>
+  <xr:revisionPtr revIDLastSave="3080" documentId="8_{6C3C763F-D9E1-4E6D-8C86-4D28C6C6C4A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{28AA28AD-F28D-471A-96C7-4BA0C5EB3522}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="740" firstSheet="3" activeTab="7" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="740" firstSheet="7" activeTab="7" xr2:uid="{7EC05EA9-5315-43E9-8396-FB9501FE745C}"/>
   </bookViews>
   <sheets>
     <sheet name="Key_Assumptions_draft" sheetId="27" state="hidden" r:id="rId1"/>
-    <sheet name="Community_Engagement" sheetId="28" state="hidden" r:id="rId2"/>
+    <sheet name="Chart1" sheetId="28" state="hidden" r:id="rId2"/>
     <sheet name="Revenue_Profit_Balance" sheetId="19" r:id="rId3"/>
     <sheet name="Funding_And_Connections" sheetId="23" r:id="rId4"/>
     <sheet name="Comprehensive" sheetId="3" r:id="rId5"/>
@@ -4046,7 +4046,7 @@
         <v>882.35294117647061</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" ref="H4:H5" si="0">G4/40</f>
+        <f t="shared" ref="H4" si="0">G4/40</f>
         <v>22.058823529411764</v>
       </c>
     </row>
@@ -10244,8 +10244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7959888-B526-4FAC-9FC1-7A03020906F6}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11287,7 +11287,7 @@
   <dimension ref="A3:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>